<commit_message>
console log those who did not get the route, added chalk
</commit_message>
<xml_diff>
--- a/EzForm.xlsx
+++ b/EzForm.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:U111"/>
+  <dimension ref="A1:U110"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -450,30 +450,18 @@
         <v>Атлант Груп</v>
       </c>
       <c r="B2" t="str">
-        <v>Борис Артём</v>
+        <v>Борис Антон</v>
       </c>
       <c r="C2" t="str">
-        <v>У452СН199</v>
+        <v>У223РЕ197</v>
       </c>
       <c r="D2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E2" t="str">
-        <v>шоссе Энтузиастов, д. 10/2</v>
+        <v>г. Дедовск, 1-ая Главная, д. 1</v>
       </c>
       <c r="F2" t="str">
-        <v/>
-      </c>
-      <c r="G2" t="str">
-        <v>Красноказарменная улица, д. 14А, к. 2</v>
-      </c>
-      <c r="H2" t="str">
-        <v/>
-      </c>
-      <c r="I2" t="str">
-        <v>Перовское шоссе, д. 16/2</v>
-      </c>
-      <c r="J2" t="str">
         <v/>
       </c>
     </row>
@@ -482,30 +470,36 @@
         <v>Атлант Груп</v>
       </c>
       <c r="B3" t="str">
-        <v>Бузятов Алексей</v>
+        <v>Борис Артём</v>
       </c>
       <c r="C3" t="str">
-        <v>Е130УТ799</v>
+        <v>У452СН199</v>
       </c>
       <c r="D3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E3" t="str">
-        <v>Венёвская улица, д. 4</v>
+        <v>Нижегородская улица, д. 71</v>
       </c>
       <c r="F3" t="str">
         <v/>
       </c>
       <c r="G3" t="str">
-        <v>г. поселение Воскресенское, Чечёрский проезд, д. 122, к. 1</v>
+        <v>Перовское шоссе, д. 16/2</v>
       </c>
       <c r="H3" t="str">
         <v/>
       </c>
       <c r="I3" t="str">
-        <v>Южнобутовская улица, д. 117</v>
+        <v>Красноказарменная улица, д. 14А, к. 2</v>
       </c>
       <c r="J3" t="str">
+        <v/>
+      </c>
+      <c r="K3" t="str">
+        <v>шоссе Энтузиастов, д. 10/2</v>
+      </c>
+      <c r="L3" t="str">
         <v/>
       </c>
     </row>
@@ -514,48 +508,30 @@
         <v>Атлант Груп</v>
       </c>
       <c r="B4" t="str">
-        <v>Володин Евгений</v>
+        <v>Востриков Максим</v>
       </c>
       <c r="C4" t="str">
-        <v>О583АТ32</v>
+        <v>К387УВ77</v>
       </c>
       <c r="D4">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E4" t="str">
-        <v>улица Габричевского, д. 10, к. 1</v>
+        <v>г. Подольск, Бородинский бульвар, д. 7</v>
       </c>
       <c r="F4" t="str">
         <v/>
       </c>
       <c r="G4" t="str">
-        <v>улица Расплетина, д. 13</v>
+        <v>г. Подольск, улица Чистова, д. 3</v>
       </c>
       <c r="H4" t="str">
         <v/>
       </c>
       <c r="I4" t="str">
-        <v>улица Маршала Новикова, д. 2, к. 2</v>
+        <v>г. Подольск, Мраморная улица, д. 4</v>
       </c>
       <c r="J4" t="str">
-        <v/>
-      </c>
-      <c r="K4" t="str">
-        <v>Таллинская улица, д. 16, к. 1</v>
-      </c>
-      <c r="L4" t="str">
-        <v/>
-      </c>
-      <c r="M4" t="str">
-        <v>Маршала Катукова, д. 24, к. 4</v>
-      </c>
-      <c r="N4" t="str">
-        <v/>
-      </c>
-      <c r="O4" t="str">
-        <v>улица Маршала Катукова, д. 3, к. 1</v>
-      </c>
-      <c r="P4" t="str">
         <v/>
       </c>
     </row>
@@ -570,24 +546,36 @@
         <v>Р130ОВ05</v>
       </c>
       <c r="D5">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E5" t="str">
-        <v>улица Александры Монаховой, д. 105, к. 1</v>
+        <v>улица Мусы Джалиля, д. 27, стр. 2, к. 2</v>
       </c>
       <c r="F5" t="str">
         <v/>
       </c>
       <c r="G5" t="str">
-        <v>г. посёлок Коммунарка, улица Александры Монаховой, д. 96, к. 2</v>
+        <v>Каширское шоссе, д. 80</v>
       </c>
       <c r="H5" t="str">
         <v/>
       </c>
       <c r="I5" t="str">
-        <v>улица Горчакова, д. 1</v>
+        <v>улица Борисовские Пруды, д. 5, к. 1</v>
       </c>
       <c r="J5" t="str">
+        <v/>
+      </c>
+      <c r="K5" t="str">
+        <v>улица Борисовские Пруды, д. 8А</v>
+      </c>
+      <c r="L5" t="str">
+        <v/>
+      </c>
+      <c r="M5" t="str">
+        <v>улица Борисовские Пруды, д. 14, к. 3</v>
+      </c>
+      <c r="N5" t="str">
         <v/>
       </c>
     </row>
@@ -602,36 +590,18 @@
         <v>У972РУ790</v>
       </c>
       <c r="D6">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E6" t="str">
-        <v>Святоозерская, д. 14</v>
+        <v>г. Дмитров, Профессиональная улица, д. 22, к. 1</v>
       </c>
       <c r="F6" t="str">
         <v/>
       </c>
       <c r="G6" t="str">
-        <v>г. Люберцы, улица Шевлякова, д. 2/24</v>
+        <v>г. Дмитров, Советская улица, д. 5</v>
       </c>
       <c r="H6" t="str">
-        <v/>
-      </c>
-      <c r="I6" t="str">
-        <v>г. Люберцы, улица Попова, д. 34/1</v>
-      </c>
-      <c r="J6" t="str">
-        <v/>
-      </c>
-      <c r="K6" t="str">
-        <v>г. Люберцы, Комсомольский проспект, д. 7/1</v>
-      </c>
-      <c r="L6" t="str">
-        <v/>
-      </c>
-      <c r="M6" t="str">
-        <v>г. Люберцы, Комсомольский проспект, д. 7/1</v>
-      </c>
-      <c r="N6" t="str">
         <v/>
       </c>
     </row>
@@ -646,42 +616,24 @@
         <v>М392РА799</v>
       </c>
       <c r="D7">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E7" t="str">
-        <v>1-й Очаковский переулок, д. 1</v>
+        <v>г. Долгопрудный, Набережная улица, д. 31</v>
       </c>
       <c r="F7" t="str">
         <v/>
       </c>
       <c r="G7" t="str">
-        <v>улица Наташи Ковшовой, д. 8А, стр. А</v>
+        <v>г. Лобня, улица Ленина, д. 18</v>
       </c>
       <c r="H7" t="str">
         <v/>
       </c>
       <c r="I7" t="str">
-        <v>Озёрная улица, д. 42</v>
+        <v>г. Химки, улица Лётчика Ивана Фёдорова, д. 8, к. 1</v>
       </c>
       <c r="J7" t="str">
-        <v/>
-      </c>
-      <c r="K7" t="str">
-        <v>Боровское шоссе, д. 2А, к. 1</v>
-      </c>
-      <c r="L7" t="str">
-        <v/>
-      </c>
-      <c r="M7" t="str">
-        <v>улица Авиаторов, д. 5, к. 6</v>
-      </c>
-      <c r="N7" t="str">
-        <v/>
-      </c>
-      <c r="O7" t="str">
-        <v>Солнцевский проспект, д. 15</v>
-      </c>
-      <c r="P7" t="str">
         <v/>
       </c>
     </row>
@@ -696,18 +648,30 @@
         <v>Р701ЕА797</v>
       </c>
       <c r="D8">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E8" t="str">
-        <v>г. Дмитров, Профессиональная улица, д. 22, к. 1</v>
+        <v>г. Ивантеевка, улица Новая Слобода, д. 3</v>
       </c>
       <c r="F8" t="str">
         <v/>
       </c>
       <c r="G8" t="str">
-        <v>г. Дмитров, Советская улица, д. 5</v>
+        <v>г. Ивантеевка, улица Новосёлки, д. 4</v>
       </c>
       <c r="H8" t="str">
+        <v/>
+      </c>
+      <c r="I8" t="str">
+        <v>г. Ивантеевка, Школьная улица, д. 16</v>
+      </c>
+      <c r="J8" t="str">
+        <v/>
+      </c>
+      <c r="K8" t="str">
+        <v>г. Щёлково, микрорайон Финский, д. 11, к. 1</v>
+      </c>
+      <c r="L8" t="str">
         <v/>
       </c>
     </row>
@@ -716,36 +680,24 @@
         <v>Атлант Груп</v>
       </c>
       <c r="B9" t="str">
-        <v>Подпригора Антон</v>
+        <v>Суханов Алексей</v>
       </c>
       <c r="C9" t="str">
-        <v>Н182ХК75</v>
+        <v>Н072КУ797</v>
       </c>
       <c r="D9">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E9" t="str">
-        <v>г. поселение Десеновское, 1-я Нововатутинская улица, д. 5</v>
+        <v>Дубнинская улица, д. 32, к. 6</v>
       </c>
       <c r="F9" t="str">
         <v/>
       </c>
       <c r="G9" t="str">
-        <v>г. Троицк, микрорайон В, д. 50</v>
+        <v>Дмитровское шоссе, д. 107А, к. 3</v>
       </c>
       <c r="H9" t="str">
-        <v/>
-      </c>
-      <c r="I9" t="str">
-        <v>г. Троицк, Академическая площадь, д. 3, кв. 2А</v>
-      </c>
-      <c r="J9" t="str">
-        <v/>
-      </c>
-      <c r="K9" t="str">
-        <v>г. Троицк, Городская улица, д. вл6</v>
-      </c>
-      <c r="L9" t="str">
         <v/>
       </c>
     </row>
@@ -754,80 +706,62 @@
         <v>Атлант Груп</v>
       </c>
       <c r="B10" t="str">
-        <v>Суханов Алексей</v>
+        <v>Трубников  Александр</v>
       </c>
       <c r="C10" t="str">
-        <v>Н072КУ797</v>
+        <v>Х734ХК190</v>
       </c>
       <c r="D10">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E10" t="str">
-        <v>Планерная улица, д. 7</v>
+        <v>Заводской проезд, д. 10</v>
       </c>
       <c r="F10" t="str">
         <v/>
       </c>
       <c r="G10" t="str">
-        <v>г. Химки, Молодёжная улица, д. 15Б, к. Б</v>
+        <v>Измайловский проезд, д. 10, к. 3</v>
       </c>
       <c r="H10" t="str">
         <v/>
       </c>
       <c r="I10" t="str">
-        <v>Родионовская, д. 5</v>
+        <v>9-я Парковая улица, д. 6, к. 1</v>
       </c>
       <c r="J10" t="str">
         <v/>
       </c>
       <c r="K10" t="str">
-        <v>Соколово-Мещерская улица, д. 25</v>
+        <v>Вольная улица, д. 28/4, к. 1</v>
       </c>
       <c r="L10" t="str">
-        <v/>
-      </c>
-      <c r="M10" t="str">
-        <v>г. Химки, Молодёжная улица, д. 52</v>
-      </c>
-      <c r="N10" t="str">
-        <v/>
-      </c>
-      <c r="O10" t="str">
-        <v>г. деревня Путилково, Новотушинская улица, д. 2</v>
-      </c>
-      <c r="P10" t="str">
         <v/>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>Атлант Груп</v>
+        <v>ЛоялАвто</v>
       </c>
       <c r="B11" t="str">
-        <v>Трубников  Александр</v>
+        <v xml:space="preserve">Алыбин Николай </v>
       </c>
       <c r="C11" t="str">
-        <v>Х734ХК190</v>
+        <v>Х718ЕЕ50</v>
       </c>
       <c r="D11">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E11" t="str">
-        <v>Локомотивный проезд, д. 4</v>
+        <v>Походный проезд, д. 4, к. 1</v>
       </c>
       <c r="F11" t="str">
         <v/>
       </c>
       <c r="G11" t="str">
-        <v>3-й Нижнелихоборский проезд, д. 3, кв. 1</v>
+        <v>г. Красногорск, улица Жуковского, д. 17</v>
       </c>
       <c r="H11" t="str">
-        <v/>
-      </c>
-      <c r="I11" t="str">
-        <v>Большая Академическая улица, д. 75, к. 2</v>
-      </c>
-      <c r="J11" t="str">
         <v/>
       </c>
     </row>
@@ -836,28 +770,28 @@
         <v>ЛоялАвто</v>
       </c>
       <c r="B12" t="str">
-        <v>Абдуллаев Бакытбек</v>
+        <v>Гвиздон Валерий</v>
       </c>
       <c r="C12" t="str">
-        <v>Н018УК777</v>
+        <v>Х270ОХ12</v>
       </c>
       <c r="D12">
         <v>3</v>
       </c>
       <c r="E12" t="str">
-        <v>Брянская улица, д. 12</v>
+        <v>Боровское шоссе, д. 2А, к. 1</v>
       </c>
       <c r="F12" t="str">
         <v/>
       </c>
       <c r="G12" t="str">
-        <v>улица Барклая, д. 5, к. 4</v>
+        <v>улица Авиаторов, д. 5, к. 6</v>
       </c>
       <c r="H12" t="str">
         <v/>
       </c>
       <c r="I12" t="str">
-        <v>Кастанаевская улица, д. 16, к. 1</v>
+        <v>Солнцевский проспект, д. 15</v>
       </c>
       <c r="J12" t="str">
         <v/>
@@ -868,36 +802,30 @@
         <v>ЛоялАвто</v>
       </c>
       <c r="B13" t="str">
-        <v>Алимканов Тилекбек</v>
+        <v>Жусупбаев Дилмурат</v>
       </c>
       <c r="C13" t="str">
-        <v>О556ЕР196</v>
+        <v>Т672НВ790</v>
       </c>
       <c r="D13">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E13" t="str">
-        <v>Варшавское шоссе, д. 86А</v>
+        <v>Соколово-Мещерская улица, д. 25</v>
       </c>
       <c r="F13" t="str">
         <v/>
       </c>
       <c r="G13" t="str">
-        <v>Чертановская улица, д. 32, к. 1</v>
+        <v>г. Химки, Молодёжная улица, д. 52</v>
       </c>
       <c r="H13" t="str">
         <v/>
       </c>
       <c r="I13" t="str">
-        <v>улица Красного Маяка, д. 15А, стр. 1</v>
+        <v>г. Химки, Молодёжная улица, д. 15Б, к. Б</v>
       </c>
       <c r="J13" t="str">
-        <v/>
-      </c>
-      <c r="K13" t="str">
-        <v>Кировоградская, д. 30</v>
-      </c>
-      <c r="L13" t="str">
         <v/>
       </c>
     </row>
@@ -906,30 +834,42 @@
         <v>ЛоялАвто</v>
       </c>
       <c r="B14" t="str">
-        <v xml:space="preserve">Алыбин Николай </v>
+        <v>Исаев Сергей</v>
       </c>
       <c r="C14" t="str">
-        <v>Х718ЕЕ50</v>
+        <v>С703КР12</v>
       </c>
       <c r="D14">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E14" t="str">
-        <v>проспект Мира, д. 124, к. 2</v>
+        <v>Суздальская улица, д. 12А</v>
       </c>
       <c r="F14" t="str">
         <v/>
       </c>
       <c r="G14" t="str">
-        <v>улица Академика Королёва, д. 13, стр. 1</v>
+        <v>г. Реутов, улица имени Академика В.Н. Челомея, д. 12</v>
       </c>
       <c r="H14" t="str">
         <v/>
       </c>
       <c r="I14" t="str">
-        <v>Большая Марфинская улица, д. 4, к. 1</v>
+        <v>г. Реутов, Юбилейный проспект, д. 72</v>
       </c>
       <c r="J14" t="str">
+        <v/>
+      </c>
+      <c r="K14" t="str">
+        <v>г. Реутов, улица Октября, д. вл10</v>
+      </c>
+      <c r="L14" t="str">
+        <v/>
+      </c>
+      <c r="M14" t="str">
+        <v>Кетчерская улица, д. 4Б, стр. 1</v>
+      </c>
+      <c r="N14" t="str">
         <v/>
       </c>
     </row>
@@ -938,30 +878,36 @@
         <v>ЛоялАвто</v>
       </c>
       <c r="B15" t="str">
-        <v>Белов Рудольф</v>
+        <v>Исхаков Эмиль</v>
       </c>
       <c r="C15" t="str">
-        <v>А722УМ799</v>
+        <v>А181ВН797</v>
       </c>
       <c r="D15">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E15" t="str">
-        <v>площадь Джавахарлала Неру, д. 1</v>
+        <v>3-й Нижнелихоборский проезд, д. 3, кв. 1</v>
       </c>
       <c r="F15" t="str">
         <v/>
       </c>
       <c r="G15" t="str">
-        <v>улица Марии Ульяновой, д. 9, к. 3</v>
+        <v>Большая Академическая улица, д. 75, к. 2</v>
       </c>
       <c r="H15" t="str">
         <v/>
       </c>
       <c r="I15" t="str">
-        <v>улица Кравченко, д. 11</v>
+        <v>проезд Черепановых, д. 36</v>
       </c>
       <c r="J15" t="str">
+        <v/>
+      </c>
+      <c r="K15" t="str">
+        <v>улица Дубки, д. 4А</v>
+      </c>
+      <c r="L15" t="str">
         <v/>
       </c>
     </row>
@@ -970,42 +916,36 @@
         <v>ЛоялАвто</v>
       </c>
       <c r="B16" t="str">
-        <v>Гвиздон Валерий</v>
+        <v>Ковалев  Андрей</v>
       </c>
       <c r="C16" t="str">
-        <v>Х270ОХ12</v>
+        <v>М527ЕК777</v>
       </c>
       <c r="D16">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E16" t="str">
-        <v>г. Люберцы, улица Кирова, д. 9, к. 5</v>
+        <v>г. Королёв, Пионерская улица, д. 30, к. 9</v>
       </c>
       <c r="F16" t="str">
         <v/>
       </c>
       <c r="G16" t="str">
-        <v>г. Люберцы, Проспек Победы, д. 6, кв. 019</v>
+        <v>г. Королёв, проспект Космонавтов, д. 34Б, к. Б</v>
       </c>
       <c r="H16" t="str">
         <v/>
       </c>
       <c r="I16" t="str">
-        <v>г. Люберцы, проспект Гагарина, д. 28/1</v>
+        <v>г. Королёв, проезд Макаренко, д. 1</v>
       </c>
       <c r="J16" t="str">
         <v/>
       </c>
       <c r="K16" t="str">
-        <v>г. Люберцы, Смирновская улица, д. 21, к. 2</v>
+        <v>г. Королёв, улица 50-летия ВЛКСМ, д. 6, к. Е</v>
       </c>
       <c r="L16" t="str">
-        <v/>
-      </c>
-      <c r="M16" t="str">
-        <v>г. Люберцы, Московская улица, д. 11</v>
-      </c>
-      <c r="N16" t="str">
         <v/>
       </c>
     </row>
@@ -1014,36 +954,30 @@
         <v>ЛоялАвто</v>
       </c>
       <c r="B17" t="str">
-        <v>Дузь Леонид</v>
+        <v>Кошель Филипп</v>
       </c>
       <c r="C17" t="str">
-        <v>У136СЕ48</v>
+        <v>В849НУ193</v>
       </c>
       <c r="D17">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E17" t="str">
-        <v>г. Мытищи, Коммунистическая улица, д. 1</v>
+        <v>г. Троицк, микрорайон В, д. 50</v>
       </c>
       <c r="F17" t="str">
         <v/>
       </c>
       <c r="G17" t="str">
-        <v>Холмогорская улица, д. 2, стр. 2, к. 2</v>
+        <v>г. Троицк, Академическая площадь, д. 3, кв. 2А</v>
       </c>
       <c r="H17" t="str">
         <v/>
       </c>
       <c r="I17" t="str">
-        <v>Ярославское шоссе, д. 28, к. 1</v>
+        <v>г. Троицк, Городская улица, д. вл6</v>
       </c>
       <c r="J17" t="str">
-        <v/>
-      </c>
-      <c r="K17" t="str">
-        <v>Ярославское шоссе, д. 124</v>
-      </c>
-      <c r="L17" t="str">
         <v/>
       </c>
     </row>
@@ -1052,36 +986,30 @@
         <v>ЛоялАвто</v>
       </c>
       <c r="B18" t="str">
-        <v>Жусупбаев Дилмурат</v>
+        <v>Мурзаев Талант</v>
       </c>
       <c r="C18" t="str">
-        <v>Т672НВ790</v>
+        <v>М980АМ62</v>
       </c>
       <c r="D18">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E18" t="str">
-        <v>Вольная улица, д. 28/4, к. 1</v>
+        <v>г. посёлок Коммунарка, Бачуринская улица, д. 11А, к. 2</v>
       </c>
       <c r="F18" t="str">
         <v/>
       </c>
       <c r="G18" t="str">
-        <v>Щербаковская, д. 58А</v>
+        <v>г. посёлок Коммунарка, улица Липовый Парк, д. 2</v>
       </c>
       <c r="H18" t="str">
         <v/>
       </c>
       <c r="I18" t="str">
-        <v>Щербаковская улица, д. 20</v>
+        <v>г. Коммунарка, -, д. 7А</v>
       </c>
       <c r="J18" t="str">
-        <v/>
-      </c>
-      <c r="K18" t="str">
-        <v>Суворовская улица, д. 24</v>
-      </c>
-      <c r="L18" t="str">
         <v/>
       </c>
     </row>
@@ -1090,34 +1018,34 @@
         <v>ЛоялАвто</v>
       </c>
       <c r="B19" t="str">
-        <v>Исаев Сергей</v>
+        <v>Наматбеков Майрамбек</v>
       </c>
       <c r="C19" t="str">
-        <v>С703КР12</v>
+        <v>Е885КС979</v>
       </c>
       <c r="D19">
         <v>4</v>
       </c>
       <c r="E19" t="str">
-        <v>улица Речников, д. 14, к. 1</v>
+        <v>улица Горчакова, д. 1</v>
       </c>
       <c r="F19" t="str">
         <v/>
       </c>
       <c r="G19" t="str">
-        <v>проспект Андропова, д. 22</v>
+        <v>Южнобутовская улица, д. 117</v>
       </c>
       <c r="H19" t="str">
         <v/>
       </c>
       <c r="I19" t="str">
-        <v>Нагатинская улица, д. 16</v>
+        <v>г. поселение Воскресенское, Чечёрский проезд, д. 122, к. 1</v>
       </c>
       <c r="J19" t="str">
         <v/>
       </c>
       <c r="K19" t="str">
-        <v>улица Академика Миллионщикова, д. 19</v>
+        <v>Венёвская улица, д. 4</v>
       </c>
       <c r="L19" t="str">
         <v/>
@@ -1128,36 +1056,30 @@
         <v>ЛоялАвто</v>
       </c>
       <c r="B20" t="str">
-        <v>Исхаков Эмиль</v>
+        <v>Некоз Дмитрий</v>
       </c>
       <c r="C20" t="str">
-        <v>А181ВН797</v>
+        <v>Е550УК197</v>
       </c>
       <c r="D20">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E20" t="str">
-        <v>Снайперская улица, д. 9А</v>
+        <v>улица Большая Ордынка, д. 44, стр. 2</v>
       </c>
       <c r="F20" t="str">
         <v/>
       </c>
       <c r="G20" t="str">
-        <v>Кетчерская улица, д. 4Б, стр. 1</v>
+        <v>улица Арбат, д. 4, стр. 1</v>
       </c>
       <c r="H20" t="str">
         <v/>
       </c>
       <c r="I20" t="str">
-        <v>Суздальская улица, д. 12А</v>
+        <v>Газетный переулок, д. 13, стр. 1</v>
       </c>
       <c r="J20" t="str">
-        <v/>
-      </c>
-      <c r="K20" t="str">
-        <v>Лермонтовский проспект, д. 2, к. 1</v>
-      </c>
-      <c r="L20" t="str">
         <v/>
       </c>
     </row>
@@ -1166,24 +1088,36 @@
         <v>ЛоялАвто</v>
       </c>
       <c r="B21" t="str">
-        <v>Ковалев  Андрей</v>
+        <v>Нетреба Юрий</v>
       </c>
       <c r="C21" t="str">
-        <v>М527ЕК777</v>
+        <v>К494РН750</v>
       </c>
       <c r="D21">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E21" t="str">
-        <v>улица Дыбенко, д. 36, к. 4</v>
+        <v>Электролитный проезд, д. 16, к. 1</v>
       </c>
       <c r="F21" t="str">
         <v/>
       </c>
       <c r="G21" t="str">
-        <v>Коровинское шоссе, д. 19, к. 1</v>
+        <v>проспект 60-летия Октября, д. 18, к. 1</v>
       </c>
       <c r="H21" t="str">
+        <v/>
+      </c>
+      <c r="I21" t="str">
+        <v>улица Винокурова, д. 24, к. 4</v>
+      </c>
+      <c r="J21" t="str">
+        <v/>
+      </c>
+      <c r="K21" t="str">
+        <v>Варшавское шоссе, д. 26, стр. 7</v>
+      </c>
+      <c r="L21" t="str">
         <v/>
       </c>
     </row>
@@ -1192,30 +1126,36 @@
         <v>ЛоялАвто</v>
       </c>
       <c r="B22" t="str">
-        <v>Кравченко Андрей</v>
+        <v>Нурбек Ерлан</v>
       </c>
       <c r="C22" t="str">
-        <v>Е273ОК799</v>
+        <v>О811КО797</v>
       </c>
       <c r="D22">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E22" t="str">
-        <v>г. Раменское, Десантная улица, д. 17</v>
+        <v>улица Маршала Рыбалко, д. 2, к. 6, кв. 106</v>
       </c>
       <c r="F22" t="str">
         <v/>
       </c>
       <c r="G22" t="str">
-        <v>г. Жуковский, улица Чкалова, д. 2А, стр. 1</v>
+        <v>улица Расплетина, д. 13</v>
       </c>
       <c r="H22" t="str">
         <v/>
       </c>
       <c r="I22" t="str">
-        <v>г. Жуковский, улица Гагарина, д. 24</v>
+        <v>улица Маршала Новикова, д. 2, к. 2</v>
       </c>
       <c r="J22" t="str">
+        <v/>
+      </c>
+      <c r="K22" t="str">
+        <v>Волоколамское шоссе, д. 1, стр. 1</v>
+      </c>
+      <c r="L22" t="str">
         <v/>
       </c>
     </row>
@@ -1224,36 +1164,30 @@
         <v>ЛоялАвто</v>
       </c>
       <c r="B23" t="str">
-        <v>Макаров Алексей</v>
+        <v>Оганес Мкртчян</v>
       </c>
       <c r="C23" t="str">
-        <v>Р458ХС799</v>
+        <v>Т382УР799</v>
       </c>
       <c r="D23">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E23" t="str">
-        <v>Правобережная улица, д. 1Б</v>
+        <v>г. Щелково, Пушкина, д. 3</v>
       </c>
       <c r="F23" t="str">
         <v/>
       </c>
       <c r="G23" t="str">
-        <v>г. Химки, улица Кирова, д. 10, к. 2</v>
+        <v>г. Королёв, Бурковский проезд, д. 48, к. 2</v>
       </c>
       <c r="H23" t="str">
         <v/>
       </c>
       <c r="I23" t="str">
-        <v>г. Химки, Пролетарская, д. 15, к. 18</v>
+        <v>г. Щелково, 1-й Советский переулок, д. 5</v>
       </c>
       <c r="J23" t="str">
-        <v/>
-      </c>
-      <c r="K23" t="str">
-        <v>г. Химки, улица Чкалова, д. 10/6</v>
-      </c>
-      <c r="L23" t="str">
         <v/>
       </c>
     </row>
@@ -1262,36 +1196,42 @@
         <v>ЛоялАвто</v>
       </c>
       <c r="B24" t="str">
-        <v>Нетреба Юрий</v>
+        <v>Султанов Шамиль</v>
       </c>
       <c r="C24" t="str">
-        <v>К494РН750</v>
+        <v>К392ВК177</v>
       </c>
       <c r="D24">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E24" t="str">
-        <v>г. Люберцы, 1-й Панковский проезд, д. 27А</v>
+        <v>Перовская улица, д. 55</v>
       </c>
       <c r="F24" t="str">
         <v/>
       </c>
       <c r="G24" t="str">
-        <v>г. Лыткарино, Советская, д. 8, к. 2</v>
+        <v>Зелёный проспект, д. 3А, стр. 1</v>
       </c>
       <c r="H24" t="str">
         <v/>
       </c>
       <c r="I24" t="str">
-        <v>г. Октябрьский, улица Ленина, д. 25</v>
+        <v>2-я Владимирская улица, д. 34</v>
       </c>
       <c r="J24" t="str">
         <v/>
       </c>
       <c r="K24" t="str">
-        <v>г. рабочий посёлок Октябрьский, микрорайон Восточный, д. 1</v>
+        <v>Свободный проспект, д. 33А</v>
       </c>
       <c r="L24" t="str">
+        <v/>
+      </c>
+      <c r="M24" t="str">
+        <v>шоссе Энтузиастов, д. 55</v>
+      </c>
+      <c r="N24" t="str">
         <v/>
       </c>
     </row>
@@ -1300,30 +1240,36 @@
         <v>ЛоялАвто</v>
       </c>
       <c r="B25" t="str">
-        <v>Понятков Сергей</v>
+        <v>Филяков Алексей</v>
       </c>
       <c r="C25" t="str">
-        <v>Т466ХН799</v>
+        <v>К726ХЕ777</v>
       </c>
       <c r="D25">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E25" t="str">
-        <v>Плетешковский переулок, д. 17, стр. 1</v>
+        <v>Ленинский проспект, д. 123В</v>
       </c>
       <c r="F25" t="str">
         <v/>
       </c>
       <c r="G25" t="str">
-        <v>Большая Спасская улица, д. 8, стр. 1А</v>
+        <v>Профсоюзная улица, д. 102А</v>
       </c>
       <c r="H25" t="str">
         <v/>
       </c>
       <c r="I25" t="str">
-        <v>Садовая-Черногрязская улица, д. 8, стр. 1</v>
+        <v>Профсоюзная улица, д. 61А</v>
       </c>
       <c r="J25" t="str">
+        <v/>
+      </c>
+      <c r="K25" t="str">
+        <v>Перекопская улица, д. 34, к. 3</v>
+      </c>
+      <c r="L25" t="str">
         <v/>
       </c>
     </row>
@@ -1332,24 +1278,36 @@
         <v>ЛоялАвто</v>
       </c>
       <c r="B26" t="str">
-        <v>Рамазанов Мурад</v>
+        <v>Черноусов  Геннадий</v>
       </c>
       <c r="C26" t="str">
-        <v>А799ВХ790</v>
+        <v>У976ВР799</v>
       </c>
       <c r="D26">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E26" t="str">
-        <v>г. Апрелевка, Сентябрьская улица, д. 5, стр. 2</v>
+        <v>г. Раменское, Десантная улица, д. 17</v>
       </c>
       <c r="F26" t="str">
         <v/>
       </c>
       <c r="G26" t="str">
-        <v>г. Селятино, Клубная, д. 55</v>
+        <v>г. Раменское, Десантная улица, д. 14</v>
       </c>
       <c r="H26" t="str">
+        <v/>
+      </c>
+      <c r="I26" t="str">
+        <v>г. Жуковский, улица Чкалова, д. 2А, стр. 1</v>
+      </c>
+      <c r="J26" t="str">
+        <v/>
+      </c>
+      <c r="K26" t="str">
+        <v>г. Жуковский, улица Горького, д. 4</v>
+      </c>
+      <c r="L26" t="str">
         <v/>
       </c>
     </row>
@@ -1358,138 +1316,132 @@
         <v>ЛоялАвто</v>
       </c>
       <c r="B27" t="str">
-        <v>Султанов Шамиль</v>
+        <v>Шадыканов Руслан</v>
       </c>
       <c r="C27" t="str">
-        <v>К392ВК177</v>
+        <v>О586РВ199</v>
       </c>
       <c r="D27">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E27" t="str">
-        <v>г. Королёв, улица Карла Маркса, д. 1А</v>
+        <v>Дмитровское шоссе, д. 163А, к. 2</v>
       </c>
       <c r="F27" t="str">
         <v/>
       </c>
       <c r="G27" t="str">
-        <v>г. Королёв, улица 50-летия ВЛКСМ, д. 6, к. Е</v>
+        <v>Дмитровское шоссе, д. 169, к. 9</v>
       </c>
       <c r="H27" t="str">
-        <v/>
-      </c>
-      <c r="I27" t="str">
-        <v>г. Королёв, Пионерская улица, д. 30, к. 9</v>
-      </c>
-      <c r="J27" t="str">
         <v/>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="str">
-        <v>ЛоялАвто</v>
+        <v>МАУ</v>
       </c>
       <c r="B28" t="str">
-        <v>Филяков Алексей</v>
+        <v>Власов Александр</v>
       </c>
       <c r="C28" t="str">
-        <v>К726ХЕ777</v>
+        <v>М602МК134</v>
       </c>
       <c r="D28">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E28" t="str">
-        <v>улица Тёплый Стан, д. 10</v>
+        <v>Большая Академическая улица, д. 24, к. 2</v>
       </c>
       <c r="F28" t="str">
         <v/>
       </c>
       <c r="G28" t="str">
-        <v>улица Тёплый Стан, д. 1А</v>
+        <v>Соболевский проезд, д. 22, стр. 1</v>
       </c>
       <c r="H28" t="str">
+        <v/>
+      </c>
+      <c r="I28" t="str">
+        <v>Старопетровский проезд, д. 1, стр. 2</v>
+      </c>
+      <c r="J28" t="str">
+        <v/>
+      </c>
+      <c r="K28" t="str">
+        <v>Ленинградское шоссе, д. 13, к. 1</v>
+      </c>
+      <c r="L28" t="str">
         <v/>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="str">
-        <v>ЛоялАвто</v>
+        <v>МАУ</v>
       </c>
       <c r="B29" t="str">
-        <v>Черноусов  Геннадий</v>
+        <v>Герцев  Ян</v>
       </c>
       <c r="C29" t="str">
-        <v>У976ВР799</v>
+        <v>К609НО790</v>
       </c>
       <c r="D29">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E29" t="str">
-        <v>Измайловский проезд, д. 13</v>
+        <v>улица 26-ти Бакинских Комиссаров, д. 12, к. 2</v>
       </c>
       <c r="F29" t="str">
         <v/>
       </c>
       <c r="G29" t="str">
-        <v>Измайловский проезд, д. 10, к. 3</v>
+        <v>улица Мичуринский Проспект, Олимпийская Деревня, д. 4, к. 2</v>
       </c>
       <c r="H29" t="str">
         <v/>
       </c>
       <c r="I29" t="str">
-        <v>Верхняя Первомайская улица, д. 59/35, к. 3</v>
+        <v>Мичуринский проспект, д. 21, к. 1</v>
       </c>
       <c r="J29" t="str">
-        <v/>
-      </c>
-      <c r="K29" t="str">
-        <v>15-я Парковая улица, д. 48, к. 1</v>
-      </c>
-      <c r="L29" t="str">
         <v/>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="str">
-        <v>ЛоялАвто</v>
+        <v>МАУ</v>
       </c>
       <c r="B30" t="str">
-        <v>Эргешов Тилекбек</v>
+        <v>Глазунов  Роман</v>
       </c>
       <c r="C30" t="str">
-        <v>Р092АВ799</v>
+        <v>Р767АО799</v>
       </c>
       <c r="D30">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E30" t="str">
-        <v>г. Видное, Олимпийская улица, д. 1, к. 2</v>
+        <v>г. Домодедово, улица Гагарина, д. 37</v>
       </c>
       <c r="F30" t="str">
         <v/>
       </c>
       <c r="G30" t="str">
-        <v>г. Видное, Советская улица, д. вл10/1</v>
+        <v>г. Домодедово, Курыжова, д. 30, к. 1</v>
       </c>
       <c r="H30" t="str">
         <v/>
       </c>
       <c r="I30" t="str">
-        <v>г. Видное, Берёзовая улица, д. 11</v>
+        <v>г. Домодедово, Южнодомодедовская улица, д. 16</v>
       </c>
       <c r="J30" t="str">
         <v/>
       </c>
       <c r="K30" t="str">
-        <v>г. Видное, Ольховая улица, д. 9</v>
+        <v>г. Домодедово, улица Корнеева, д. 1</v>
       </c>
       <c r="L30" t="str">
-        <v/>
-      </c>
-      <c r="M30" t="str">
-        <v>г. Видное, проспект Ленинского Комсомола, д. 9, к. 3</v>
-      </c>
-      <c r="N30" t="str">
         <v/>
       </c>
     </row>
@@ -1498,30 +1450,42 @@
         <v>МАУ</v>
       </c>
       <c r="B31" t="str">
-        <v>Виноградов Алексей</v>
+        <v>Головин Виктор</v>
       </c>
       <c r="C31" t="str">
-        <v>Н483ХР77</v>
+        <v>В256УВ777</v>
       </c>
       <c r="D31">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E31" t="str">
-        <v>Лазоревый проезд, д. 1А, к. 1</v>
+        <v>г. Зеленоград, к. 1651</v>
       </c>
       <c r="F31" t="str">
         <v/>
       </c>
       <c r="G31" t="str">
-        <v>Снежная улица, д. 27, к. 1</v>
+        <v>г. Зеленоград, Георгиевский проспект, д. 33, к. 6</v>
       </c>
       <c r="H31" t="str">
         <v/>
       </c>
       <c r="I31" t="str">
-        <v>Радужная улица, д. 4, к. 1</v>
+        <v>г. Зеленоград, -, д. к1562</v>
       </c>
       <c r="J31" t="str">
+        <v/>
+      </c>
+      <c r="K31" t="str">
+        <v>г. Зеленоград, к. 1508</v>
+      </c>
+      <c r="L31" t="str">
+        <v/>
+      </c>
+      <c r="M31" t="str">
+        <v>г. Зеленоград, улица Панфилова, д. 28Б</v>
+      </c>
+      <c r="N31" t="str">
         <v/>
       </c>
     </row>
@@ -1530,28 +1494,28 @@
         <v>МАУ</v>
       </c>
       <c r="B32" t="str">
-        <v>Герцев  Ян</v>
+        <v>Гусейнов Тогрул</v>
       </c>
       <c r="C32" t="str">
-        <v>К609НО790</v>
+        <v>Е857АМ62</v>
       </c>
       <c r="D32">
         <v>3</v>
       </c>
       <c r="E32" t="str">
-        <v>г. Подольск, Бородинский бульвар, д. 7</v>
+        <v>Базовская улица, д. 15, к. 15</v>
       </c>
       <c r="F32" t="str">
         <v/>
       </c>
       <c r="G32" t="str">
-        <v>г. Подольск, Октябрьский проспект, д. 1Б</v>
+        <v>улица Дыбенко, д. 36, к. 4</v>
       </c>
       <c r="H32" t="str">
         <v/>
       </c>
       <c r="I32" t="str">
-        <v>г. Подольск, улица Генерала Варенникова, д. 4</v>
+        <v>Локомотивный проезд, д. 4</v>
       </c>
       <c r="J32" t="str">
         <v/>
@@ -1562,30 +1526,18 @@
         <v>МАУ</v>
       </c>
       <c r="B33" t="str">
-        <v>Глазунов  Роман</v>
+        <v>Иванов Олег</v>
       </c>
       <c r="C33" t="str">
-        <v>Р767АО799</v>
+        <v>У991ММ750</v>
       </c>
       <c r="D33">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E33" t="str">
-        <v>г. Королёв, Пионерская улица, д. 15, к. 2</v>
+        <v>г. Звенигород, Почтовая улица, д. 41, к. 1</v>
       </c>
       <c r="F33" t="str">
-        <v/>
-      </c>
-      <c r="G33" t="str">
-        <v>г. Королёв, улица Тихонравова, д. 26, к. 1</v>
-      </c>
-      <c r="H33" t="str">
-        <v/>
-      </c>
-      <c r="I33" t="str">
-        <v>г. Мытищи, 2-я Институтская улица, д. 26</v>
-      </c>
-      <c r="J33" t="str">
         <v/>
       </c>
     </row>
@@ -1594,28 +1546,28 @@
         <v>МАУ</v>
       </c>
       <c r="B34" t="str">
-        <v>Гусейнов Тогрул</v>
+        <v>Калмыков Александр</v>
       </c>
       <c r="C34" t="str">
-        <v>Е857АМ62</v>
+        <v>М899МК142</v>
       </c>
       <c r="D34">
         <v>3</v>
       </c>
       <c r="E34" t="str">
-        <v>Беговая улица, д. 14</v>
+        <v>г. Сергиев Посад, улица Матросова, д. 2/1, стр. 1</v>
       </c>
       <c r="F34" t="str">
         <v/>
       </c>
       <c r="G34" t="str">
-        <v>Звенигородское шоссе, д. 4</v>
+        <v>г. Сергиев Посад, улица Дружбы, д. 14, к. А</v>
       </c>
       <c r="H34" t="str">
         <v/>
       </c>
       <c r="I34" t="str">
-        <v>Ленинградский проспект, д. 5, стр. 7</v>
+        <v>г. Сергиев Посад, Кооперативная улица, д. 20</v>
       </c>
       <c r="J34" t="str">
         <v/>
@@ -1626,36 +1578,24 @@
         <v>МАУ</v>
       </c>
       <c r="B35" t="str">
-        <v>Иванов Олег</v>
+        <v xml:space="preserve">Марченко Андрей </v>
       </c>
       <c r="C35" t="str">
-        <v>У991ММ750</v>
+        <v>О394НТ46</v>
       </c>
       <c r="D35">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E35" t="str">
-        <v>Варшавское шоссе, д. 141А, к. 2, кв. пом. 5</v>
+        <v>г. Красногорск, Спасская улица, д. 12</v>
       </c>
       <c r="F35" t="str">
         <v/>
       </c>
       <c r="G35" t="str">
-        <v>Россошанский проезд, д. 3</v>
+        <v>г. Красногорск, Красногорский бульвар, д. 14</v>
       </c>
       <c r="H35" t="str">
-        <v/>
-      </c>
-      <c r="I35" t="str">
-        <v>улица Знаменские Садки, д. 1, к. 1</v>
-      </c>
-      <c r="J35" t="str">
-        <v/>
-      </c>
-      <c r="K35" t="str">
-        <v>Старокачаловская, д. 1, к. 2</v>
-      </c>
-      <c r="L35" t="str">
         <v/>
       </c>
     </row>
@@ -1664,28 +1604,28 @@
         <v>МАУ</v>
       </c>
       <c r="B36" t="str">
-        <v>Исаенко Владимир</v>
+        <v>Нуриев Азим</v>
       </c>
       <c r="C36" t="str">
-        <v>Х337ХА750</v>
+        <v>Е322АМ62</v>
       </c>
       <c r="D36">
         <v>3</v>
       </c>
       <c r="E36" t="str">
-        <v>г. Ивантеевка, улица Новая Слобода, д. 3</v>
+        <v>улица Марии Ульяновой, д. 9, к. 3</v>
       </c>
       <c r="F36" t="str">
         <v/>
       </c>
       <c r="G36" t="str">
-        <v>г. Ивантеевка, улица Новосёлки, д. 4</v>
+        <v>улица Удальцова, д. 42</v>
       </c>
       <c r="H36" t="str">
         <v/>
       </c>
       <c r="I36" t="str">
-        <v>г. Ивантеевка, Школьная улица, д. 16</v>
+        <v>улица Кравченко, д. 11</v>
       </c>
       <c r="J36" t="str">
         <v/>
@@ -1696,40 +1636,40 @@
         <v>МАУ</v>
       </c>
       <c r="B37" t="str">
-        <v>Калмыков Александр</v>
+        <v>Сломинский Дмитрий</v>
       </c>
       <c r="C37" t="str">
-        <v>М899МК142</v>
+        <v>В272СУ177</v>
       </c>
       <c r="D37">
         <v>5</v>
       </c>
       <c r="E37" t="str">
-        <v>г. Красногорск, Красногорский бульвар, д. 14</v>
+        <v>Волгоградский проспект, д. 177</v>
       </c>
       <c r="F37" t="str">
         <v/>
       </c>
       <c r="G37" t="str">
-        <v>г. Красногорск, Дачная улица, д. 11А</v>
+        <v>Снайперская улица, д. 9А</v>
       </c>
       <c r="H37" t="str">
         <v/>
       </c>
       <c r="I37" t="str">
-        <v>г. Красногорск, улица Ленина, д. 26А</v>
+        <v>Рязанский проспект, д. 30, к. 2</v>
       </c>
       <c r="J37" t="str">
         <v/>
       </c>
       <c r="K37" t="str">
-        <v>г. Красногорск, улица Жуковского, д. 17</v>
+        <v>Сормовская улица, д. 6</v>
       </c>
       <c r="L37" t="str">
         <v/>
       </c>
       <c r="M37" t="str">
-        <v>г. Красногорск, Заводская улица, д. 18, к. 2</v>
+        <v>Лермонтовский проспект, д. 19, к. 1</v>
       </c>
       <c r="N37" t="str">
         <v/>
@@ -1740,28 +1680,28 @@
         <v>МАУ</v>
       </c>
       <c r="B38" t="str">
-        <v>Манджиев Виталий</v>
+        <v>Трушкин Максим</v>
       </c>
       <c r="C38" t="str">
-        <v>Е399НХ08</v>
+        <v>Р103КЕ790</v>
       </c>
       <c r="D38">
         <v>3</v>
       </c>
       <c r="E38" t="str">
-        <v>г. Мытищи, 1-й Щёлковский проезд, д. 7</v>
+        <v>Кастанаевская улица, д. 45, к. 2</v>
       </c>
       <c r="F38" t="str">
         <v/>
       </c>
       <c r="G38" t="str">
-        <v>г. Мытищи, Олимпийский проспект, д. 36, к. 3</v>
+        <v>площадь Джавахарлала Неру, д. 1</v>
       </c>
       <c r="H38" t="str">
         <v/>
       </c>
       <c r="I38" t="str">
-        <v>г. Мытищи, Вокзальная площадь, д. 2</v>
+        <v>улица Вавилова, д. 66</v>
       </c>
       <c r="J38" t="str">
         <v/>
@@ -1772,36 +1712,42 @@
         <v>МАУ</v>
       </c>
       <c r="B39" t="str">
-        <v xml:space="preserve">Марченко Андрей </v>
+        <v>Хлуденцов Иван</v>
       </c>
       <c r="C39" t="str">
-        <v>О394НТ46</v>
+        <v>О178РН68</v>
       </c>
       <c r="D39">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E39" t="str">
-        <v>Краснобогатырская улица, д. 90, стр. 2</v>
+        <v>г. Дзержинский, Лесная улица, д. 11</v>
       </c>
       <c r="F39" t="str">
         <v/>
       </c>
       <c r="G39" t="str">
-        <v>2-я Прогонная, д. 10</v>
+        <v>Новороссийская улица, д. 24, к. 1</v>
       </c>
       <c r="H39" t="str">
         <v/>
       </c>
       <c r="I39" t="str">
-        <v>улица Космонавтов, д. 22</v>
+        <v>улица Перерва, д. 45</v>
       </c>
       <c r="J39" t="str">
         <v/>
       </c>
       <c r="K39" t="str">
-        <v>Миллионная улица, д. 11, к. 1</v>
+        <v>Братиславская улица, д. 16, к. 1</v>
       </c>
       <c r="L39" t="str">
+        <v/>
+      </c>
+      <c r="M39" t="str">
+        <v>Братиславская улица, д. 33</v>
+      </c>
+      <c r="N39" t="str">
         <v/>
       </c>
     </row>
@@ -1810,28 +1756,28 @@
         <v>МАУ</v>
       </c>
       <c r="B40" t="str">
-        <v>Нуриев Азим</v>
+        <v>Эркинбек Уулу Эмилбек</v>
       </c>
       <c r="C40" t="str">
-        <v>Е322АМ62</v>
+        <v>С174СА777</v>
       </c>
       <c r="D40">
         <v>3</v>
       </c>
       <c r="E40" t="str">
-        <v>г. Химки, Транспортный проезд, д. 3</v>
+        <v>г. Подольск, Февральская улица, д. 54/150</v>
       </c>
       <c r="F40" t="str">
         <v/>
       </c>
       <c r="G40" t="str">
-        <v>г. Химки, улица Горшина, д. 5</v>
+        <v>г. Подольск, улица Генерала Варенникова, д. 4</v>
       </c>
       <c r="H40" t="str">
         <v/>
       </c>
       <c r="I40" t="str">
-        <v>г. Химки, улица имени К.И. Вороницына, д. 1, к. 1</v>
+        <v>г. Подольск, улица 50 лет ВЛКСМ, д. 18, к. А, кв. 13</v>
       </c>
       <c r="J40" t="str">
         <v/>
@@ -1842,34 +1788,34 @@
         <v>МАУ</v>
       </c>
       <c r="B41" t="str">
-        <v>Трушкин Максим</v>
+        <v>Ядренников Андрей</v>
       </c>
       <c r="C41" t="str">
-        <v>Р103КЕ790</v>
+        <v>Н351ХР197</v>
       </c>
       <c r="D41">
         <v>4</v>
       </c>
       <c r="E41" t="str">
-        <v>улица Гурьянова, д. 30</v>
+        <v>Большая Спасская улица, д. 8, стр. 1А</v>
       </c>
       <c r="F41" t="str">
         <v/>
       </c>
       <c r="G41" t="str">
-        <v>5-я Кожуховская улица, д. 9</v>
+        <v>Плетешковский переулок, д. 17, стр. 1</v>
       </c>
       <c r="H41" t="str">
         <v/>
       </c>
       <c r="I41" t="str">
-        <v>улица Мастеркова, д. 6</v>
+        <v>Большая Почтовая улица, д. 43-45, стр. 2</v>
       </c>
       <c r="J41" t="str">
         <v/>
       </c>
       <c r="K41" t="str">
-        <v>Волгоградский проспект, д. 32, к. 2</v>
+        <v>Сокольническая площадь, д. 9А, стр. А</v>
       </c>
       <c r="L41" t="str">
         <v/>
@@ -1880,110 +1826,98 @@
         <v>МАУ</v>
       </c>
       <c r="B42" t="str">
-        <v>Уулу Эмилбек  Эркинбек</v>
+        <v>Ярковский Алексей</v>
       </c>
       <c r="C42" t="str">
-        <v>С174СА777</v>
+        <v>Т973АН790</v>
       </c>
       <c r="D42">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E42" t="str">
-        <v>г. Зеленоград, улица Болдов Ручей, д. 1</v>
+        <v>Суворовская улица, д. 24</v>
       </c>
       <c r="F42" t="str">
         <v/>
       </c>
       <c r="G42" t="str">
-        <v>г. Зеленоград, -, д. 403А, стр. 9</v>
+        <v>улица Космонавтов, д. 22</v>
       </c>
       <c r="H42" t="str">
         <v/>
       </c>
       <c r="I42" t="str">
-        <v>г. Зеленоград, Центральный проспект, д. -, к. 438</v>
+        <v>2-я Прогонная, д. 10</v>
       </c>
       <c r="J42" t="str">
         <v/>
       </c>
       <c r="K42" t="str">
-        <v>г. Химки, Тепличный проезд, д. 8</v>
+        <v>Краснобогатырская улица, д. 90, стр. 2</v>
       </c>
       <c r="L42" t="str">
-        <v/>
-      </c>
-      <c r="M42" t="str">
-        <v>г. Химки, Октябрьская улица, д. 1А</v>
-      </c>
-      <c r="N42" t="str">
         <v/>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="str">
-        <v>МАУ</v>
+        <v>Проект А</v>
       </c>
       <c r="B43" t="str">
-        <v>Черногор Виктор</v>
+        <v>Абдырахман Зайирбек</v>
       </c>
       <c r="C43" t="str">
-        <v>В632ХА799</v>
+        <v>Н600РХ777</v>
       </c>
       <c r="D43">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E43" t="str">
-        <v>г. Щербинка, Индустриальная, д. 9</v>
+        <v>улица Генерала Белобородова, д. 37</v>
       </c>
       <c r="F43" t="str">
         <v/>
       </c>
       <c r="G43" t="str">
-        <v>улица Барышевская Роща, д. 18</v>
+        <v>г. Красногорск, Заводская улица, д. 18, к. 2</v>
       </c>
       <c r="H43" t="str">
-        <v/>
-      </c>
-      <c r="I43" t="str">
-        <v>г. Подольск, Подольская улица, д. 10А</v>
-      </c>
-      <c r="J43" t="str">
         <v/>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="str">
-        <v>МАУ</v>
+        <v>Проект А</v>
       </c>
       <c r="B44" t="str">
-        <v>Ядренников Андрей</v>
+        <v>Алымкулов Акылбек</v>
       </c>
       <c r="C44" t="str">
-        <v>Н351ХР197</v>
+        <v>М769АМ62</v>
       </c>
       <c r="D44">
         <v>4</v>
       </c>
       <c r="E44" t="str">
-        <v>Зарайская улица, д. 26</v>
+        <v>г. Балашиха, улица Свердлова, д. 1А, кв. 151</v>
       </c>
       <c r="F44" t="str">
         <v/>
       </c>
       <c r="G44" t="str">
-        <v>Нижегородская улица, д. 71</v>
+        <v>г. Балашиха, Балашихинское шоссе, д. 10</v>
       </c>
       <c r="H44" t="str">
         <v/>
       </c>
       <c r="I44" t="str">
-        <v>2-й Грайвороновский проезд, д. 44, к. 1</v>
+        <v>г. Балашиха, улица Лукино, д. 55А</v>
       </c>
       <c r="J44" t="str">
         <v/>
       </c>
       <c r="K44" t="str">
-        <v>улица Васильцовский Стан, д. 9</v>
+        <v>г. Балашиха, Кольцевая улица, д. 3К2, к. 2</v>
       </c>
       <c r="L44" t="str">
         <v/>
@@ -1991,21 +1925,39 @@
     </row>
     <row r="45">
       <c r="A45" t="str">
-        <v>МАУ</v>
+        <v>Проект А</v>
       </c>
       <c r="B45" t="str">
-        <v>Ярковский Алексей</v>
+        <v>Артыков Мухамед</v>
       </c>
       <c r="C45" t="str">
-        <v>Т973АН790</v>
+        <v>У659КР136</v>
       </c>
       <c r="D45">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E45" t="str">
-        <v>г. Лобня, улица Ленина, д. 18</v>
+        <v>улица Красного Маяка, д. 15А, стр. 1</v>
       </c>
       <c r="F45" t="str">
+        <v/>
+      </c>
+      <c r="G45" t="str">
+        <v>Чертановская улица, д. 32, к. 1</v>
+      </c>
+      <c r="H45" t="str">
+        <v/>
+      </c>
+      <c r="I45" t="str">
+        <v>Варшавское шоссе, д. вл132/2</v>
+      </c>
+      <c r="J45" t="str">
+        <v/>
+      </c>
+      <c r="K45" t="str">
+        <v>Кировоградская, д. 30</v>
+      </c>
+      <c r="L45" t="str">
         <v/>
       </c>
     </row>
@@ -2014,28 +1966,28 @@
         <v>Проект А</v>
       </c>
       <c r="B46" t="str">
-        <v>Ёров Насруло</v>
+        <v>Аскарбеков Омурбек</v>
       </c>
       <c r="C46" t="str">
-        <v>М712хт197</v>
+        <v>А796ВО750</v>
       </c>
       <c r="D46">
         <v>3</v>
       </c>
       <c r="E46" t="str">
-        <v>г. Сергиев Посад, улица Матросова, д. 2, стр. 1</v>
+        <v>г. поселение Десеновское, 1-я Нововатутинская улица, д. 5</v>
       </c>
       <c r="F46" t="str">
         <v/>
       </c>
       <c r="G46" t="str">
-        <v>г. Сергиев Посад, улица Дружбы, д. 14, к. А</v>
+        <v>г. Московский, улица Хабарова, д. 2</v>
       </c>
       <c r="H46" t="str">
         <v/>
       </c>
       <c r="I46" t="str">
-        <v>г. Сергиев Посад, Кооперативная улица, д. 20</v>
+        <v>г. посёлок Коммунарка, улица Александры Монаховой, д. 96, к. 2</v>
       </c>
       <c r="J46" t="str">
         <v/>
@@ -2046,36 +1998,24 @@
         <v>Проект А</v>
       </c>
       <c r="B47" t="str">
-        <v>Абдырахман Зайирбек</v>
+        <v>Атамкулов Айбек</v>
       </c>
       <c r="C47" t="str">
-        <v>Н600РХ777</v>
+        <v>Е818СВ197</v>
       </c>
       <c r="D47">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E47" t="str">
-        <v>Заводской проезд, д. 10</v>
+        <v>г. Апрелевка, Сентябрьская улица, д. 5, стр. 2</v>
       </c>
       <c r="F47" t="str">
         <v/>
       </c>
       <c r="G47" t="str">
-        <v>9-я Парковая улица, д. 6, к. 1</v>
+        <v>г. Селятино, Клубная, д. 55</v>
       </c>
       <c r="H47" t="str">
-        <v/>
-      </c>
-      <c r="I47" t="str">
-        <v>шоссе Энтузиастов, д. 55</v>
-      </c>
-      <c r="J47" t="str">
-        <v/>
-      </c>
-      <c r="K47" t="str">
-        <v>г. Реутов, Садовый проезд, д. 4А</v>
-      </c>
-      <c r="L47" t="str">
         <v/>
       </c>
     </row>
@@ -2084,30 +2024,36 @@
         <v>Проект А</v>
       </c>
       <c r="B48" t="str">
-        <v>Алымкулов Акылбек</v>
+        <v>Ашурбеков Магомед</v>
       </c>
       <c r="C48" t="str">
-        <v>М769АМ62</v>
+        <v>Т500ВК05</v>
       </c>
       <c r="D48">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E48" t="str">
-        <v>г. Мытищи, улица Комарова, д. 2, к. 2</v>
+        <v>Новотушинский проезд, д. 6, к. 1</v>
       </c>
       <c r="F48" t="str">
         <v/>
       </c>
       <c r="G48" t="str">
-        <v>г. Мытищи, улица Колпакова, д. 10</v>
+        <v>Митинская улица, д. 27</v>
       </c>
       <c r="H48" t="str">
         <v/>
       </c>
       <c r="I48" t="str">
-        <v>г. Мытищи, Новомытищинский проспект, д. 17</v>
+        <v>Митинская улица, д. 55</v>
       </c>
       <c r="J48" t="str">
+        <v/>
+      </c>
+      <c r="K48" t="str">
+        <v>Пятницкое шоссе, д. 15, к. 1</v>
+      </c>
+      <c r="L48" t="str">
         <v/>
       </c>
     </row>
@@ -2116,48 +2062,36 @@
         <v>Проект А</v>
       </c>
       <c r="B49" t="str">
-        <v>Артыков Мухамед</v>
+        <v>Ашуров Рахмуддин</v>
       </c>
       <c r="C49" t="str">
-        <v>У659КР136</v>
+        <v>в135ук33</v>
       </c>
       <c r="D49">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E49" t="str">
-        <v>Большая Академическая улица, д. 24, к. 2</v>
+        <v>Снежная улица, д. 27, к. 1</v>
       </c>
       <c r="F49" t="str">
         <v/>
       </c>
       <c r="G49" t="str">
-        <v>Соболевский проезд, д. 22, стр. 1</v>
+        <v>проезд Дежнёва, д. 29, к. 1</v>
       </c>
       <c r="H49" t="str">
         <v/>
       </c>
       <c r="I49" t="str">
-        <v>проезд Черепановых, д. 36</v>
+        <v>Ясный пр, д. 16</v>
       </c>
       <c r="J49" t="str">
         <v/>
       </c>
       <c r="K49" t="str">
-        <v>Авангардная улица, д. 3</v>
+        <v>Радужная улица, д. 4, к. 1</v>
       </c>
       <c r="L49" t="str">
-        <v/>
-      </c>
-      <c r="M49" t="str">
-        <v>Старопетровский проезд, д. 1, стр. 2</v>
-      </c>
-      <c r="N49" t="str">
-        <v/>
-      </c>
-      <c r="O49" t="str">
-        <v>Ленинградское шоссе, д. 13, к. 1</v>
-      </c>
-      <c r="P49" t="str">
         <v/>
       </c>
     </row>
@@ -2166,28 +2100,28 @@
         <v>Проект А</v>
       </c>
       <c r="B50" t="str">
-        <v>Аскарбеков Омурбек</v>
+        <v>Бабкин Александр</v>
       </c>
       <c r="C50" t="str">
-        <v>А796ВО750</v>
+        <v>Р406АЕ790</v>
       </c>
       <c r="D50">
         <v>3</v>
       </c>
       <c r="E50" t="str">
-        <v>г. Пушкино, Московский проспект, д. 59</v>
+        <v>г. Химки, улица Чкалова, д. 10/6</v>
       </c>
       <c r="F50" t="str">
         <v/>
       </c>
       <c r="G50" t="str">
-        <v>г. Пушкино, микрорайон Серебрянка, д. 48, к. 2</v>
+        <v>г. Химки, улица Кирова, д. 10, к. 2</v>
       </c>
       <c r="H50" t="str">
         <v/>
       </c>
       <c r="I50" t="str">
-        <v>г. Пушкино, Набережная улица, д. 35, к. 6</v>
+        <v>г. Химки, улица Горшина, д. 5</v>
       </c>
       <c r="J50" t="str">
         <v/>
@@ -2198,30 +2132,42 @@
         <v>Проект А</v>
       </c>
       <c r="B51" t="str">
-        <v>Ашурбеков Магомед</v>
+        <v>Бородин Александр</v>
       </c>
       <c r="C51" t="str">
-        <v>Т500ВК05</v>
+        <v>О519КО</v>
       </c>
       <c r="D51">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E51" t="str">
-        <v>Большая Тульская улица, д. 13</v>
+        <v>г. Видное, Олимпийская улица, д. 1, к. 2</v>
       </c>
       <c r="F51" t="str">
         <v/>
       </c>
       <c r="G51" t="str">
-        <v>2-й Донской проезд, д. 10, стр. 2</v>
+        <v>г. Видное, Советская улица, д. вл10/1</v>
       </c>
       <c r="H51" t="str">
         <v/>
       </c>
       <c r="I51" t="str">
-        <v>улица Серпуховский Вал, д. 17, к. 1</v>
+        <v>г. Видное, Берёзовая улица, д. 11</v>
       </c>
       <c r="J51" t="str">
+        <v/>
+      </c>
+      <c r="K51" t="str">
+        <v>г. Видное, Ольховая улица, д. 9</v>
+      </c>
+      <c r="L51" t="str">
+        <v/>
+      </c>
+      <c r="M51" t="str">
+        <v>г. Видное, проспект Ленинского Комсомола, д. 9, к. 3</v>
+      </c>
+      <c r="N51" t="str">
         <v/>
       </c>
     </row>
@@ -2230,34 +2176,34 @@
         <v>Проект А</v>
       </c>
       <c r="B52" t="str">
-        <v>Бордашевский Сергей</v>
+        <v>Дубанакулов Адылбек</v>
       </c>
       <c r="C52" t="str">
-        <v>У624ЕХ777</v>
+        <v>С746НА790</v>
       </c>
       <c r="D52">
         <v>4</v>
       </c>
       <c r="E52" t="str">
-        <v>Каширское шоссе, д. 80</v>
+        <v>Семеновский пер., д. 18</v>
       </c>
       <c r="F52" t="str">
         <v/>
       </c>
       <c r="G52" t="str">
-        <v>Варшавское шоссе, д. 26, стр. 7</v>
+        <v>Щербаковская улица, д. 20</v>
       </c>
       <c r="H52" t="str">
         <v/>
       </c>
       <c r="I52" t="str">
-        <v>Электролитный проезд, д. 16, к. 1</v>
+        <v>Открытое шоссе, д. 24, к. 11</v>
       </c>
       <c r="J52" t="str">
         <v/>
       </c>
       <c r="K52" t="str">
-        <v>улица Борисовские Пруды, д. 8А</v>
+        <v>Амурская улица, д. 19</v>
       </c>
       <c r="L52" t="str">
         <v/>
@@ -2268,28 +2214,28 @@
         <v>Проект А</v>
       </c>
       <c r="B53" t="str">
-        <v>Дандиев  Эрмек</v>
+        <v>Дубанакулов Бактилек</v>
       </c>
       <c r="C53" t="str">
-        <v>у042еа797</v>
+        <v>Х938КМ37</v>
       </c>
       <c r="D53">
         <v>3</v>
       </c>
       <c r="E53" t="str">
-        <v>г. Солнечногорск, Крестьянская улица, д. 7</v>
+        <v>г. Химки, улица имени К.И. Вороницына, д. 1, к. 1</v>
       </c>
       <c r="F53" t="str">
         <v/>
       </c>
       <c r="G53" t="str">
-        <v>г. Солнечногорск, Обуховская улица, д. 50Б</v>
+        <v>г. Химки, Транспортный проезд, д. 3</v>
       </c>
       <c r="H53" t="str">
         <v/>
       </c>
       <c r="I53" t="str">
-        <v>г. деревня Голубое, Тверецкий проезд, д. 16, к. 3</v>
+        <v>г. Химки, Пролетарская, д. 15, к. 18</v>
       </c>
       <c r="J53" t="str">
         <v/>
@@ -2300,36 +2246,24 @@
         <v>Проект А</v>
       </c>
       <c r="B54" t="str">
-        <v>Дубанакулов Адылбек</v>
+        <v>Исаков Гулмырза</v>
       </c>
       <c r="C54" t="str">
-        <v>С746НА790</v>
+        <v>Т754ММ142</v>
       </c>
       <c r="D54">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E54" t="str">
-        <v>г. Балашиха, Кольцевая улица, д. 3К2, к. 2</v>
+        <v>г. Щёлково, улица Радиоцентра № 5, д. 16</v>
       </c>
       <c r="F54" t="str">
         <v/>
       </c>
       <c r="G54" t="str">
-        <v>г. Балашиха, Балашихинское шоссе, д. 10</v>
+        <v>г. Лосино-Петровский, улица Гоголя, д. 21</v>
       </c>
       <c r="H54" t="str">
-        <v/>
-      </c>
-      <c r="I54" t="str">
-        <v>г. Балашиха, улица Лукино, д. 55А</v>
-      </c>
-      <c r="J54" t="str">
-        <v/>
-      </c>
-      <c r="K54" t="str">
-        <v>Хабаровская улица, д. 4, к. 1</v>
-      </c>
-      <c r="L54" t="str">
         <v/>
       </c>
     </row>
@@ -2338,30 +2272,24 @@
         <v>Проект А</v>
       </c>
       <c r="B55" t="str">
-        <v>Дубанакулов Бактилек</v>
+        <v>Кандаров Азиз</v>
       </c>
       <c r="C55" t="str">
-        <v>Х938КМ37</v>
+        <v>К331ТХ750</v>
       </c>
       <c r="D55">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E55" t="str">
-        <v>г. Мытищи, улица Семашко, д. 25</v>
+        <v>улица Габричевского, д. 10, к. 1</v>
       </c>
       <c r="F55" t="str">
         <v/>
       </c>
       <c r="G55" t="str">
-        <v>улица Конёнкова, д. 23</v>
+        <v>улица Маршала Катукова, д. 3, к. 1</v>
       </c>
       <c r="H55" t="str">
-        <v/>
-      </c>
-      <c r="I55" t="str">
-        <v>Плещеева, д. 8</v>
-      </c>
-      <c r="J55" t="str">
         <v/>
       </c>
     </row>
@@ -2370,30 +2298,36 @@
         <v>Проект А</v>
       </c>
       <c r="B56" t="str">
-        <v>Исаков Саматбек</v>
+        <v>Магамедов Мурад Р</v>
       </c>
       <c r="C56" t="str">
-        <v>У852ММ77</v>
+        <v>К056НЕ799</v>
       </c>
       <c r="D56">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E56" t="str">
-        <v>г. Мытищи, Борисовка, д. 20А</v>
+        <v>Большая Тульская улица, д. 13</v>
       </c>
       <c r="F56" t="str">
         <v/>
       </c>
       <c r="G56" t="str">
-        <v>г. Мытищи, проспект Астрахова, д. 6</v>
+        <v>2-й Донской проезд, д. 10, стр. 2</v>
       </c>
       <c r="H56" t="str">
         <v/>
       </c>
       <c r="I56" t="str">
-        <v>г. Мытищи, Олимпийский проспект, д. вл13с1, стр. 1, к. Б</v>
+        <v>улица Серпуховский Вал, д. 17, к. 1</v>
       </c>
       <c r="J56" t="str">
+        <v/>
+      </c>
+      <c r="K56" t="str">
+        <v>Севастопольский проспект, д. 11Е</v>
+      </c>
+      <c r="L56" t="str">
         <v/>
       </c>
     </row>
@@ -2402,36 +2336,24 @@
         <v>Проект А</v>
       </c>
       <c r="B57" t="str">
-        <v>Кандаров Азиз</v>
+        <v>Мадалиев Максат</v>
       </c>
       <c r="C57" t="str">
-        <v>К331ТХ750</v>
+        <v>е315ку19</v>
       </c>
       <c r="D57">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E57" t="str">
-        <v>Бирюлёвская улица, д. 43</v>
+        <v>г. Одинцово, Белорусская улица, д. 5</v>
       </c>
       <c r="F57" t="str">
         <v/>
       </c>
       <c r="G57" t="str">
-        <v>Загорьевская, д. 5</v>
+        <v>г. Лесной Городок, Фасадная, д. 2, к. 1</v>
       </c>
       <c r="H57" t="str">
-        <v/>
-      </c>
-      <c r="I57" t="str">
-        <v>Булатниковский проезд, д. 2В, к. 4</v>
-      </c>
-      <c r="J57" t="str">
-        <v/>
-      </c>
-      <c r="K57" t="str">
-        <v>Булатниковская улица, д. 2А</v>
-      </c>
-      <c r="L57" t="str">
         <v/>
       </c>
     </row>
@@ -2440,48 +2362,36 @@
         <v>Проект А</v>
       </c>
       <c r="B58" t="str">
-        <v>Керимов Парвиз</v>
+        <v>Максат Азамат</v>
       </c>
       <c r="C58" t="str">
-        <v>А695ХС750</v>
+        <v>К220ко77</v>
       </c>
       <c r="D58">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E58" t="str">
-        <v>Волоколамское шоссе, д. 15/22, кв. 1</v>
+        <v>г. Мытищи, улица Колпакова, д. 10</v>
       </c>
       <c r="F58" t="str">
         <v/>
       </c>
       <c r="G58" t="str">
-        <v>Волоколамское шоссе, д. 1, стр. 1</v>
+        <v>г. Мытищи, Борисовка, д. 20А</v>
       </c>
       <c r="H58" t="str">
         <v/>
       </c>
       <c r="I58" t="str">
-        <v>улица Маршала Бирюзова, д. 4, к. 1</v>
+        <v>г. Мытищи, Лётная улица, д. 27А</v>
       </c>
       <c r="J58" t="str">
         <v/>
       </c>
       <c r="K58" t="str">
-        <v>улица Маршала Тухачевского, д. 50, к. 2</v>
+        <v>г. Мытищи, Новомытищинский проспект, д. 17</v>
       </c>
       <c r="L58" t="str">
-        <v/>
-      </c>
-      <c r="M58" t="str">
-        <v>проспект Маршала Жукова, д. 49</v>
-      </c>
-      <c r="N58" t="str">
-        <v/>
-      </c>
-      <c r="O58" t="str">
-        <v>улица Мнёвники, д. 23</v>
-      </c>
-      <c r="P58" t="str">
         <v/>
       </c>
     </row>
@@ -2490,30 +2400,36 @@
         <v>Проект А</v>
       </c>
       <c r="B59" t="str">
-        <v>Лялин Генадий</v>
+        <v>Максат Бакытбек</v>
       </c>
       <c r="C59" t="str">
-        <v>Е127ту69</v>
+        <v>А060УА69</v>
       </c>
       <c r="D59">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E59" t="str">
-        <v>проезд Дежнёва, д. 29, к. 1</v>
+        <v>Новокузнецкая улица, д. 13, стр. 1</v>
       </c>
       <c r="F59" t="str">
         <v/>
       </c>
       <c r="G59" t="str">
-        <v>Ясный пр, д. 16</v>
+        <v>2-й Грайвороновский проезд, д. 44, к. 1</v>
       </c>
       <c r="H59" t="str">
         <v/>
       </c>
       <c r="I59" t="str">
-        <v>Широкая улица, д. 7, к. 2</v>
+        <v>Зарайская улица, д. 26</v>
       </c>
       <c r="J59" t="str">
+        <v/>
+      </c>
+      <c r="K59" t="str">
+        <v>улица Михайлова, д. 31А</v>
+      </c>
+      <c r="L59" t="str">
         <v/>
       </c>
     </row>
@@ -2522,36 +2438,24 @@
         <v>Проект А</v>
       </c>
       <c r="B60" t="str">
-        <v>Мадалиев Максат</v>
+        <v>Мамытов Усон</v>
       </c>
       <c r="C60" t="str">
-        <v>е315ку19</v>
+        <v>в402но790</v>
       </c>
       <c r="D60">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E60" t="str">
-        <v>г. Красногорск, бульвар Космонавтов, д. 17</v>
+        <v>г. Солнечногорск, Обуховская улица, д. 50Б</v>
       </c>
       <c r="F60" t="str">
         <v/>
       </c>
       <c r="G60" t="str">
-        <v>г. Красногорск, Светлая улица, д. 3А, стр. 4</v>
+        <v>г. деревня Голубое, Тверецкий проезд, д. 16, к. 3</v>
       </c>
       <c r="H60" t="str">
-        <v/>
-      </c>
-      <c r="I60" t="str">
-        <v>г. Дедовск, 1-ая Главная, д. 1</v>
-      </c>
-      <c r="J60" t="str">
-        <v/>
-      </c>
-      <c r="K60" t="str">
-        <v>г. Звенигород, Почтовая улица, д. 41, к. 1</v>
-      </c>
-      <c r="L60" t="str">
         <v/>
       </c>
     </row>
@@ -2560,30 +2464,24 @@
         <v>Проект А</v>
       </c>
       <c r="B61" t="str">
-        <v>Максат Азамат</v>
+        <v>Мирзакулов Талантбек</v>
       </c>
       <c r="C61" t="str">
-        <v>К220ко77</v>
+        <v>В549ТР62</v>
       </c>
       <c r="D61">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E61" t="str">
-        <v>Долгоруковская улица, д. 40, кв. 10</v>
+        <v>Таллинская улица, д. 16, к. 1</v>
       </c>
       <c r="F61" t="str">
         <v/>
       </c>
       <c r="G61" t="str">
-        <v>Тихвинская улица, д. 20</v>
+        <v>Маршала Катукова, д. 24, к. 4</v>
       </c>
       <c r="H61" t="str">
-        <v/>
-      </c>
-      <c r="I61" t="str">
-        <v>улица Лобачика, д. 23, к. 1</v>
-      </c>
-      <c r="J61" t="str">
         <v/>
       </c>
     </row>
@@ -2592,42 +2490,36 @@
         <v>Проект А</v>
       </c>
       <c r="B62" t="str">
-        <v>Мамытов Усон</v>
+        <v>Нарынбеков Дастан</v>
       </c>
       <c r="C62" t="str">
-        <v>в402но790</v>
+        <v>у820вх797</v>
       </c>
       <c r="D62">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E62" t="str">
-        <v>г. Долгопрудный, Московское шоссе, д. 37, к. А</v>
+        <v>Звенигородское шоссе, д. 4</v>
       </c>
       <c r="F62" t="str">
         <v/>
       </c>
       <c r="G62" t="str">
-        <v>г. Долгопрудный, Лихачёвское шоссе, д. 6</v>
+        <v>улица Маршала Тухачевского, д. 50, к. 2</v>
       </c>
       <c r="H62" t="str">
         <v/>
       </c>
       <c r="I62" t="str">
-        <v>г. Долгопрудный, проспект Пацаева, д. 12</v>
+        <v>проспект Маршала Жукова, д. 49</v>
       </c>
       <c r="J62" t="str">
         <v/>
       </c>
       <c r="K62" t="str">
-        <v>г. Долгопрудный, Набережная улица, д. 31</v>
+        <v>улица Мнёвники, д. 23</v>
       </c>
       <c r="L62" t="str">
-        <v/>
-      </c>
-      <c r="M62" t="str">
-        <v>Дмитровское шоссе, д. 169, к. 9</v>
-      </c>
-      <c r="N62" t="str">
         <v/>
       </c>
     </row>
@@ -2636,36 +2528,30 @@
         <v>Проект А</v>
       </c>
       <c r="B63" t="str">
-        <v>Мирзакулов Талантбек</v>
+        <v>Омошев Бекмырза</v>
       </c>
       <c r="C63" t="str">
-        <v>В549ТР62</v>
+        <v>Х011ЕС37</v>
       </c>
       <c r="D63">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E63" t="str">
-        <v>Свободный проспект, д. 33А</v>
+        <v>Дорогобужская улица, д. 3</v>
       </c>
       <c r="F63" t="str">
         <v/>
       </c>
       <c r="G63" t="str">
-        <v>2-я Владимирская улица, д. 34</v>
+        <v>Ярцевская улица, д. 19</v>
       </c>
       <c r="H63" t="str">
         <v/>
       </c>
       <c r="I63" t="str">
-        <v>Зелёный проспект, д. 3А, стр. 1</v>
+        <v>улица Толбухина, д. 13, к. 1</v>
       </c>
       <c r="J63" t="str">
-        <v/>
-      </c>
-      <c r="K63" t="str">
-        <v>Перовская улица, д. 55</v>
-      </c>
-      <c r="L63" t="str">
         <v/>
       </c>
     </row>
@@ -2674,40 +2560,40 @@
         <v>Проект А</v>
       </c>
       <c r="B64" t="str">
-        <v>Мирзамомун Аднаев</v>
+        <v>Омошев Замир</v>
       </c>
       <c r="C64" t="str">
-        <v>О815НВ190</v>
+        <v>о122нт790</v>
       </c>
       <c r="D64">
         <v>5</v>
       </c>
       <c r="E64" t="str">
-        <v>г. Дзержинский, Лесная улица, д. 11</v>
+        <v>Каширское шоссе, д. 65, к. 3</v>
       </c>
       <c r="F64" t="str">
         <v/>
       </c>
       <c r="G64" t="str">
-        <v>г. Котельники, Кузьминская улица, д. 17</v>
+        <v>Каширское шоссе (дублёр), д. 61, к. 3А</v>
       </c>
       <c r="H64" t="str">
         <v/>
       </c>
       <c r="I64" t="str">
-        <v>г. Люберцы, Новорязанское шоссе, д. 1А</v>
+        <v>улица Генерала Белова, д. 43, к. 2</v>
       </c>
       <c r="J64" t="str">
         <v/>
       </c>
       <c r="K64" t="str">
-        <v>Жулебинский бульвар, д. 30, к. 1</v>
+        <v>Гурьевский проезд, д. 17, к. 1</v>
       </c>
       <c r="L64" t="str">
         <v/>
       </c>
       <c r="M64" t="str">
-        <v>Лермонтовский проспект, д. 19, к. 1</v>
+        <v>Ясеневая улица, д. 29</v>
       </c>
       <c r="N64" t="str">
         <v/>
@@ -2718,30 +2604,42 @@
         <v>Проект А</v>
       </c>
       <c r="B65" t="str">
-        <v>Нематжанов Миразиз</v>
+        <v>Райев Жаныбек</v>
       </c>
       <c r="C65" t="str">
-        <v>а314тм62</v>
+        <v>Р394ММ40</v>
       </c>
       <c r="D65">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E65" t="str">
-        <v>Перекопская улица, д. 34, к. 3</v>
+        <v>г. Люберцы, Московская улица, д. 11</v>
       </c>
       <c r="F65" t="str">
         <v/>
       </c>
       <c r="G65" t="str">
-        <v>Профсоюзная улица, д. 61А</v>
+        <v>г. Люберцы, Новорязанское шоссе, д. 1А</v>
       </c>
       <c r="H65" t="str">
         <v/>
       </c>
       <c r="I65" t="str">
-        <v>Чонгарский бульвар, д. 26А, к. 3</v>
+        <v>Жулебинский бульвар, д. 30, к. 1</v>
       </c>
       <c r="J65" t="str">
+        <v/>
+      </c>
+      <c r="K65" t="str">
+        <v>г. Люберцы, улица Кирова, д. 9, к. 5</v>
+      </c>
+      <c r="L65" t="str">
+        <v/>
+      </c>
+      <c r="M65" t="str">
+        <v>г. Люберцы, Комсомольский проспект, д. 7/1</v>
+      </c>
+      <c r="N65" t="str">
         <v/>
       </c>
     </row>
@@ -2750,36 +2648,42 @@
         <v>Проект А</v>
       </c>
       <c r="B66" t="str">
-        <v>Омошев Замир</v>
+        <v xml:space="preserve">Рамазанов Ибрагим </v>
       </c>
       <c r="C66" t="str">
-        <v>о122нт790</v>
+        <v>р034кт05</v>
       </c>
       <c r="D66">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E66" t="str">
-        <v>г. Домодедово, Курыжова, д. 30, к. 1</v>
+        <v>Донецкая улица, д. 34, к. 1</v>
       </c>
       <c r="F66" t="str">
         <v/>
       </c>
       <c r="G66" t="str">
-        <v>г. Домодедово, Южнодомодедовская улица, д. 16</v>
+        <v>улица Перерва, д. 32</v>
       </c>
       <c r="H66" t="str">
         <v/>
       </c>
       <c r="I66" t="str">
-        <v>г. Домодедово, улица Корнеева, д. 1</v>
+        <v>Люблинская улица, д. 102А</v>
       </c>
       <c r="J66" t="str">
         <v/>
       </c>
       <c r="K66" t="str">
-        <v>г. Домодедово, улица Гагарина, д. 37</v>
+        <v>Братеевская улица, д. 16, к. 6</v>
       </c>
       <c r="L66" t="str">
+        <v/>
+      </c>
+      <c r="M66" t="str">
+        <v>Паромная улица, д. 9, к. 1</v>
+      </c>
+      <c r="N66" t="str">
         <v/>
       </c>
     </row>
@@ -2788,30 +2692,36 @@
         <v>Проект А</v>
       </c>
       <c r="B67" t="str">
-        <v>Осконбаев Камчыбек</v>
+        <v>Сагындыков Бекназар</v>
       </c>
       <c r="C67" t="str">
-        <v>х015тх69</v>
+        <v>К417НК790</v>
       </c>
       <c r="D67">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E67" t="str">
-        <v>Севастопольский проспект, д. 11Е</v>
+        <v>бульвар Яна Райниса, д. 31</v>
       </c>
       <c r="F67" t="str">
         <v/>
       </c>
       <c r="G67" t="str">
-        <v>улица Винокурова, д. 24, к. 4</v>
+        <v>улица Героев Панфиловцев, д. 1А, кв. 211</v>
       </c>
       <c r="H67" t="str">
         <v/>
       </c>
       <c r="I67" t="str">
-        <v>проспект 60-летия Октября, д. 18, к. 1</v>
+        <v>Планерная улица, д. 7</v>
       </c>
       <c r="J67" t="str">
+        <v/>
+      </c>
+      <c r="K67" t="str">
+        <v>г. деревня Путилково, Новотушинская улица, д. 2</v>
+      </c>
+      <c r="L67" t="str">
         <v/>
       </c>
     </row>
@@ -2820,42 +2730,36 @@
         <v>Проект А</v>
       </c>
       <c r="B68" t="str">
-        <v>Пулатов Играм</v>
+        <v>Солтанов  Эмиль</v>
       </c>
       <c r="C68" t="str">
-        <v>К486РК190</v>
+        <v>А602КМ797</v>
       </c>
       <c r="D68">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E68" t="str">
-        <v>Дубнинская, д. 3</v>
+        <v>улица Маршала Савицкого, д. 18, к. 2</v>
       </c>
       <c r="F68" t="str">
         <v/>
       </c>
       <c r="G68" t="str">
-        <v>Дубнинская улица, д. 53, к. 3</v>
+        <v>г. Подольск, Ленина, д. 14</v>
       </c>
       <c r="H68" t="str">
         <v/>
       </c>
       <c r="I68" t="str">
-        <v>Селигерская, д. 18, к. 3</v>
+        <v>г. Подольск, Подольская улица, д. 10А</v>
       </c>
       <c r="J68" t="str">
         <v/>
       </c>
       <c r="K68" t="str">
-        <v>Дмитровское шоссе, д. 68</v>
+        <v>г. Подольск, Быковская улица, д. 10</v>
       </c>
       <c r="L68" t="str">
-        <v/>
-      </c>
-      <c r="M68" t="str">
-        <v>Дубнинская улица, д. 12Б, стр. 12</v>
-      </c>
-      <c r="N68" t="str">
         <v/>
       </c>
     </row>
@@ -2864,24 +2768,30 @@
         <v>Проект А</v>
       </c>
       <c r="B69" t="str">
-        <v>Райев Жаныбек</v>
+        <v>Сулейманов Ибаят</v>
       </c>
       <c r="C69" t="str">
-        <v>Р394ММ40</v>
+        <v>А320ТР62</v>
       </c>
       <c r="D69">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E69" t="str">
-        <v>г. Раменское, улица Чугунова, д. 32А</v>
+        <v>улица 8 Марта, д. 6</v>
       </c>
       <c r="F69" t="str">
         <v/>
       </c>
       <c r="G69" t="str">
-        <v>г. Раменское, улица Михалевича, д. 5</v>
+        <v>4-й Вятский переулок, д. 18, к. 2</v>
       </c>
       <c r="H69" t="str">
+        <v/>
+      </c>
+      <c r="I69" t="str">
+        <v>Тихвинская улица, д. 20</v>
+      </c>
+      <c r="J69" t="str">
         <v/>
       </c>
     </row>
@@ -2890,48 +2800,30 @@
         <v>Проект А</v>
       </c>
       <c r="B70" t="str">
-        <v xml:space="preserve">Рамазанов Ибрагим </v>
+        <v>Токтогулов Асан</v>
       </c>
       <c r="C70" t="str">
-        <v>р034кт05</v>
+        <v>а638тр62</v>
       </c>
       <c r="D70">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E70" t="str">
-        <v>Тушинская улица, д. 17</v>
+        <v>1-й Очаковский переулок, д. 1</v>
       </c>
       <c r="F70" t="str">
         <v/>
       </c>
       <c r="G70" t="str">
-        <v>улица Свободы, д. 40, к. 1</v>
+        <v>улица Наташи Ковшовой, д. 8А, стр. А</v>
       </c>
       <c r="H70" t="str">
         <v/>
       </c>
       <c r="I70" t="str">
-        <v>улица Героев Панфиловцев, д. 1А, кв. 211</v>
+        <v>Озёрная улица, д. 42</v>
       </c>
       <c r="J70" t="str">
-        <v/>
-      </c>
-      <c r="K70" t="str">
-        <v>бульвар Яна Райниса, д. 31</v>
-      </c>
-      <c r="L70" t="str">
-        <v/>
-      </c>
-      <c r="M70" t="str">
-        <v>Походный проезд, д. 4, к. 1</v>
-      </c>
-      <c r="N70" t="str">
-        <v/>
-      </c>
-      <c r="O70" t="str">
-        <v>г. Красногорск, Спасская улица, д. 12</v>
-      </c>
-      <c r="P70" t="str">
         <v/>
       </c>
     </row>
@@ -2940,36 +2832,30 @@
         <v>Проект А</v>
       </c>
       <c r="B71" t="str">
-        <v>Токтогулов Асан</v>
+        <v xml:space="preserve">Умаралиев  Мухамед </v>
       </c>
       <c r="C71" t="str">
-        <v>а638тр62</v>
+        <v>с851ак777</v>
       </c>
       <c r="D71">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E71" t="str">
-        <v>г. Балашиха, улица Евстафьева, д. 1/9</v>
+        <v>г. Балашиха, улица Ленина, д. 1/5, к. 5</v>
       </c>
       <c r="F71" t="str">
         <v/>
       </c>
       <c r="G71" t="str">
-        <v>г. Балашиха, шоссе Энтузиастов, д. вл1Алит6В</v>
+        <v>г. микрорайон Железнодорожный, Балашиха, Андрея Белого, д. 1</v>
       </c>
       <c r="H71" t="str">
         <v/>
       </c>
       <c r="I71" t="str">
-        <v>г. Реутов, Комсомольская улица, д. 21, к. 1</v>
+        <v>г. Балашиха, Речная, д. 5</v>
       </c>
       <c r="J71" t="str">
-        <v/>
-      </c>
-      <c r="K71" t="str">
-        <v>г. Реутов, Ленина, д. 21</v>
-      </c>
-      <c r="L71" t="str">
         <v/>
       </c>
     </row>
@@ -2978,42 +2864,30 @@
         <v>Проект А</v>
       </c>
       <c r="B72" t="str">
-        <v>Турсуналиев Женишбек</v>
+        <v>Хапизов Алтынбек</v>
       </c>
       <c r="C72" t="str">
-        <v>Т440ЕК138</v>
+        <v>У362УТ71</v>
       </c>
       <c r="D72">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E72" t="str">
-        <v>г. Зеленоград, Георгиевский проспект, д. 33, к. 6</v>
+        <v>бульвар Академика Ландау, д. 3</v>
       </c>
       <c r="F72" t="str">
         <v/>
       </c>
       <c r="G72" t="str">
-        <v>г. Зеленоград, -, д. к1562</v>
+        <v>улица Конёнкова, д. 23</v>
       </c>
       <c r="H72" t="str">
         <v/>
       </c>
       <c r="I72" t="str">
-        <v>г. Зеленоград, к. 1508</v>
+        <v>Широкая улица, д. 7, к. 2</v>
       </c>
       <c r="J72" t="str">
-        <v/>
-      </c>
-      <c r="K72" t="str">
-        <v>г. Зеленоград, улица Лётчицы Тарасовой, к. 2022</v>
-      </c>
-      <c r="L72" t="str">
-        <v/>
-      </c>
-      <c r="M72" t="str">
-        <v>г. Зеленоград, улица Панфилова, д. 28Б</v>
-      </c>
-      <c r="N72" t="str">
         <v/>
       </c>
     </row>
@@ -3022,24 +2896,30 @@
         <v>Проект А</v>
       </c>
       <c r="B73" t="str">
-        <v>Уланбеков  Самат</v>
+        <v>Чолпонбек Асан</v>
       </c>
       <c r="C73" t="str">
-        <v>А221ВХ76</v>
+        <v>в877ме77</v>
       </c>
       <c r="D73">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E73" t="str">
-        <v>Ленинский проспект, д. 123В</v>
+        <v>3-й Сетуньский проезд, д. 16</v>
       </c>
       <c r="F73" t="str">
         <v/>
       </c>
       <c r="G73" t="str">
-        <v>улица 26-ти Бакинских Комиссаров, д. 12, к. 2</v>
+        <v>Мосфильмовская улица, д. 27</v>
       </c>
       <c r="H73" t="str">
+        <v/>
+      </c>
+      <c r="I73" t="str">
+        <v>Ленинский проспект, д. 44</v>
+      </c>
+      <c r="J73" t="str">
         <v/>
       </c>
     </row>
@@ -3048,122 +2928,110 @@
         <v>Проект А</v>
       </c>
       <c r="B74" t="str">
-        <v xml:space="preserve">Умаралиев  Мухамед </v>
+        <v>Чыйбылов Сталбек</v>
       </c>
       <c r="C74" t="str">
-        <v>с851ак777</v>
+        <v>с495оа89</v>
       </c>
       <c r="D74">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E74" t="str">
-        <v>улица Дубки, д. 4А</v>
+        <v>г. Реутов, Комсомольская улица, д. 21, к. 1</v>
       </c>
       <c r="F74" t="str">
         <v/>
       </c>
       <c r="G74" t="str">
-        <v>4-й Вятский переулок, д. 18, к. 2</v>
+        <v>г. Балашиха, улица Некрасова, д. 13А</v>
       </c>
       <c r="H74" t="str">
         <v/>
       </c>
       <c r="I74" t="str">
-        <v>улица 8 Марта, д. 6</v>
+        <v>г. Старая Купавна, Октябрьская улица, д. 19</v>
       </c>
       <c r="J74" t="str">
         <v/>
       </c>
       <c r="K74" t="str">
-        <v>Самеда Вургуна, д. 11</v>
+        <v>г. Балашиха, шоссе Энтузиастов, д. вл1Алит6В</v>
       </c>
       <c r="L74" t="str">
-        <v/>
-      </c>
-      <c r="M74" t="str">
-        <v>улица Полины Осипенко, д. 8</v>
-      </c>
-      <c r="N74" t="str">
         <v/>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="str">
-        <v>Проект А</v>
+        <v>СТРИТ ЛОГИСТИК</v>
       </c>
       <c r="B75" t="str">
-        <v>Хапизов Алтынбек</v>
+        <v>Бакланов Сергей</v>
       </c>
       <c r="C75" t="str">
-        <v>У362УТ71</v>
+        <v>В979ЕХ979</v>
       </c>
       <c r="D75">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E75" t="str">
-        <v>Новороссийская улица, д. 24, к. 1</v>
+        <v>Волгоградский проспект, д. 32, к. 2</v>
       </c>
       <c r="F75" t="str">
         <v/>
       </c>
       <c r="G75" t="str">
-        <v>Краснодарская улица, д. 16</v>
+        <v>улица Мастеркова, д. 6</v>
       </c>
       <c r="H75" t="str">
         <v/>
       </c>
       <c r="I75" t="str">
-        <v>улица Артюхиной, д. 24, к. 1</v>
+        <v>5-я Кожуховская улица, д. 9</v>
       </c>
       <c r="J75" t="str">
         <v/>
       </c>
       <c r="K75" t="str">
-        <v>Волжский бульвар, д. 38</v>
+        <v>улица Гурьянова, д. 30</v>
       </c>
       <c r="L75" t="str">
-        <v/>
-      </c>
-      <c r="M75" t="str">
-        <v>улица Юных Ленинцев, д. 52</v>
-      </c>
-      <c r="N75" t="str">
         <v/>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="str">
-        <v>Проект А</v>
+        <v>СТРИТ ЛОГИСТИК</v>
       </c>
       <c r="B76" t="str">
-        <v>Чолпонбек Асан</v>
+        <v>Баткаев Равиль</v>
       </c>
       <c r="C76" t="str">
-        <v>в877ме77</v>
+        <v>Р415ВУ190</v>
       </c>
       <c r="D76">
         <v>4</v>
       </c>
       <c r="E76" t="str">
-        <v>г. рабочий посёлок Дрожжино, Новое шоссе, д. 11</v>
+        <v>Ярославское шоссе, д. 124</v>
       </c>
       <c r="F76" t="str">
         <v/>
       </c>
       <c r="G76" t="str">
-        <v>улица Маршала Савицкого, д. 18, к. 2</v>
+        <v>г. Мытищи, улица Семашко, д. 25</v>
       </c>
       <c r="H76" t="str">
         <v/>
       </c>
       <c r="I76" t="str">
-        <v>улица Брусилова, д. 13</v>
+        <v>г. Мытищи, Олимпийский проспект, д. вл13с1, стр. 1, к. Б</v>
       </c>
       <c r="J76" t="str">
         <v/>
       </c>
       <c r="K76" t="str">
-        <v>г. Бутово, жилой комплекс Бутово Парк, д. 28</v>
+        <v>г. Мытищи, Вокзальная площадь, д. 2</v>
       </c>
       <c r="L76" t="str">
         <v/>
@@ -3171,31 +3039,31 @@
     </row>
     <row r="77">
       <c r="A77" t="str">
-        <v>Проект А</v>
+        <v>СТРИТ ЛОГИСТИК</v>
       </c>
       <c r="B77" t="str">
-        <v>Чыйбылов Сталбек</v>
+        <v>Билялов Ринат</v>
       </c>
       <c r="C77" t="str">
-        <v>с495оа89</v>
+        <v>Х475уу152</v>
       </c>
       <c r="D77">
         <v>3</v>
       </c>
       <c r="E77" t="str">
-        <v>1-й Неопалимовский переулок, д. 16, к. 13</v>
+        <v>Правобережная улица, д. 1Б</v>
       </c>
       <c r="F77" t="str">
         <v/>
       </c>
       <c r="G77" t="str">
-        <v>улица Арбат, д. 4, стр. 1</v>
+        <v>г. Долгопрудный, Лихачёвское шоссе, д. 6</v>
       </c>
       <c r="H77" t="str">
         <v/>
       </c>
       <c r="I77" t="str">
-        <v>Газетный переулок, д. 13, стр. 1</v>
+        <v>г. Химки, Совхозная улица, д. 13</v>
       </c>
       <c r="J77" t="str">
         <v/>
@@ -3203,27 +3071,39 @@
     </row>
     <row r="78">
       <c r="A78" t="str">
-        <v>Проект А</v>
+        <v>СТРИТ ЛОГИСТИК</v>
       </c>
       <c r="B78" t="str">
-        <v>Юсупов Файзулло</v>
+        <v>Богачев Виталий</v>
       </c>
       <c r="C78" t="str">
-        <v>О401УЕ40</v>
+        <v>М046ЕТ790</v>
       </c>
       <c r="D78">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E78" t="str">
-        <v>г. поселение Внуковское, Омская улица, д. 7А</v>
+        <v>Чонгарский бульвар, д. 26А, к. 3</v>
       </c>
       <c r="F78" t="str">
         <v/>
       </c>
       <c r="G78" t="str">
-        <v>г. Внуково, Центральная улица, д. 8Б, кв. 212</v>
+        <v>Варшавское шоссе, д. 86А</v>
       </c>
       <c r="H78" t="str">
+        <v/>
+      </c>
+      <c r="I78" t="str">
+        <v>Сумской проезд, д. 8, к. 1</v>
+      </c>
+      <c r="J78" t="str">
+        <v/>
+      </c>
+      <c r="K78" t="str">
+        <v>Варшавское шоссе, д. 97</v>
+      </c>
+      <c r="L78" t="str">
         <v/>
       </c>
     </row>
@@ -3232,42 +3112,30 @@
         <v>СТРИТ ЛОГИСТИК</v>
       </c>
       <c r="B79" t="str">
-        <v>Бакланов Сергей</v>
+        <v>Галимов Динар</v>
       </c>
       <c r="C79" t="str">
-        <v>В979ЕХ979</v>
+        <v>Е099КН702</v>
       </c>
       <c r="D79">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E79" t="str">
-        <v>Каширское шоссе, д. 65, к. 3</v>
+        <v>Новопеределкинская улица, д. 13</v>
       </c>
       <c r="F79" t="str">
         <v/>
       </c>
       <c r="G79" t="str">
-        <v>Каширское шоссе (дублёр), д. 61, к. 3А</v>
+        <v>г. поселение Внуковское, улица Корнея Чуковского, д. 3</v>
       </c>
       <c r="H79" t="str">
         <v/>
       </c>
       <c r="I79" t="str">
-        <v>улица Генерала Белова, д. 43, к. 2</v>
+        <v>улица Шолохова, д. 5, к. 2</v>
       </c>
       <c r="J79" t="str">
-        <v/>
-      </c>
-      <c r="K79" t="str">
-        <v>Гурьевский проезд, д. 17, к. 1</v>
-      </c>
-      <c r="L79" t="str">
-        <v/>
-      </c>
-      <c r="M79" t="str">
-        <v>Ясеневая улица, д. 29</v>
-      </c>
-      <c r="N79" t="str">
         <v/>
       </c>
     </row>
@@ -3276,30 +3144,42 @@
         <v>СТРИТ ЛОГИСТИК</v>
       </c>
       <c r="B80" t="str">
-        <v>Баткаев Равиль</v>
+        <v>Евтюшкин Иван</v>
       </c>
       <c r="C80" t="str">
-        <v>Р415ВУ190</v>
+        <v>е135ус799</v>
       </c>
       <c r="D80">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E80" t="str">
-        <v>Семеновский пер., д. 18</v>
+        <v>Измайловский проезд, д. 13</v>
       </c>
       <c r="F80" t="str">
         <v/>
       </c>
       <c r="G80" t="str">
-        <v>Большая Почтовая улица, д. 43-45, стр. 2</v>
+        <v>Верхняя Первомайская улица, д. 59/35, к. 3</v>
       </c>
       <c r="H80" t="str">
         <v/>
       </c>
       <c r="I80" t="str">
-        <v>Сокольническая площадь, д. 9А, стр. А</v>
+        <v>Щёлковское шоссе, д. 79, к. 1</v>
       </c>
       <c r="J80" t="str">
+        <v/>
+      </c>
+      <c r="K80" t="str">
+        <v>Байкальская улица, д. 37</v>
+      </c>
+      <c r="L80" t="str">
+        <v/>
+      </c>
+      <c r="M80" t="str">
+        <v>Хабаровская улица, д. 4, к. 1</v>
+      </c>
+      <c r="N80" t="str">
         <v/>
       </c>
     </row>
@@ -3308,36 +3188,42 @@
         <v>СТРИТ ЛОГИСТИК</v>
       </c>
       <c r="B81" t="str">
-        <v>Богачев Виталий</v>
+        <v>Егоров Илья</v>
       </c>
       <c r="C81" t="str">
-        <v>М046ЕТ790</v>
+        <v>Р399АВ99</v>
       </c>
       <c r="D81">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E81" t="str">
-        <v>Кантемировская улица, д. 20, к. 1</v>
+        <v>Краснодарская улица, д. 16</v>
       </c>
       <c r="F81" t="str">
         <v/>
       </c>
       <c r="G81" t="str">
-        <v>Варшавское шоссе, д. 97</v>
+        <v>улица Артюхиной, д. 24, к. 1</v>
       </c>
       <c r="H81" t="str">
         <v/>
       </c>
       <c r="I81" t="str">
-        <v>Сумской проезд, д. 8, к. 1</v>
+        <v>Волжский бульвар, д. 38</v>
       </c>
       <c r="J81" t="str">
         <v/>
       </c>
       <c r="K81" t="str">
-        <v>Варшавское шоссе, д. вл132/2</v>
+        <v>улица Васильцовский Стан, д. 9</v>
       </c>
       <c r="L81" t="str">
+        <v/>
+      </c>
+      <c r="M81" t="str">
+        <v>улица Юных Ленинцев, д. 52</v>
+      </c>
+      <c r="N81" t="str">
         <v/>
       </c>
     </row>
@@ -3346,34 +3232,34 @@
         <v>СТРИТ ЛОГИСТИК</v>
       </c>
       <c r="B82" t="str">
-        <v>Евтюшкин Иван</v>
+        <v>Заднев Евгений</v>
       </c>
       <c r="C82" t="str">
-        <v>е135ус799</v>
+        <v>к803ее163</v>
       </c>
       <c r="D82">
         <v>4</v>
       </c>
       <c r="E82" t="str">
-        <v>Онежская улица, д. 49</v>
+        <v>улица Академика Миллионщикова, д. 19</v>
       </c>
       <c r="F82" t="str">
         <v/>
       </c>
       <c r="G82" t="str">
-        <v>Базовская улица, д. 15, к. 15</v>
+        <v>Нагатинская улица, д. 16</v>
       </c>
       <c r="H82" t="str">
         <v/>
       </c>
       <c r="I82" t="str">
-        <v>улица Лавочкина, д. 34</v>
+        <v>проспект Андропова, д. 22</v>
       </c>
       <c r="J82" t="str">
         <v/>
       </c>
       <c r="K82" t="str">
-        <v>Дмитровское шоссе, д. 107А, к. 3</v>
+        <v>улица Речников, д. 14, к. 1</v>
       </c>
       <c r="L82" t="str">
         <v/>
@@ -3384,34 +3270,34 @@
         <v>СТРИТ ЛОГИСТИК</v>
       </c>
       <c r="B83" t="str">
-        <v>Заднев Евгений</v>
+        <v>Зверев Андрей</v>
       </c>
       <c r="C83" t="str">
-        <v>к803ее163</v>
+        <v>С722ВН797</v>
       </c>
       <c r="D83">
         <v>4</v>
       </c>
       <c r="E83" t="str">
-        <v>г. Щёлково, улица Радиоцентра № 5, д. 16</v>
+        <v>Дмитровское шоссе, д. 165Д, к. 6</v>
       </c>
       <c r="F83" t="str">
         <v/>
       </c>
       <c r="G83" t="str">
-        <v>г. Щёлково, 1-й Советский переулок, д. 25</v>
+        <v>г. Долгопрудный, Московское шоссе, д. 27, к. Б</v>
       </c>
       <c r="H83" t="str">
         <v/>
       </c>
       <c r="I83" t="str">
-        <v>г. Щёлково, микрорайон Финский, д. 11, к. 1</v>
+        <v>г. Долгопрудный, Московское шоссе, д. 37, к. А</v>
       </c>
       <c r="J83" t="str">
         <v/>
       </c>
       <c r="K83" t="str">
-        <v>г. Щелково, Пушкина, д. 3</v>
+        <v>г. Долгопрудный, проспект Пацаева, д. 12</v>
       </c>
       <c r="L83" t="str">
         <v/>
@@ -3422,34 +3308,34 @@
         <v>СТРИТ ЛОГИСТИК</v>
       </c>
       <c r="B84" t="str">
-        <v>Зверев Андрей</v>
+        <v>Ивочкин Сергей</v>
       </c>
       <c r="C84" t="str">
-        <v>С722ВН797</v>
+        <v>A811AE790</v>
       </c>
       <c r="D84">
         <v>4</v>
       </c>
       <c r="E84" t="str">
-        <v>Тайнинская улица, д. 9</v>
+        <v>Дубнинская, д. 3</v>
       </c>
       <c r="F84" t="str">
         <v/>
       </c>
       <c r="G84" t="str">
-        <v>улица Коминтерна, д. 33, к. 2</v>
+        <v>Селигерская, д. 18, к. 3</v>
       </c>
       <c r="H84" t="str">
         <v/>
       </c>
       <c r="I84" t="str">
-        <v>Минусинская улица, д. 9</v>
+        <v>Дубнинская улица, д. 53, к. 3</v>
       </c>
       <c r="J84" t="str">
         <v/>
       </c>
       <c r="K84" t="str">
-        <v>улица Лётчика Бабушкина, д. 39</v>
+        <v>Дубнинская улица, д. 12Б, стр. 12</v>
       </c>
       <c r="L84" t="str">
         <v/>
@@ -3460,24 +3346,36 @@
         <v>СТРИТ ЛОГИСТИК</v>
       </c>
       <c r="B85" t="str">
-        <v>Ивочкин Сергей</v>
+        <v>Котляров Алексей</v>
       </c>
       <c r="C85" t="str">
-        <v>A811AE790</v>
+        <v>Р 043 КО 750</v>
       </c>
       <c r="D85">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E85" t="str">
-        <v>г. Старая Купавна, Октябрьская улица, д. 19</v>
+        <v>улица Лётчика Бабушкина, д. 39</v>
       </c>
       <c r="F85" t="str">
         <v/>
       </c>
       <c r="G85" t="str">
-        <v>г. Лосино-Петровский, улица Гоголя, д. 21</v>
+        <v>Минусинская улица, д. 9</v>
       </c>
       <c r="H85" t="str">
+        <v/>
+      </c>
+      <c r="I85" t="str">
+        <v>улица Коминтерна, д. 33, к. 2</v>
+      </c>
+      <c r="J85" t="str">
+        <v/>
+      </c>
+      <c r="K85" t="str">
+        <v>Тайнинская улица, д. 9</v>
+      </c>
+      <c r="L85" t="str">
         <v/>
       </c>
     </row>
@@ -3486,30 +3384,36 @@
         <v>СТРИТ ЛОГИСТИК</v>
       </c>
       <c r="B86" t="str">
-        <v>Комаров Сергей</v>
+        <v>Кузнецов Александр Васильевич</v>
       </c>
       <c r="C86" t="str">
-        <v>х582нт150</v>
+        <v>у823ех790</v>
       </c>
       <c r="D86">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E86" t="str">
-        <v>Новокузнецкая улица, д. 13, стр. 1</v>
+        <v>г. Лыткарино, Советская, д. 8, к. 2</v>
       </c>
       <c r="F86" t="str">
         <v/>
       </c>
       <c r="G86" t="str">
-        <v>улица Большая Ордынка, д. 44, стр. 2</v>
+        <v>г. Жуковский, Молодёжная улица, д. 21, к. А</v>
       </c>
       <c r="H86" t="str">
         <v/>
       </c>
       <c r="I86" t="str">
-        <v>Мытная улица, д. 48</v>
+        <v>г. Жуковский, улица Гагарина, д. 24</v>
       </c>
       <c r="J86" t="str">
+        <v/>
+      </c>
+      <c r="K86" t="str">
+        <v>г. Жуковский, улица Баженова, д. 4/1</v>
+      </c>
+      <c r="L86" t="str">
         <v/>
       </c>
     </row>
@@ -3518,30 +3422,42 @@
         <v>СТРИТ ЛОГИСТИК</v>
       </c>
       <c r="B87" t="str">
-        <v>Кузнецов Александр Васильевич</v>
+        <v>Кузнецов Алексей Др</v>
       </c>
       <c r="C87" t="str">
-        <v>у823ех790</v>
+        <v>Н081НМ777</v>
       </c>
       <c r="D87">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E87" t="str">
-        <v>г. Бронницы, Советская улица, д. 73</v>
+        <v>Покровская улица, д. 17, к. 3</v>
       </c>
       <c r="F87" t="str">
         <v/>
       </c>
       <c r="G87" t="str">
-        <v>г. Жуковский, Молодёжная улица, д. 21, к. А</v>
+        <v>Рождественская улица, д. 4</v>
       </c>
       <c r="H87" t="str">
         <v/>
       </c>
       <c r="I87" t="str">
-        <v>г. Жуковский, улица Баженова, д. 4/1</v>
+        <v>г. Люберцы, улица Попова, д. 34/1</v>
       </c>
       <c r="J87" t="str">
+        <v/>
+      </c>
+      <c r="K87" t="str">
+        <v>г. Люберцы, улица Шевлякова, д. 2/24</v>
+      </c>
+      <c r="L87" t="str">
+        <v/>
+      </c>
+      <c r="M87" t="str">
+        <v>Святоозёрская улица, д. 14</v>
+      </c>
+      <c r="N87" t="str">
         <v/>
       </c>
     </row>
@@ -3550,28 +3466,28 @@
         <v>СТРИТ ЛОГИСТИК</v>
       </c>
       <c r="B88" t="str">
-        <v>Кузнецов Алексей Др</v>
+        <v>Лапшинов Павел</v>
       </c>
       <c r="C88" t="str">
-        <v>Н081НМ777</v>
+        <v>С364ак177</v>
       </c>
       <c r="D88">
         <v>3</v>
       </c>
       <c r="E88" t="str">
-        <v>г. посёлок Коммунарка, улица Липовый Парк, д. 2</v>
+        <v>Ленинградский проспект, д. 5, стр. 7</v>
       </c>
       <c r="F88" t="str">
         <v/>
       </c>
       <c r="G88" t="str">
-        <v>г. посёлок Коммунарка, Бачуринская улица, д. 11А, к. 2</v>
+        <v>улица Полины Осипенко, д. 8</v>
       </c>
       <c r="H88" t="str">
         <v/>
       </c>
       <c r="I88" t="str">
-        <v>г. Коммунарка, -, д. 7А</v>
+        <v>Долгоруковская улица, д. 40, кв. 10</v>
       </c>
       <c r="J88" t="str">
         <v/>
@@ -3582,42 +3498,24 @@
         <v>СТРИТ ЛОГИСТИК</v>
       </c>
       <c r="B89" t="str">
-        <v>Летецкий Леонид</v>
+        <v>Лось Владимир</v>
       </c>
       <c r="C89" t="str">
-        <v>в729вр150</v>
+        <v>М316НС193</v>
       </c>
       <c r="D89">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E89" t="str">
-        <v>г. Московский, улица Хабарова, д. 2</v>
+        <v>Волоколамское шоссе, д. 15/22, кв. 1</v>
       </c>
       <c r="F89" t="str">
         <v/>
       </c>
       <c r="G89" t="str">
-        <v>г. поселение Внуковское, улица Корнея Чуковского, д. 3</v>
+        <v>улица Маршала Бирюзова, д. 4, к. 1</v>
       </c>
       <c r="H89" t="str">
-        <v/>
-      </c>
-      <c r="I89" t="str">
-        <v>улица Лётчика Грицевца, д. 12</v>
-      </c>
-      <c r="J89" t="str">
-        <v/>
-      </c>
-      <c r="K89" t="str">
-        <v>улица Шолохова, д. 5, к. 2</v>
-      </c>
-      <c r="L89" t="str">
-        <v/>
-      </c>
-      <c r="M89" t="str">
-        <v>Новопеределкинская улица, д. 13</v>
-      </c>
-      <c r="N89" t="str">
         <v/>
       </c>
     </row>
@@ -3626,40 +3524,40 @@
         <v>СТРИТ ЛОГИСТИК</v>
       </c>
       <c r="B90" t="str">
-        <v>Лось Владимир</v>
+        <v>Макухин Антон</v>
       </c>
       <c r="C90" t="str">
-        <v>М316НС193</v>
+        <v>Х871УС197</v>
       </c>
       <c r="D90">
         <v>5</v>
       </c>
       <c r="E90" t="str">
-        <v>Городецкая улица, д. 13, стр. 1, к. 19</v>
+        <v>г. Люберцы, 1-й Панковский проезд, д. 27</v>
       </c>
       <c r="F90" t="str">
         <v/>
       </c>
       <c r="G90" t="str">
-        <v>г. Реутов, улица имени Академика В.Н. Челомея, д. 12</v>
+        <v>г. Люберцы, улица Камова, д. 11/5</v>
       </c>
       <c r="H90" t="str">
         <v/>
       </c>
       <c r="I90" t="str">
-        <v>г. Реутов, Юбилейный проспект, д. 72</v>
+        <v>г. Люберцы, проспект Гагарина, д. 28/1</v>
       </c>
       <c r="J90" t="str">
         <v/>
       </c>
       <c r="K90" t="str">
-        <v>г. Реутов, улица Октября, д. 28</v>
+        <v>г. Люберцы, Проспек Победы, д. 6, кв. 019</v>
       </c>
       <c r="L90" t="str">
         <v/>
       </c>
       <c r="M90" t="str">
-        <v>г. Реутов, улица Октября, д. вл10</v>
+        <v>г. Люберцы, Смирновская улица, д. 21, к. 2</v>
       </c>
       <c r="N90" t="str">
         <v/>
@@ -3670,42 +3568,30 @@
         <v>СТРИТ ЛОГИСТИК</v>
       </c>
       <c r="B91" t="str">
-        <v>Макухин Антон</v>
+        <v>Малянов Евгений</v>
       </c>
       <c r="C91" t="str">
-        <v>Х871УС197</v>
+        <v>Р583КУ177</v>
       </c>
       <c r="D91">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E91" t="str">
-        <v>Волгоградский проспект, д. 177</v>
+        <v>улица Лавочкина, д. 34</v>
       </c>
       <c r="F91" t="str">
         <v/>
       </c>
       <c r="G91" t="str">
-        <v>улица Михайлова, д. 31А</v>
+        <v>Авангардная улица, д. 3</v>
       </c>
       <c r="H91" t="str">
         <v/>
       </c>
       <c r="I91" t="str">
-        <v>Рязанский проспект, д. 30, к. 2</v>
+        <v>Самеда Вургуна, д. 11</v>
       </c>
       <c r="J91" t="str">
-        <v/>
-      </c>
-      <c r="K91" t="str">
-        <v>Сормовская улица, д. 6</v>
-      </c>
-      <c r="L91" t="str">
-        <v/>
-      </c>
-      <c r="M91" t="str">
-        <v>Рязанский проспект, д. 48</v>
-      </c>
-      <c r="N91" t="str">
         <v/>
       </c>
     </row>
@@ -3714,34 +3600,34 @@
         <v>СТРИТ ЛОГИСТИК</v>
       </c>
       <c r="B92" t="str">
-        <v>Малянов Евгений</v>
+        <v>Метлихин Игорь</v>
       </c>
       <c r="C92" t="str">
-        <v>Р583КУ177</v>
+        <v>М609КТ790</v>
       </c>
       <c r="D92">
         <v>4</v>
       </c>
       <c r="E92" t="str">
-        <v>Дмитровское шоссе, д. 163А, к. 2</v>
+        <v>проспект Мира, д. 124, к. 2</v>
       </c>
       <c r="F92" t="str">
         <v/>
       </c>
       <c r="G92" t="str">
-        <v>Дмитровское шоссе, д. 165Д, к. 6</v>
+        <v>улица Академика Королёва, д. 13, стр. 1</v>
       </c>
       <c r="H92" t="str">
         <v/>
       </c>
       <c r="I92" t="str">
-        <v>г. Долгопрудный, Московское шоссе, д. 27, к. Б</v>
+        <v>Огородный проезд, д. 10</v>
       </c>
       <c r="J92" t="str">
         <v/>
       </c>
       <c r="K92" t="str">
-        <v>бульвар Академика Ландау, д. 3</v>
+        <v>Шереметьевская улица, д. 20</v>
       </c>
       <c r="L92" t="str">
         <v/>
@@ -3752,42 +3638,36 @@
         <v>СТРИТ ЛОГИСТИК</v>
       </c>
       <c r="B93" t="str">
-        <v>Метлихин Игорь</v>
+        <v>Мифтахутдинов Айрат</v>
       </c>
       <c r="C93" t="str">
-        <v>М609КТ790</v>
+        <v>р987ав777</v>
       </c>
       <c r="D93">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E93" t="str">
-        <v>г. Химки, Совхозная улица, д. 13</v>
+        <v>улица Тёплый Стан, д. 10</v>
       </c>
       <c r="F93" t="str">
         <v/>
       </c>
       <c r="G93" t="str">
-        <v>Дегунинская улица, д. 10, стр. 2</v>
+        <v>улица Тёплый Стан, д. 1А</v>
       </c>
       <c r="H93" t="str">
         <v/>
       </c>
       <c r="I93" t="str">
-        <v>Ангарская улица, д. 57, к. 1</v>
+        <v>Профсоюзная улица, д. 103А</v>
       </c>
       <c r="J93" t="str">
         <v/>
       </c>
       <c r="K93" t="str">
-        <v>Лобненская улица, д. 4А</v>
+        <v>Ясногорская улица, д. 7А</v>
       </c>
       <c r="L93" t="str">
-        <v/>
-      </c>
-      <c r="M93" t="str">
-        <v>Дубнинская, д. 32, к. 6</v>
-      </c>
-      <c r="N93" t="str">
         <v/>
       </c>
     </row>
@@ -3796,28 +3676,28 @@
         <v>СТРИТ ЛОГИСТИК</v>
       </c>
       <c r="B94" t="str">
-        <v>Мифтахутдинов Айрат</v>
+        <v>Мусаев Бахлул</v>
       </c>
       <c r="C94" t="str">
-        <v>р987ав777</v>
+        <v>В207Во797</v>
       </c>
       <c r="D94">
         <v>3</v>
       </c>
       <c r="E94" t="str">
-        <v>Шереметьевская улица, д. 20</v>
+        <v>г. Раменское, Крымская улица, д. 12, стр. офис 17</v>
       </c>
       <c r="F94" t="str">
         <v/>
       </c>
       <c r="G94" t="str">
-        <v>Огородный проезд, д. 10</v>
+        <v>г. Раменское, улица Михалевича, д. 5</v>
       </c>
       <c r="H94" t="str">
         <v/>
       </c>
       <c r="I94" t="str">
-        <v>проспект Мира, д. 81</v>
+        <v>г. Раменское, улица Чугунова, д. 32А</v>
       </c>
       <c r="J94" t="str">
         <v/>
@@ -3828,30 +3708,36 @@
         <v>СТРИТ ЛОГИСТИК</v>
       </c>
       <c r="B95" t="str">
-        <v>Неменущий Илья</v>
+        <v>Нариманов Тамирлан</v>
       </c>
       <c r="C95" t="str">
-        <v>м631ео82</v>
+        <v>с469ок777</v>
       </c>
       <c r="D95">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E95" t="str">
-        <v>г. Балашиха, Речная, д. 5</v>
+        <v>г. Пушкино, Московский проспект, д. 59</v>
       </c>
       <c r="F95" t="str">
         <v/>
       </c>
       <c r="G95" t="str">
-        <v>г. микрорайон Железнодорожный, Балашиха, Андрея Белого, д. 1</v>
+        <v>г. Пушкино, микрорайон Серебрянка, д. 48, к. 2</v>
       </c>
       <c r="H95" t="str">
         <v/>
       </c>
       <c r="I95" t="str">
-        <v>г. Балашиха, улица Ленина, д. 1/5, к. 5</v>
+        <v>г. Пушкино, Набережная улица, д. 35, к. 6</v>
       </c>
       <c r="J95" t="str">
+        <v/>
+      </c>
+      <c r="K95" t="str">
+        <v>г. Мытищи, 2-я Институтская улица, д. 26</v>
+      </c>
+      <c r="L95" t="str">
         <v/>
       </c>
     </row>
@@ -3860,34 +3746,34 @@
         <v>СТРИТ ЛОГИСТИК</v>
       </c>
       <c r="B96" t="str">
-        <v>Нестеров Леонид</v>
+        <v>Неменущий Илья</v>
       </c>
       <c r="C96" t="str">
-        <v>н698мн777</v>
+        <v>м631ео82</v>
       </c>
       <c r="D96">
         <v>4</v>
       </c>
       <c r="E96" t="str">
-        <v>Мичуринский проспект, д. 21, к. 1</v>
+        <v>Большая Марфинская улица, д. 4, к. 1</v>
       </c>
       <c r="F96" t="str">
         <v/>
       </c>
       <c r="G96" t="str">
-        <v>Мосфильмовская улица, д. 27</v>
+        <v>Алтуфьевское шоссе, д. 40Г</v>
       </c>
       <c r="H96" t="str">
         <v/>
       </c>
       <c r="I96" t="str">
-        <v>улица Хамовнический Вал, д. 24</v>
+        <v>Алтуфьевское шоссе, д. 48, к. 2</v>
       </c>
       <c r="J96" t="str">
         <v/>
       </c>
       <c r="K96" t="str">
-        <v>3-й Сетуньский проезд, д. 16</v>
+        <v>Плещеева, д. 8</v>
       </c>
       <c r="L96" t="str">
         <v/>
@@ -3904,36 +3790,30 @@
         <v>Е564ка164</v>
       </c>
       <c r="D97">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E97" t="str">
-        <v>Люблинская улица, д. 102А</v>
+        <v>г. Бутово, жилой комплекс Бутово Парк, д. 28</v>
       </c>
       <c r="F97" t="str">
         <v/>
       </c>
       <c r="G97" t="str">
-        <v>Братиславская улица, д. 16, к. 1</v>
+        <v>г. Щербинка, Индустриальная, д. 9</v>
       </c>
       <c r="H97" t="str">
         <v/>
       </c>
       <c r="I97" t="str">
-        <v>улица Перерва, д. 45</v>
+        <v>улица Брусилова, д. 13</v>
       </c>
       <c r="J97" t="str">
         <v/>
       </c>
       <c r="K97" t="str">
-        <v>Донецкая улица, д. 34, к. 1</v>
+        <v>г. рабочий посёлок Дрожжино, Новое шоссе, д. 11</v>
       </c>
       <c r="L97" t="str">
-        <v/>
-      </c>
-      <c r="M97" t="str">
-        <v>улица Перерва, д. 32</v>
-      </c>
-      <c r="N97" t="str">
         <v/>
       </c>
     </row>
@@ -3951,25 +3831,25 @@
         <v>4</v>
       </c>
       <c r="E98" t="str">
-        <v>Открытое шоссе, д. 24, к. 11</v>
+        <v>Лобненская улица, д. 4А</v>
       </c>
       <c r="F98" t="str">
         <v/>
       </c>
       <c r="G98" t="str">
-        <v>Амурская улица, д. 19</v>
+        <v>Ангарская улица, д. 57, к. 1</v>
       </c>
       <c r="H98" t="str">
         <v/>
       </c>
       <c r="I98" t="str">
-        <v>Байкальская улица, д. 37</v>
+        <v>Коровинское шоссе, д. 19, к. 1</v>
       </c>
       <c r="J98" t="str">
         <v/>
       </c>
       <c r="K98" t="str">
-        <v>Щёлковское шоссе, д. 79, к. 1</v>
+        <v>Дегунинская улица, д. 10, стр. 2</v>
       </c>
       <c r="L98" t="str">
         <v/>
@@ -3989,19 +3869,19 @@
         <v>3</v>
       </c>
       <c r="E99" t="str">
-        <v>г. Подольск, улица Чистова, д. 3</v>
+        <v>Алтуфьевское шоссе, д. 27</v>
       </c>
       <c r="F99" t="str">
         <v/>
       </c>
       <c r="G99" t="str">
-        <v>г. Подольск, улица 50 лет ВЛКСМ, д. 18, к. А, кв. 13</v>
+        <v>Олонецкая улица, д. 4</v>
       </c>
       <c r="H99" t="str">
         <v/>
       </c>
       <c r="I99" t="str">
-        <v>г. Подольск, Февральская улица, д. 54/150</v>
+        <v>Лазоревый проезд, д. 1А, к. 1</v>
       </c>
       <c r="J99" t="str">
         <v/>
@@ -4012,36 +3892,42 @@
         <v>СТРИТ ЛОГИСТИК</v>
       </c>
       <c r="B100" t="str">
-        <v>Саруханян Армен</v>
+        <v>Рыбин Алексей</v>
       </c>
       <c r="C100" t="str">
-        <v>к350ом750</v>
+        <v>к973ом777</v>
       </c>
       <c r="D100">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E100" t="str">
-        <v>г. Одинцово, Белорусская улица, д. 5</v>
+        <v>г. Зеленоград, улица Болдов Ручей, д. 1</v>
       </c>
       <c r="F100" t="str">
         <v/>
       </c>
       <c r="G100" t="str">
-        <v>г. Лесной Городок, Фасадная, д. 2, к. 1</v>
+        <v>г. Зеленоград, -, д. 403А, стр. 9</v>
       </c>
       <c r="H100" t="str">
         <v/>
       </c>
       <c r="I100" t="str">
-        <v>г. Одинцово, Союзная улица, д. 1, к. В</v>
+        <v>г. Зеленоград, Центральный проспект, д. -, к. 438</v>
       </c>
       <c r="J100" t="str">
         <v/>
       </c>
       <c r="K100" t="str">
-        <v>г. Одинцово, улица Чикина, д. 8А, к. А</v>
+        <v>г. Химки, Тепличный проезд, д. 8</v>
       </c>
       <c r="L100" t="str">
+        <v/>
+      </c>
+      <c r="M100" t="str">
+        <v>г. Химки, Октябрьская улица, д. 1А</v>
+      </c>
+      <c r="N100" t="str">
         <v/>
       </c>
     </row>
@@ -4050,40 +3936,40 @@
         <v>СТРИТ ЛОГИСТИК</v>
       </c>
       <c r="B101" t="str">
-        <v>Смирнягин Алексей</v>
+        <v>Стукалин Дмитрий</v>
       </c>
       <c r="C101" t="str">
-        <v>Т997км777</v>
+        <v>у155не790</v>
       </c>
       <c r="D101">
         <v>5</v>
       </c>
       <c r="E101" t="str">
-        <v>Братиславская, д. 33</v>
+        <v>Булатниковская улица, д. 2А</v>
       </c>
       <c r="F101" t="str">
         <v/>
       </c>
       <c r="G101" t="str">
-        <v>улица Борисовские Пруды, д. 14, к. 3</v>
+        <v>Булатниковский проезд, д. 2В, к. 4</v>
       </c>
       <c r="H101" t="str">
         <v/>
       </c>
       <c r="I101" t="str">
-        <v>Паромная улица, д. 9, к. 1</v>
+        <v>Россошанский проезд, д. 3</v>
       </c>
       <c r="J101" t="str">
         <v/>
       </c>
       <c r="K101" t="str">
-        <v>Братеевская улица, д. 16, к. 6</v>
+        <v>Бирюлёвская улица, д. 43</v>
       </c>
       <c r="L101" t="str">
         <v/>
       </c>
       <c r="M101" t="str">
-        <v>улица Мусы Джалиля, д. 27, стр. 2, к. 2</v>
+        <v>Михневская улица, д. 4</v>
       </c>
       <c r="N101" t="str">
         <v/>
@@ -4094,22 +3980,22 @@
         <v>СТРИТ ЛОГИСТИК</v>
       </c>
       <c r="B102" t="str">
-        <v>Стукалин Дмитрий</v>
+        <v>Сулайманов Кубат</v>
       </c>
       <c r="C102" t="str">
-        <v>у155не790</v>
+        <v>Е641ХМ199</v>
       </c>
       <c r="D102">
         <v>2</v>
       </c>
       <c r="E102" t="str">
-        <v>улица Удальцова, д. 42</v>
+        <v>г. Одинцово, Союзная улица, д. 1, к. В</v>
       </c>
       <c r="F102" t="str">
         <v/>
       </c>
       <c r="G102" t="str">
-        <v>улица Мичуринский Проспект, Олимпийская Деревня, д. 4, к. 2</v>
+        <v>г. Одинцово, улица Чикина, д. 8А, к. А</v>
       </c>
       <c r="H102" t="str">
         <v/>
@@ -4120,34 +4006,34 @@
         <v>СТРИТ ЛОГИСТИК</v>
       </c>
       <c r="B103" t="str">
-        <v>Сулайманов Кубат</v>
+        <v>Третьяков Сергей</v>
       </c>
       <c r="C103" t="str">
-        <v>Е641ХМ199</v>
+        <v>Н915АЕ790</v>
       </c>
       <c r="D103">
         <v>4</v>
       </c>
       <c r="E103" t="str">
-        <v>Покровская улица, д. 17, к. 3</v>
+        <v>г. Мытищи, Коммунистическая улица, д. 1</v>
       </c>
       <c r="F103" t="str">
         <v/>
       </c>
       <c r="G103" t="str">
-        <v>г. Люберцы, улица Камова, д. 11/5</v>
+        <v>г. Королёв, Пионерская улица, д. 12</v>
       </c>
       <c r="H103" t="str">
         <v/>
       </c>
       <c r="I103" t="str">
-        <v>Рождественская улица, д. 4</v>
+        <v>г. Королёв, улица Карла Маркса, д. 1А</v>
       </c>
       <c r="J103" t="str">
         <v/>
       </c>
       <c r="K103" t="str">
-        <v>Рождественская, д. 18</v>
+        <v>г. Королёв, Пионерская улица, д. 15, к. 2</v>
       </c>
       <c r="L103" t="str">
         <v/>
@@ -4158,30 +4044,36 @@
         <v>СТРИТ ЛОГИСТИК</v>
       </c>
       <c r="B104" t="str">
-        <v>Третьяков Сергей</v>
+        <v>Федарков Сергей</v>
       </c>
       <c r="C104" t="str">
-        <v>Н915АЕ790</v>
+        <v>х460тх197</v>
       </c>
       <c r="D104">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E104" t="str">
-        <v>Профсоюзная улица, д. 102А</v>
+        <v>г. Балашиха, улица Евстафьева, д. 1/9</v>
       </c>
       <c r="F104" t="str">
         <v/>
       </c>
       <c r="G104" t="str">
-        <v>Профсоюзная улица, д. 103А</v>
+        <v>г. Балашиха, проспект Ленина, д. 74</v>
       </c>
       <c r="H104" t="str">
         <v/>
       </c>
       <c r="I104" t="str">
-        <v>Ясногорская улица, д. 7А</v>
+        <v>г. Балашиха, улица Твардовского, д. 44</v>
       </c>
       <c r="J104" t="str">
+        <v/>
+      </c>
+      <c r="K104" t="str">
+        <v>г. Балашиха, Живописная улица, д. 1</v>
+      </c>
+      <c r="L104" t="str">
         <v/>
       </c>
     </row>
@@ -4196,24 +4088,18 @@
         <v>У093оу77</v>
       </c>
       <c r="D105">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E105" t="str">
-        <v>Алтуфьевское шоссе, д. 40Г</v>
+        <v>г. Одинцово, Кутузовская улица, д. 72Б</v>
       </c>
       <c r="F105" t="str">
         <v/>
       </c>
       <c r="G105" t="str">
-        <v>Алтуфьевское шоссе, д. 27</v>
+        <v>г. Одинцово, улица Чистяковой, д. 67</v>
       </c>
       <c r="H105" t="str">
-        <v/>
-      </c>
-      <c r="I105" t="str">
-        <v>Алтуфьевское шоссе, д. 48, к. 2</v>
-      </c>
-      <c r="J105" t="str">
         <v/>
       </c>
     </row>
@@ -4228,42 +4114,24 @@
         <v>н268вт797</v>
       </c>
       <c r="D106">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E106" t="str">
-        <v>Новотушинский проезд, д. 6, к. 1</v>
+        <v>г. Красногорск, улица Ленина, д. 26А</v>
       </c>
       <c r="F106" t="str">
         <v/>
       </c>
       <c r="G106" t="str">
-        <v>Пятницкое шоссе, д. 15, к. 1</v>
+        <v>г. Красногорск, бульвар Космонавтов, д. 17</v>
       </c>
       <c r="H106" t="str">
         <v/>
       </c>
       <c r="I106" t="str">
-        <v>Митинская улица, д. 55</v>
+        <v>г. Красногорск, Светлая улица, д. 3А, стр. 4</v>
       </c>
       <c r="J106" t="str">
-        <v/>
-      </c>
-      <c r="K106" t="str">
-        <v>Митинская улица, д. 27</v>
-      </c>
-      <c r="L106" t="str">
-        <v/>
-      </c>
-      <c r="M106" t="str">
-        <v>улица Генерала Белобородова, д. 20, к. 1</v>
-      </c>
-      <c r="N106" t="str">
-        <v/>
-      </c>
-      <c r="O106" t="str">
-        <v>улица Генерала Белобородова, д. 37</v>
-      </c>
-      <c r="P106" t="str">
         <v/>
       </c>
     </row>
@@ -4281,19 +4149,19 @@
         <v>3</v>
       </c>
       <c r="E107" t="str">
-        <v>г. Подольск, Мраморная улица, д. 4</v>
+        <v>улица Лётчика Грицевца, д. 12</v>
       </c>
       <c r="F107" t="str">
         <v/>
       </c>
       <c r="G107" t="str">
-        <v>г. Подольск, Ленина, д. 14</v>
+        <v>г. поселение Внуковское, Омская улица, д. 7А</v>
       </c>
       <c r="H107" t="str">
         <v/>
       </c>
       <c r="I107" t="str">
-        <v>г. Подольск, Быковская улица, д. 10</v>
+        <v>г. Внуково, Центральная улица, д. 8Б, кв. 212</v>
       </c>
       <c r="J107" t="str">
         <v/>
@@ -4304,30 +4172,36 @@
         <v>СТРИТ ЛОГИСТИК</v>
       </c>
       <c r="B108" t="str">
-        <v>Хлебников Олег</v>
+        <v>Хохряев Сергей</v>
       </c>
       <c r="C108" t="str">
-        <v>н210нс68</v>
+        <v>р220оа77</v>
       </c>
       <c r="D108">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E108" t="str">
-        <v>г. Королёв, проспект Космонавтов, д. 34Б, к. Б</v>
+        <v>Варшавское шоссе, д. 141А, к. 2, кв. пом. 5</v>
       </c>
       <c r="F108" t="str">
         <v/>
       </c>
       <c r="G108" t="str">
-        <v>г. Королёв, Бурковский проезд, д. 48, к. 2</v>
+        <v>улица Поляны, д. 5</v>
       </c>
       <c r="H108" t="str">
         <v/>
       </c>
       <c r="I108" t="str">
-        <v>г. Королёв, Станционная площадь, д. 4</v>
+        <v>улица Знаменские Садки, д. 1, к. 1</v>
       </c>
       <c r="J108" t="str">
+        <v/>
+      </c>
+      <c r="K108" t="str">
+        <v>Старокачаловская, д. 1, к. 2</v>
+      </c>
+      <c r="L108" t="str">
         <v/>
       </c>
     </row>
@@ -4336,34 +4210,34 @@
         <v>СТРИТ ЛОГИСТИК</v>
       </c>
       <c r="B109" t="str">
-        <v>Хохряев Сергей</v>
+        <v>Чёрный Алексей</v>
       </c>
       <c r="C109" t="str">
-        <v>р220оа77</v>
+        <v>А780КС797</v>
       </c>
       <c r="D109">
         <v>4</v>
       </c>
       <c r="E109" t="str">
-        <v>г. Балашиха, проспект Ленина, д. 74</v>
+        <v>г. Мытищи, улица Комарова, д. 2, к. 2</v>
       </c>
       <c r="F109" t="str">
         <v/>
       </c>
       <c r="G109" t="str">
-        <v>г. Балашиха, Живописная улица, д. 1</v>
+        <v>г. Мытищи, Олимпийский проспект, д. 36, к. 3</v>
       </c>
       <c r="H109" t="str">
         <v/>
       </c>
       <c r="I109" t="str">
-        <v>г. Балашиха, улица Некрасова, д. 13А, к. А</v>
+        <v>г. Мытищи, проспект Астрахова, д. 6</v>
       </c>
       <c r="J109" t="str">
         <v/>
       </c>
       <c r="K109" t="str">
-        <v>г. Балашиха, улица Свердлова, д. 1А, кв. 151</v>
+        <v>г. Мытищи, 1-й Щёлковский проезд, д. 7</v>
       </c>
       <c r="L109" t="str">
         <v/>
@@ -4374,80 +4248,36 @@
         <v>СТРИТ ЛОГИСТИК</v>
       </c>
       <c r="B110" t="str">
-        <v>Чёрный Алексей</v>
+        <v>Шорохов Василий</v>
       </c>
       <c r="C110" t="str">
-        <v>А780КС797</v>
+        <v xml:space="preserve"> Н118ХР123</v>
       </c>
       <c r="D110">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E110" t="str">
-        <v>г. Одинцово, улица Чистяковой, д. 67</v>
+        <v>г. рабочий посёлок Октябрьский, улица Ленина, д. 25</v>
       </c>
       <c r="F110" t="str">
         <v/>
       </c>
       <c r="G110" t="str">
-        <v>Ярцевская улица, д. 19</v>
+        <v>г. Бронницы, Советская улица, д. 73</v>
       </c>
       <c r="H110" t="str">
         <v/>
       </c>
       <c r="I110" t="str">
-        <v>Дорогобужская улица, д. 3</v>
+        <v>г. рабочий посёлок Октябрьский, микрорайон Восточный, д. 1</v>
       </c>
       <c r="J110" t="str">
-        <v/>
-      </c>
-      <c r="K110" t="str">
-        <v>г. Одинцово, Кутузовская улица, д. 72Б</v>
-      </c>
-      <c r="L110" t="str">
-        <v/>
-      </c>
-      <c r="M110" t="str">
-        <v>Кастанаевская улица, д. 45, к. 2</v>
-      </c>
-      <c r="N110" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="111">
-      <c r="A111" t="str">
-        <v>СТРИТ ЛОГИСТИК</v>
-      </c>
-      <c r="B111" t="str">
-        <v>Шорохов Василий</v>
-      </c>
-      <c r="C111" t="str">
-        <v xml:space="preserve"> Н118ХР123</v>
-      </c>
-      <c r="D111">
-        <v>3</v>
-      </c>
-      <c r="E111" t="str">
-        <v>Ленинский проспект, д. 44</v>
-      </c>
-      <c r="F111" t="str">
-        <v/>
-      </c>
-      <c r="G111" t="str">
-        <v>улица Вавилова, д. 66</v>
-      </c>
-      <c r="H111" t="str">
-        <v/>
-      </c>
-      <c r="I111" t="str">
-        <v>Нахимовский проспект, д. 63, к. 2</v>
-      </c>
-      <c r="J111" t="str">
         <v/>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:U111"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:U110"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated gitignore, fixed syntax bug
</commit_message>
<xml_diff>
--- a/EzForm.xlsx
+++ b/EzForm.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:U110"/>
+  <dimension ref="A1:U106"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -456,12 +456,30 @@
         <v>У223РЕ197</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E2" t="str">
-        <v>г. Дедовск, 1-ая Главная, д. 1</v>
+        <v>г. Королёв, Пионерская улица, д. 12</v>
       </c>
       <c r="F2" t="str">
+        <v/>
+      </c>
+      <c r="G2" t="str">
+        <v>г. Королёв, Бурковский проезд, д. 48, к. 2</v>
+      </c>
+      <c r="H2" t="str">
+        <v/>
+      </c>
+      <c r="I2" t="str">
+        <v>г. Королёв, улица Карла Маркса, д. 1А</v>
+      </c>
+      <c r="J2" t="str">
+        <v/>
+      </c>
+      <c r="K2" t="str">
+        <v>г. Королёв, Пионерская улица, д. 15, к. 2</v>
+      </c>
+      <c r="L2" t="str">
         <v/>
       </c>
     </row>
@@ -470,36 +488,30 @@
         <v>Атлант Груп</v>
       </c>
       <c r="B3" t="str">
-        <v>Борис Артём</v>
+        <v>Володин Евгений</v>
       </c>
       <c r="C3" t="str">
-        <v>У452СН199</v>
+        <v>О583АТ32</v>
       </c>
       <c r="D3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E3" t="str">
-        <v>Нижегородская улица, д. 71</v>
+        <v>улица Габричевского, д. 10, к. 1</v>
       </c>
       <c r="F3" t="str">
         <v/>
       </c>
       <c r="G3" t="str">
-        <v>Перовское шоссе, д. 16/2</v>
+        <v>улица Маршала Новикова, д. 2, к. 2</v>
       </c>
       <c r="H3" t="str">
         <v/>
       </c>
       <c r="I3" t="str">
-        <v>Красноказарменная улица, д. 14А, к. 2</v>
+        <v>улица Маршала Рыбалко, д. 2, к. 6, кв. 106</v>
       </c>
       <c r="J3" t="str">
-        <v/>
-      </c>
-      <c r="K3" t="str">
-        <v>шоссе Энтузиастов, д. 10/2</v>
-      </c>
-      <c r="L3" t="str">
         <v/>
       </c>
     </row>
@@ -508,28 +520,28 @@
         <v>Атлант Груп</v>
       </c>
       <c r="B4" t="str">
-        <v>Востриков Максим</v>
+        <v>Гасанов Сайгид</v>
       </c>
       <c r="C4" t="str">
-        <v>К387УВ77</v>
+        <v>Р130ОВ05</v>
       </c>
       <c r="D4">
         <v>3</v>
       </c>
       <c r="E4" t="str">
-        <v>г. Подольск, Бородинский бульвар, д. 7</v>
+        <v>Новотушинский проезд, д. 6, к. 1</v>
       </c>
       <c r="F4" t="str">
         <v/>
       </c>
       <c r="G4" t="str">
-        <v>г. Подольск, улица Чистова, д. 3</v>
+        <v>Пятницкое шоссе, д. 15, к. 1</v>
       </c>
       <c r="H4" t="str">
         <v/>
       </c>
       <c r="I4" t="str">
-        <v>г. Подольск, Мраморная улица, д. 4</v>
+        <v>Походный проезд, д. 4, к. 1</v>
       </c>
       <c r="J4" t="str">
         <v/>
@@ -540,40 +552,40 @@
         <v>Атлант Груп</v>
       </c>
       <c r="B5" t="str">
-        <v>Гасанов Сайгид</v>
+        <v>Джафаров Рассул</v>
       </c>
       <c r="C5" t="str">
-        <v>Р130ОВ05</v>
+        <v>У972РУ790</v>
       </c>
       <c r="D5">
         <v>5</v>
       </c>
       <c r="E5" t="str">
-        <v>улица Мусы Джалиля, д. 27, стр. 2, к. 2</v>
+        <v>Снайперская улица, д. 9А</v>
       </c>
       <c r="F5" t="str">
         <v/>
       </c>
       <c r="G5" t="str">
-        <v>Каширское шоссе, д. 80</v>
+        <v>улица Михайлова, д. 31А</v>
       </c>
       <c r="H5" t="str">
         <v/>
       </c>
       <c r="I5" t="str">
-        <v>улица Борисовские Пруды, д. 5, к. 1</v>
+        <v>Зарайская улица, д. 26</v>
       </c>
       <c r="J5" t="str">
         <v/>
       </c>
       <c r="K5" t="str">
-        <v>улица Борисовские Пруды, д. 8А</v>
+        <v>2-й Грайвороновский проезд, д. 44, к. 1</v>
       </c>
       <c r="L5" t="str">
         <v/>
       </c>
       <c r="M5" t="str">
-        <v>улица Борисовские Пруды, д. 14, к. 3</v>
+        <v>Сормовская улица, д. 6</v>
       </c>
       <c r="N5" t="str">
         <v/>
@@ -584,24 +596,36 @@
         <v>Атлант Груп</v>
       </c>
       <c r="B6" t="str">
-        <v>Джафаров Рассул</v>
+        <v>Павлюткин Александр</v>
       </c>
       <c r="C6" t="str">
-        <v>У972РУ790</v>
+        <v>Р701ЕА797</v>
       </c>
       <c r="D6">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E6" t="str">
-        <v>г. Дмитров, Профессиональная улица, д. 22, к. 1</v>
+        <v>Семеновский пер., д. 18</v>
       </c>
       <c r="F6" t="str">
         <v/>
       </c>
       <c r="G6" t="str">
-        <v>г. Дмитров, Советская улица, д. 5</v>
+        <v>Суворовская улица, д. 24</v>
       </c>
       <c r="H6" t="str">
+        <v/>
+      </c>
+      <c r="I6" t="str">
+        <v>2-я Прогонная, д. 10</v>
+      </c>
+      <c r="J6" t="str">
+        <v/>
+      </c>
+      <c r="K6" t="str">
+        <v>Краснобогатырская улица, д. 90, стр. 2</v>
+      </c>
+      <c r="L6" t="str">
         <v/>
       </c>
     </row>
@@ -610,28 +634,28 @@
         <v>Атлант Груп</v>
       </c>
       <c r="B7" t="str">
-        <v>Казаков Олег</v>
+        <v>Сизов Георгий</v>
       </c>
       <c r="C7" t="str">
-        <v>М392РА799</v>
+        <v>О419ВВ790</v>
       </c>
       <c r="D7">
         <v>3</v>
       </c>
       <c r="E7" t="str">
-        <v>г. Долгопрудный, Набережная улица, д. 31</v>
+        <v>Дмитровское шоссе, д. 163А, к. 2</v>
       </c>
       <c r="F7" t="str">
         <v/>
       </c>
       <c r="G7" t="str">
-        <v>г. Лобня, улица Ленина, д. 18</v>
+        <v>Дмитровское шоссе, д. 165Д, к. 6</v>
       </c>
       <c r="H7" t="str">
         <v/>
       </c>
       <c r="I7" t="str">
-        <v>г. Химки, улица Лётчика Ивана Фёдорова, д. 8, к. 1</v>
+        <v>Дмитровское шоссе, д. 169, к. 9</v>
       </c>
       <c r="J7" t="str">
         <v/>
@@ -642,36 +666,30 @@
         <v>Атлант Груп</v>
       </c>
       <c r="B8" t="str">
-        <v>Павлюткин Александр</v>
+        <v>Суханов Алексей</v>
       </c>
       <c r="C8" t="str">
-        <v>Р701ЕА797</v>
+        <v>Н072КУ797</v>
       </c>
       <c r="D8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E8" t="str">
-        <v>г. Ивантеевка, улица Новая Слобода, д. 3</v>
+        <v>Коровинское шоссе, д. 19, к. 1</v>
       </c>
       <c r="F8" t="str">
         <v/>
       </c>
       <c r="G8" t="str">
-        <v>г. Ивантеевка, улица Новосёлки, д. 4</v>
+        <v>Базовская улица, д. 15, к. 15</v>
       </c>
       <c r="H8" t="str">
         <v/>
       </c>
       <c r="I8" t="str">
-        <v>г. Ивантеевка, Школьная улица, д. 16</v>
+        <v>Дегунинская улица, д. 10, стр. 2</v>
       </c>
       <c r="J8" t="str">
-        <v/>
-      </c>
-      <c r="K8" t="str">
-        <v>г. Щёлково, микрорайон Финский, д. 11, к. 1</v>
-      </c>
-      <c r="L8" t="str">
         <v/>
       </c>
     </row>
@@ -680,24 +698,36 @@
         <v>Атлант Груп</v>
       </c>
       <c r="B9" t="str">
-        <v>Суханов Алексей</v>
+        <v>Трубников  Александр</v>
       </c>
       <c r="C9" t="str">
-        <v>Н072КУ797</v>
+        <v>Х734ХК190</v>
       </c>
       <c r="D9">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E9" t="str">
-        <v>Дубнинская улица, д. 32, к. 6</v>
+        <v>Олонецкая улица, д. 4</v>
       </c>
       <c r="F9" t="str">
         <v/>
       </c>
       <c r="G9" t="str">
-        <v>Дмитровское шоссе, д. 107А, к. 3</v>
+        <v>Алтуфьевское шоссе, д. 40Г</v>
       </c>
       <c r="H9" t="str">
+        <v/>
+      </c>
+      <c r="I9" t="str">
+        <v>Алтуфьевское шоссе, д. 48, к. 2</v>
+      </c>
+      <c r="J9" t="str">
+        <v/>
+      </c>
+      <c r="K9" t="str">
+        <v>Плещеева, д. 8</v>
+      </c>
+      <c r="L9" t="str">
         <v/>
       </c>
     </row>
@@ -706,36 +736,30 @@
         <v>Атлант Груп</v>
       </c>
       <c r="B10" t="str">
-        <v>Трубников  Александр</v>
+        <v>Шатилов Александр</v>
       </c>
       <c r="C10" t="str">
-        <v>Х734ХК190</v>
+        <v>К531КМ790</v>
       </c>
       <c r="D10">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E10" t="str">
-        <v>Заводской проезд, д. 10</v>
+        <v>г. Бронницы, Советская улица, д. 73</v>
       </c>
       <c r="F10" t="str">
         <v/>
       </c>
       <c r="G10" t="str">
-        <v>Измайловский проезд, д. 10, к. 3</v>
+        <v>г. Раменское, Десантная улица, д. 14</v>
       </c>
       <c r="H10" t="str">
         <v/>
       </c>
       <c r="I10" t="str">
-        <v>9-я Парковая улица, д. 6, к. 1</v>
+        <v>г. Раменское, Десантная улица, д. 17</v>
       </c>
       <c r="J10" t="str">
-        <v/>
-      </c>
-      <c r="K10" t="str">
-        <v>Вольная улица, д. 28/4, к. 1</v>
-      </c>
-      <c r="L10" t="str">
         <v/>
       </c>
     </row>
@@ -744,24 +768,36 @@
         <v>ЛоялАвто</v>
       </c>
       <c r="B11" t="str">
-        <v xml:space="preserve">Алыбин Николай </v>
+        <v>Абдуллаев Бакытбек</v>
       </c>
       <c r="C11" t="str">
-        <v>Х718ЕЕ50</v>
+        <v>Н018УК777</v>
       </c>
       <c r="D11">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E11" t="str">
-        <v>Походный проезд, д. 4, к. 1</v>
+        <v>г. Подольск, Бородинский бульвар, д. 7</v>
       </c>
       <c r="F11" t="str">
         <v/>
       </c>
       <c r="G11" t="str">
-        <v>г. Красногорск, улица Жуковского, д. 17</v>
+        <v>г. Подольск, улица Чистова, д. 3</v>
       </c>
       <c r="H11" t="str">
+        <v/>
+      </c>
+      <c r="I11" t="str">
+        <v>г. Подольск, улица 50 лет ВЛКСМ, д. 18, к. А, кв. 13</v>
+      </c>
+      <c r="J11" t="str">
+        <v/>
+      </c>
+      <c r="K11" t="str">
+        <v>г. Подольск, улица Генерала Варенникова, д. 4</v>
+      </c>
+      <c r="L11" t="str">
         <v/>
       </c>
     </row>
@@ -770,30 +806,24 @@
         <v>ЛоялАвто</v>
       </c>
       <c r="B12" t="str">
-        <v>Гвиздон Валерий</v>
+        <v>Исхаков Эмиль</v>
       </c>
       <c r="C12" t="str">
-        <v>Х270ОХ12</v>
+        <v>А181ВН797</v>
       </c>
       <c r="D12">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E12" t="str">
-        <v>Боровское шоссе, д. 2А, к. 1</v>
+        <v>г. Химки, Октябрьская улица, д. 1А</v>
       </c>
       <c r="F12" t="str">
         <v/>
       </c>
       <c r="G12" t="str">
-        <v>улица Авиаторов, д. 5, к. 6</v>
+        <v>г. Химки, Тепличный проезд, д. 8</v>
       </c>
       <c r="H12" t="str">
-        <v/>
-      </c>
-      <c r="I12" t="str">
-        <v>Солнцевский проспект, д. 15</v>
-      </c>
-      <c r="J12" t="str">
         <v/>
       </c>
     </row>
@@ -802,28 +832,28 @@
         <v>ЛоялАвто</v>
       </c>
       <c r="B13" t="str">
-        <v>Жусупбаев Дилмурат</v>
+        <v>Ковалев  Андрей</v>
       </c>
       <c r="C13" t="str">
-        <v>Т672НВ790</v>
+        <v>М527ЕК777</v>
       </c>
       <c r="D13">
         <v>3</v>
       </c>
       <c r="E13" t="str">
-        <v>Соколово-Мещерская улица, д. 25</v>
+        <v>Кастанаевская улица, д. 45, к. 2</v>
       </c>
       <c r="F13" t="str">
         <v/>
       </c>
       <c r="G13" t="str">
-        <v>г. Химки, Молодёжная улица, д. 52</v>
+        <v>Мосфильмовская улица, д. 27</v>
       </c>
       <c r="H13" t="str">
         <v/>
       </c>
       <c r="I13" t="str">
-        <v>г. Химки, Молодёжная улица, д. 15Б, к. Б</v>
+        <v>3-й Сетуньский проезд, д. 16</v>
       </c>
       <c r="J13" t="str">
         <v/>
@@ -834,42 +864,36 @@
         <v>ЛоялАвто</v>
       </c>
       <c r="B14" t="str">
-        <v>Исаев Сергей</v>
+        <v>Мурзаев Талант</v>
       </c>
       <c r="C14" t="str">
-        <v>С703КР12</v>
+        <v>М980АМ62</v>
       </c>
       <c r="D14">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E14" t="str">
-        <v>Суздальская улица, д. 12А</v>
+        <v>Булатниковский проезд, д. 2В, к. 4</v>
       </c>
       <c r="F14" t="str">
         <v/>
       </c>
       <c r="G14" t="str">
-        <v>г. Реутов, улица имени Академика В.Н. Челомея, д. 12</v>
+        <v>Варшавское шоссе, д. вл132/2</v>
       </c>
       <c r="H14" t="str">
         <v/>
       </c>
       <c r="I14" t="str">
-        <v>г. Реутов, Юбилейный проспект, д. 72</v>
+        <v>Сумской проезд, д. 8, к. 1</v>
       </c>
       <c r="J14" t="str">
         <v/>
       </c>
       <c r="K14" t="str">
-        <v>г. Реутов, улица Октября, д. вл10</v>
+        <v>Варшавское шоссе, д. 97</v>
       </c>
       <c r="L14" t="str">
-        <v/>
-      </c>
-      <c r="M14" t="str">
-        <v>Кетчерская улица, д. 4Б, стр. 1</v>
-      </c>
-      <c r="N14" t="str">
         <v/>
       </c>
     </row>
@@ -878,36 +902,42 @@
         <v>ЛоялАвто</v>
       </c>
       <c r="B15" t="str">
-        <v>Исхаков Эмиль</v>
+        <v>Наматбеков Майрамбек</v>
       </c>
       <c r="C15" t="str">
-        <v>А181ВН797</v>
+        <v>Е885КС979</v>
       </c>
       <c r="D15">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E15" t="str">
-        <v>3-й Нижнелихоборский проезд, д. 3, кв. 1</v>
+        <v>Покровская улица, д. 17, к. 3</v>
       </c>
       <c r="F15" t="str">
         <v/>
       </c>
       <c r="G15" t="str">
-        <v>Большая Академическая улица, д. 75, к. 2</v>
+        <v>Рождественская улица, д. 4</v>
       </c>
       <c r="H15" t="str">
         <v/>
       </c>
       <c r="I15" t="str">
-        <v>проезд Черепановых, д. 36</v>
+        <v>г. Люберцы, улица Попова, д. 34/1</v>
       </c>
       <c r="J15" t="str">
         <v/>
       </c>
       <c r="K15" t="str">
-        <v>улица Дубки, д. 4А</v>
+        <v>г. Люберцы, улица Шевлякова, д. 2/24</v>
       </c>
       <c r="L15" t="str">
+        <v/>
+      </c>
+      <c r="M15" t="str">
+        <v>Святоозёрская улица, д. 14</v>
+      </c>
+      <c r="N15" t="str">
         <v/>
       </c>
     </row>
@@ -916,34 +946,34 @@
         <v>ЛоялАвто</v>
       </c>
       <c r="B16" t="str">
-        <v>Ковалев  Андрей</v>
+        <v>Нурбек Ерлан</v>
       </c>
       <c r="C16" t="str">
-        <v>М527ЕК777</v>
+        <v>О811КО797</v>
       </c>
       <c r="D16">
         <v>4</v>
       </c>
       <c r="E16" t="str">
-        <v>г. Королёв, Пионерская улица, д. 30, к. 9</v>
+        <v>Ленинский проспект, д. 44</v>
       </c>
       <c r="F16" t="str">
         <v/>
       </c>
       <c r="G16" t="str">
-        <v>г. Королёв, проспект Космонавтов, д. 34Б, к. Б</v>
+        <v>проспект 60-летия Октября, д. 18, к. 1</v>
       </c>
       <c r="H16" t="str">
         <v/>
       </c>
       <c r="I16" t="str">
-        <v>г. Королёв, проезд Макаренко, д. 1</v>
+        <v>Севастопольский проспект, д. 11Е</v>
       </c>
       <c r="J16" t="str">
         <v/>
       </c>
       <c r="K16" t="str">
-        <v>г. Королёв, улица 50-летия ВЛКСМ, д. 6, к. Е</v>
+        <v>улица Винокурова, д. 24, к. 4</v>
       </c>
       <c r="L16" t="str">
         <v/>
@@ -954,30 +984,36 @@
         <v>ЛоялАвто</v>
       </c>
       <c r="B17" t="str">
-        <v>Кошель Филипп</v>
+        <v>Оганес Мкртчян</v>
       </c>
       <c r="C17" t="str">
-        <v>В849НУ193</v>
+        <v>Т382УР799</v>
       </c>
       <c r="D17">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E17" t="str">
-        <v>г. Троицк, микрорайон В, д. 50</v>
+        <v>Ясногорская улица, д. 7А</v>
       </c>
       <c r="F17" t="str">
         <v/>
       </c>
       <c r="G17" t="str">
-        <v>г. Троицк, Академическая площадь, д. 3, кв. 2А</v>
+        <v>улица Тёплый Стан, д. 1А</v>
       </c>
       <c r="H17" t="str">
         <v/>
       </c>
       <c r="I17" t="str">
-        <v>г. Троицк, Городская улица, д. вл6</v>
+        <v>улица Тёплый Стан, д. 10</v>
       </c>
       <c r="J17" t="str">
+        <v/>
+      </c>
+      <c r="K17" t="str">
+        <v>Ленинский проспект, д. 123В</v>
+      </c>
+      <c r="L17" t="str">
         <v/>
       </c>
     </row>
@@ -986,28 +1022,28 @@
         <v>ЛоялАвто</v>
       </c>
       <c r="B18" t="str">
-        <v>Мурзаев Талант</v>
+        <v>Рамазанов Мурад</v>
       </c>
       <c r="C18" t="str">
-        <v>М980АМ62</v>
+        <v>А799ВХ790</v>
       </c>
       <c r="D18">
         <v>3</v>
       </c>
       <c r="E18" t="str">
-        <v>г. посёлок Коммунарка, Бачуринская улица, д. 11А, к. 2</v>
+        <v>Дмитровское шоссе, д. 107А, к. 3</v>
       </c>
       <c r="F18" t="str">
         <v/>
       </c>
       <c r="G18" t="str">
-        <v>г. посёлок Коммунарка, улица Липовый Парк, д. 2</v>
+        <v>Лобненская улица, д. 4А</v>
       </c>
       <c r="H18" t="str">
         <v/>
       </c>
       <c r="I18" t="str">
-        <v>г. Коммунарка, -, д. 7А</v>
+        <v>Ангарская улица, д. 57, к. 1</v>
       </c>
       <c r="J18" t="str">
         <v/>
@@ -1018,36 +1054,42 @@
         <v>ЛоялАвто</v>
       </c>
       <c r="B19" t="str">
-        <v>Наматбеков Майрамбек</v>
+        <v>Султанов Шамиль</v>
       </c>
       <c r="C19" t="str">
-        <v>Е885КС979</v>
+        <v>К392ВК177</v>
       </c>
       <c r="D19">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E19" t="str">
-        <v>улица Горчакова, д. 1</v>
+        <v>г. Зеленоград, -, д. к1562</v>
       </c>
       <c r="F19" t="str">
         <v/>
       </c>
       <c r="G19" t="str">
-        <v>Южнобутовская улица, д. 117</v>
+        <v>проезд Дежнёва, д. 29, к. 1</v>
       </c>
       <c r="H19" t="str">
         <v/>
       </c>
       <c r="I19" t="str">
-        <v>г. поселение Воскресенское, Чечёрский проезд, д. 122, к. 1</v>
+        <v>Ясный пр, д. 16</v>
       </c>
       <c r="J19" t="str">
         <v/>
       </c>
       <c r="K19" t="str">
-        <v>Венёвская улица, д. 4</v>
+        <v>улица Конёнкова, д. 23</v>
       </c>
       <c r="L19" t="str">
+        <v/>
+      </c>
+      <c r="M19" t="str">
+        <v>Широкая улица, д. 7, к. 2</v>
+      </c>
+      <c r="N19" t="str">
         <v/>
       </c>
     </row>
@@ -1056,30 +1098,36 @@
         <v>ЛоялАвто</v>
       </c>
       <c r="B20" t="str">
-        <v>Некоз Дмитрий</v>
+        <v>Филяков Алексей</v>
       </c>
       <c r="C20" t="str">
-        <v>Е550УК197</v>
+        <v>К726ХЕ777</v>
       </c>
       <c r="D20">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E20" t="str">
-        <v>улица Большая Ордынка, д. 44, стр. 2</v>
+        <v>улица 26-ти Бакинских Комиссаров, д. 12, к. 2</v>
       </c>
       <c r="F20" t="str">
         <v/>
       </c>
       <c r="G20" t="str">
-        <v>улица Арбат, д. 4, стр. 1</v>
+        <v>улица Удальцова, д. 42</v>
       </c>
       <c r="H20" t="str">
         <v/>
       </c>
       <c r="I20" t="str">
-        <v>Газетный переулок, д. 13, стр. 1</v>
+        <v>Мичуринский проспект, д. 21, к. 1</v>
       </c>
       <c r="J20" t="str">
+        <v/>
+      </c>
+      <c r="K20" t="str">
+        <v>улица Мичуринский Проспект, Олимпийская Деревня, д. 4, к. 2</v>
+      </c>
+      <c r="L20" t="str">
         <v/>
       </c>
     </row>
@@ -1088,36 +1136,30 @@
         <v>ЛоялАвто</v>
       </c>
       <c r="B21" t="str">
-        <v>Нетреба Юрий</v>
+        <v>Черноусов  Геннадий</v>
       </c>
       <c r="C21" t="str">
-        <v>К494РН750</v>
+        <v>У976ВР799</v>
       </c>
       <c r="D21">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E21" t="str">
-        <v>Электролитный проезд, д. 16, к. 1</v>
+        <v>улица Лавочкина, д. 34</v>
       </c>
       <c r="F21" t="str">
         <v/>
       </c>
       <c r="G21" t="str">
-        <v>проспект 60-летия Октября, д. 18, к. 1</v>
+        <v>Авангардная улица, д. 3</v>
       </c>
       <c r="H21" t="str">
         <v/>
       </c>
       <c r="I21" t="str">
-        <v>улица Винокурова, д. 24, к. 4</v>
+        <v>проезд Черепановых, д. 36</v>
       </c>
       <c r="J21" t="str">
-        <v/>
-      </c>
-      <c r="K21" t="str">
-        <v>Варшавское шоссе, д. 26, стр. 7</v>
-      </c>
-      <c r="L21" t="str">
         <v/>
       </c>
     </row>
@@ -1126,110 +1168,128 @@
         <v>ЛоялАвто</v>
       </c>
       <c r="B22" t="str">
-        <v>Нурбек Ерлан</v>
+        <v>Шадыканов Руслан</v>
       </c>
       <c r="C22" t="str">
-        <v>О811КО797</v>
+        <v>О586РВ199</v>
       </c>
       <c r="D22">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E22" t="str">
-        <v>улица Маршала Рыбалко, д. 2, к. 6, кв. 106</v>
+        <v>улица Горчакова, д. 1</v>
       </c>
       <c r="F22" t="str">
         <v/>
       </c>
       <c r="G22" t="str">
-        <v>улица Расплетина, д. 13</v>
+        <v>Венёвская улица, д. 4</v>
       </c>
       <c r="H22" t="str">
         <v/>
       </c>
       <c r="I22" t="str">
-        <v>улица Маршала Новикова, д. 2, к. 2</v>
+        <v>улица Поляны, д. 5</v>
       </c>
       <c r="J22" t="str">
         <v/>
       </c>
       <c r="K22" t="str">
-        <v>Волоколамское шоссе, д. 1, стр. 1</v>
+        <v>улица Знаменские Садки, д. 1, к. 1</v>
       </c>
       <c r="L22" t="str">
+        <v/>
+      </c>
+      <c r="M22" t="str">
+        <v>Старокачаловская, д. 1, к. 2</v>
+      </c>
+      <c r="N22" t="str">
         <v/>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="str">
-        <v>ЛоялАвто</v>
+        <v>МАУ</v>
       </c>
       <c r="B23" t="str">
-        <v>Оганес Мкртчян</v>
+        <v>Власов Александр</v>
       </c>
       <c r="C23" t="str">
-        <v>Т382УР799</v>
+        <v>М602МК134</v>
       </c>
       <c r="D23">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E23" t="str">
-        <v>г. Щелково, Пушкина, д. 3</v>
+        <v>Волгоградский проспект, д. 177</v>
       </c>
       <c r="F23" t="str">
         <v/>
       </c>
       <c r="G23" t="str">
-        <v>г. Королёв, Бурковский проезд, д. 48, к. 2</v>
+        <v>Рязанский проспект, д. 30, к. 2</v>
       </c>
       <c r="H23" t="str">
         <v/>
       </c>
       <c r="I23" t="str">
-        <v>г. Щелково, 1-й Советский переулок, д. 5</v>
+        <v>улица Васильцовский Стан, д. 9</v>
       </c>
       <c r="J23" t="str">
+        <v/>
+      </c>
+      <c r="K23" t="str">
+        <v>Волжский бульвар, д. 38</v>
+      </c>
+      <c r="L23" t="str">
+        <v/>
+      </c>
+      <c r="M23" t="str">
+        <v>улица Юных Ленинцев, д. 52</v>
+      </c>
+      <c r="N23" t="str">
         <v/>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="str">
-        <v>ЛоялАвто</v>
+        <v>МАУ</v>
       </c>
       <c r="B24" t="str">
-        <v>Султанов Шамиль</v>
+        <v>Гусейнов Тогрул</v>
       </c>
       <c r="C24" t="str">
-        <v>К392ВК177</v>
+        <v>Е857АМ62</v>
       </c>
       <c r="D24">
         <v>5</v>
       </c>
       <c r="E24" t="str">
-        <v>Перовская улица, д. 55</v>
+        <v>г. Дзержинский, Лесная улица, д. 11</v>
       </c>
       <c r="F24" t="str">
         <v/>
       </c>
       <c r="G24" t="str">
-        <v>Зелёный проспект, д. 3А, стр. 1</v>
+        <v>Братиславская улица, д. 33</v>
       </c>
       <c r="H24" t="str">
         <v/>
       </c>
       <c r="I24" t="str">
-        <v>2-я Владимирская улица, д. 34</v>
+        <v>Краснодарская улица, д. 16</v>
       </c>
       <c r="J24" t="str">
         <v/>
       </c>
       <c r="K24" t="str">
-        <v>Свободный проспект, д. 33А</v>
+        <v>улица Артюхиной, д. 24, к. 1</v>
       </c>
       <c r="L24" t="str">
         <v/>
       </c>
       <c r="M24" t="str">
-        <v>шоссе Энтузиастов, д. 55</v>
+        <v>Новороссийская улица, д. 24, к. 1</v>
       </c>
       <c r="N24" t="str">
         <v/>
@@ -1237,37 +1297,37 @@
     </row>
     <row r="25">
       <c r="A25" t="str">
-        <v>ЛоялАвто</v>
+        <v>МАУ</v>
       </c>
       <c r="B25" t="str">
-        <v>Филяков Алексей</v>
+        <v>Калмыков Александр</v>
       </c>
       <c r="C25" t="str">
-        <v>К726ХЕ777</v>
+        <v>М899МК142</v>
       </c>
       <c r="D25">
         <v>4</v>
       </c>
       <c r="E25" t="str">
-        <v>Ленинский проспект, д. 123В</v>
+        <v>Минусинская улица, д. 9</v>
       </c>
       <c r="F25" t="str">
         <v/>
       </c>
       <c r="G25" t="str">
-        <v>Профсоюзная улица, д. 102А</v>
+        <v>улица Коминтерна, д. 33, к. 2</v>
       </c>
       <c r="H25" t="str">
         <v/>
       </c>
       <c r="I25" t="str">
-        <v>Профсоюзная улица, д. 61А</v>
+        <v>Тайнинская улица, д. 9</v>
       </c>
       <c r="J25" t="str">
         <v/>
       </c>
       <c r="K25" t="str">
-        <v>Перекопская улица, д. 34, к. 3</v>
+        <v>улица Лётчика Бабушкина, д. 39</v>
       </c>
       <c r="L25" t="str">
         <v/>
@@ -1275,65 +1335,77 @@
     </row>
     <row r="26">
       <c r="A26" t="str">
-        <v>ЛоялАвто</v>
+        <v>МАУ</v>
       </c>
       <c r="B26" t="str">
-        <v>Черноусов  Геннадий</v>
+        <v xml:space="preserve">Марченко Андрей </v>
       </c>
       <c r="C26" t="str">
-        <v>У976ВР799</v>
+        <v>О394НТ46</v>
       </c>
       <c r="D26">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E26" t="str">
-        <v>г. Раменское, Десантная улица, д. 17</v>
+        <v>г. Старая Купавна, Октябрьская улица, д. 19</v>
       </c>
       <c r="F26" t="str">
         <v/>
       </c>
       <c r="G26" t="str">
-        <v>г. Раменское, Десантная улица, д. 14</v>
+        <v>г. Лосино-Петровский, улица Гоголя, д. 21</v>
       </c>
       <c r="H26" t="str">
         <v/>
       </c>
       <c r="I26" t="str">
-        <v>г. Жуковский, улица Чкалова, д. 2А, стр. 1</v>
+        <v>г. Щёлково, улица Радиоцентра № 5, д. 16</v>
       </c>
       <c r="J26" t="str">
-        <v/>
-      </c>
-      <c r="K26" t="str">
-        <v>г. Жуковский, улица Горького, д. 4</v>
-      </c>
-      <c r="L26" t="str">
         <v/>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="str">
-        <v>ЛоялАвто</v>
+        <v>МАУ</v>
       </c>
       <c r="B27" t="str">
-        <v>Шадыканов Руслан</v>
+        <v>Нуриев Азим</v>
       </c>
       <c r="C27" t="str">
-        <v>О586РВ199</v>
+        <v>Е322АМ62</v>
       </c>
       <c r="D27">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E27" t="str">
-        <v>Дмитровское шоссе, д. 163А, к. 2</v>
+        <v>Перовская улица, д. 55</v>
       </c>
       <c r="F27" t="str">
         <v/>
       </c>
       <c r="G27" t="str">
-        <v>Дмитровское шоссе, д. 169, к. 9</v>
+        <v>2-я Владимирская улица, д. 34</v>
       </c>
       <c r="H27" t="str">
+        <v/>
+      </c>
+      <c r="I27" t="str">
+        <v>Зелёный проспект, д. 3А, стр. 1</v>
+      </c>
+      <c r="J27" t="str">
+        <v/>
+      </c>
+      <c r="K27" t="str">
+        <v>Свободный проспект, д. 33А</v>
+      </c>
+      <c r="L27" t="str">
+        <v/>
+      </c>
+      <c r="M27" t="str">
+        <v>Кетчерская улица, д. 4Б, стр. 1</v>
+      </c>
+      <c r="N27" t="str">
         <v/>
       </c>
     </row>
@@ -1342,36 +1414,30 @@
         <v>МАУ</v>
       </c>
       <c r="B28" t="str">
-        <v>Власов Александр</v>
+        <v>Сломинский Дмитрий</v>
       </c>
       <c r="C28" t="str">
-        <v>М602МК134</v>
+        <v>В272СУ177</v>
       </c>
       <c r="D28">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E28" t="str">
-        <v>Большая Академическая улица, д. 24, к. 2</v>
+        <v>улица Большая Ордынка, д. 44, стр. 2</v>
       </c>
       <c r="F28" t="str">
         <v/>
       </c>
       <c r="G28" t="str">
-        <v>Соболевский проезд, д. 22, стр. 1</v>
+        <v>улица Арбат, д. 4, стр. 1</v>
       </c>
       <c r="H28" t="str">
         <v/>
       </c>
       <c r="I28" t="str">
-        <v>Старопетровский проезд, д. 1, стр. 2</v>
+        <v>Газетный переулок, д. 13, стр. 1</v>
       </c>
       <c r="J28" t="str">
-        <v/>
-      </c>
-      <c r="K28" t="str">
-        <v>Ленинградское шоссе, д. 13, к. 1</v>
-      </c>
-      <c r="L28" t="str">
         <v/>
       </c>
     </row>
@@ -1380,30 +1446,36 @@
         <v>МАУ</v>
       </c>
       <c r="B29" t="str">
-        <v>Герцев  Ян</v>
+        <v>Стребков Игорь</v>
       </c>
       <c r="C29" t="str">
-        <v>К609НО790</v>
+        <v>Н353УТ199</v>
       </c>
       <c r="D29">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E29" t="str">
-        <v>улица 26-ти Бакинских Комиссаров, д. 12, к. 2</v>
+        <v>г. Мытищи, улица Комарова, д. 2, к. 2</v>
       </c>
       <c r="F29" t="str">
         <v/>
       </c>
       <c r="G29" t="str">
-        <v>улица Мичуринский Проспект, Олимпийская Деревня, д. 4, к. 2</v>
+        <v>г. Мытищи, улица Колпакова, д. 10</v>
       </c>
       <c r="H29" t="str">
         <v/>
       </c>
       <c r="I29" t="str">
-        <v>Мичуринский проспект, д. 21, к. 1</v>
+        <v>г. Мытищи, проспект Астрахова, д. 6</v>
       </c>
       <c r="J29" t="str">
+        <v/>
+      </c>
+      <c r="K29" t="str">
+        <v>г. Мытищи, 1-й Щёлковский проезд, д. 7</v>
+      </c>
+      <c r="L29" t="str">
         <v/>
       </c>
     </row>
@@ -1412,36 +1484,42 @@
         <v>МАУ</v>
       </c>
       <c r="B30" t="str">
-        <v>Глазунов  Роман</v>
+        <v>Хлуденцов Иван</v>
       </c>
       <c r="C30" t="str">
-        <v>Р767АО799</v>
+        <v>О178РН68</v>
       </c>
       <c r="D30">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E30" t="str">
-        <v>г. Домодедово, улица Гагарина, д. 37</v>
+        <v>г. Балашиха, улица Некрасова, д. 13А</v>
       </c>
       <c r="F30" t="str">
         <v/>
       </c>
       <c r="G30" t="str">
-        <v>г. Домодедово, Курыжова, д. 30, к. 1</v>
+        <v>г. Балашиха, улица Твардовского, д. 44</v>
       </c>
       <c r="H30" t="str">
         <v/>
       </c>
       <c r="I30" t="str">
-        <v>г. Домодедово, Южнодомодедовская улица, д. 16</v>
+        <v>г. Балашиха, проспект Ленина, д. 74</v>
       </c>
       <c r="J30" t="str">
         <v/>
       </c>
       <c r="K30" t="str">
-        <v>г. Домодедово, улица Корнеева, д. 1</v>
+        <v>г. Балашиха, улица Свердлова, д. 1А, кв. 151</v>
       </c>
       <c r="L30" t="str">
+        <v/>
+      </c>
+      <c r="M30" t="str">
+        <v>г. Балашиха, Живописная улица, д. 1</v>
+      </c>
+      <c r="N30" t="str">
         <v/>
       </c>
     </row>
@@ -1450,42 +1528,30 @@
         <v>МАУ</v>
       </c>
       <c r="B31" t="str">
-        <v>Головин Виктор</v>
+        <v>Черногор Виктор</v>
       </c>
       <c r="C31" t="str">
-        <v>В256УВ777</v>
+        <v>В632ХА799</v>
       </c>
       <c r="D31">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E31" t="str">
-        <v>г. Зеленоград, к. 1651</v>
+        <v>г. Ивантеевка, улица Новая Слобода, д. 3</v>
       </c>
       <c r="F31" t="str">
         <v/>
       </c>
       <c r="G31" t="str">
-        <v>г. Зеленоград, Георгиевский проспект, д. 33, к. 6</v>
+        <v>г. Ивантеевка, улица Новосёлки, д. 4</v>
       </c>
       <c r="H31" t="str">
         <v/>
       </c>
       <c r="I31" t="str">
-        <v>г. Зеленоград, -, д. к1562</v>
+        <v>г. Ивантеевка, Школьная улица, д. 16</v>
       </c>
       <c r="J31" t="str">
-        <v/>
-      </c>
-      <c r="K31" t="str">
-        <v>г. Зеленоград, к. 1508</v>
-      </c>
-      <c r="L31" t="str">
-        <v/>
-      </c>
-      <c r="M31" t="str">
-        <v>г. Зеленоград, улица Панфилова, д. 28Б</v>
-      </c>
-      <c r="N31" t="str">
         <v/>
       </c>
     </row>
@@ -1494,30 +1560,36 @@
         <v>МАУ</v>
       </c>
       <c r="B32" t="str">
-        <v>Гусейнов Тогрул</v>
+        <v>Эркинбек Уулу Эмилбек</v>
       </c>
       <c r="C32" t="str">
-        <v>Е857АМ62</v>
+        <v>С174СА777</v>
       </c>
       <c r="D32">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E32" t="str">
-        <v>Базовская улица, д. 15, к. 15</v>
+        <v>г. Бутово, жилой комплекс Бутово Парк, д. 28</v>
       </c>
       <c r="F32" t="str">
         <v/>
       </c>
       <c r="G32" t="str">
-        <v>улица Дыбенко, д. 36, к. 4</v>
+        <v>улица Маршала Савицкого, д. 18, к. 2</v>
       </c>
       <c r="H32" t="str">
         <v/>
       </c>
       <c r="I32" t="str">
-        <v>Локомотивный проезд, д. 4</v>
+        <v>улица Брусилова, д. 13</v>
       </c>
       <c r="J32" t="str">
+        <v/>
+      </c>
+      <c r="K32" t="str">
+        <v>г. рабочий посёлок Дрожжино, Новое шоссе, д. 11</v>
+      </c>
+      <c r="L32" t="str">
         <v/>
       </c>
     </row>
@@ -1526,18 +1598,42 @@
         <v>МАУ</v>
       </c>
       <c r="B33" t="str">
-        <v>Иванов Олег</v>
+        <v>Ядренников Андрей</v>
       </c>
       <c r="C33" t="str">
-        <v>У991ММ750</v>
+        <v>Н351ХР197</v>
       </c>
       <c r="D33">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E33" t="str">
-        <v>г. Звенигород, Почтовая улица, д. 41, к. 1</v>
+        <v>Варшавское шоссе, д. 141А, к. 2, кв. пом. 5</v>
       </c>
       <c r="F33" t="str">
+        <v/>
+      </c>
+      <c r="G33" t="str">
+        <v>Россошанский проезд, д. 3</v>
+      </c>
+      <c r="H33" t="str">
+        <v/>
+      </c>
+      <c r="I33" t="str">
+        <v>Чертановская улица, д. 32, к. 1</v>
+      </c>
+      <c r="J33" t="str">
+        <v/>
+      </c>
+      <c r="K33" t="str">
+        <v>улица Красного Маяка, д. 15А, стр. 1</v>
+      </c>
+      <c r="L33" t="str">
+        <v/>
+      </c>
+      <c r="M33" t="str">
+        <v>Кировоградская, д. 30</v>
+      </c>
+      <c r="N33" t="str">
         <v/>
       </c>
     </row>
@@ -1546,28 +1642,28 @@
         <v>МАУ</v>
       </c>
       <c r="B34" t="str">
-        <v>Калмыков Александр</v>
+        <v>Ярковский Алексей</v>
       </c>
       <c r="C34" t="str">
-        <v>М899МК142</v>
+        <v>Т973АН790</v>
       </c>
       <c r="D34">
         <v>3</v>
       </c>
       <c r="E34" t="str">
-        <v>г. Сергиев Посад, улица Матросова, д. 2/1, стр. 1</v>
+        <v>г. Зеленоград, к. 1651</v>
       </c>
       <c r="F34" t="str">
         <v/>
       </c>
       <c r="G34" t="str">
-        <v>г. Сергиев Посад, улица Дружбы, д. 14, к. А</v>
+        <v>г. деревня Голубое, Тверецкий проезд, д. 16, к. 3</v>
       </c>
       <c r="H34" t="str">
         <v/>
       </c>
       <c r="I34" t="str">
-        <v>г. Сергиев Посад, Кооперативная улица, д. 20</v>
+        <v>г. Зеленоград, Георгиевский проспект, д. 33, к. 6</v>
       </c>
       <c r="J34" t="str">
         <v/>
@@ -1575,57 +1671,69 @@
     </row>
     <row r="35">
       <c r="A35" t="str">
-        <v>МАУ</v>
+        <v>Проект А</v>
       </c>
       <c r="B35" t="str">
-        <v xml:space="preserve">Марченко Андрей </v>
+        <v>Ёров Насруло</v>
       </c>
       <c r="C35" t="str">
-        <v>О394НТ46</v>
+        <v>М712хт197</v>
       </c>
       <c r="D35">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E35" t="str">
-        <v>г. Красногорск, Спасская улица, д. 12</v>
+        <v>г. посёлок Коммунарка, улица Александры Монаховой, д. 96, к. 2</v>
       </c>
       <c r="F35" t="str">
         <v/>
       </c>
       <c r="G35" t="str">
-        <v>г. Красногорск, Красногорский бульвар, д. 14</v>
+        <v>г. посёлок Коммунарка, улица Липовый Парк, д. 2</v>
       </c>
       <c r="H35" t="str">
+        <v/>
+      </c>
+      <c r="I35" t="str">
+        <v>г. Коммунарка, -, д. 7А</v>
+      </c>
+      <c r="J35" t="str">
+        <v/>
+      </c>
+      <c r="K35" t="str">
+        <v>г. посёлок Коммунарка, Бачуринская улица, д. 11А, к. 2</v>
+      </c>
+      <c r="L35" t="str">
         <v/>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="str">
-        <v>МАУ</v>
+        <v>Проект А</v>
       </c>
       <c r="B36" t="str">
-        <v>Нуриев Азим</v>
+        <v>Абдырахман Зайирбек</v>
       </c>
       <c r="C36" t="str">
-        <v>Е322АМ62</v>
+        <v>Н600РХ777</v>
       </c>
       <c r="D36">
         <v>3</v>
       </c>
       <c r="E36" t="str">
-        <v>улица Марии Ульяновой, д. 9, к. 3</v>
+        <v>г. Зеленоград, к. 1508</v>
       </c>
       <c r="F36" t="str">
         <v/>
       </c>
       <c r="G36" t="str">
-        <v>улица Удальцова, д. 42</v>
+        <v>г. Зеленоград, -, д. 403А, стр. 9</v>
       </c>
       <c r="H36" t="str">
         <v/>
       </c>
       <c r="I36" t="str">
-        <v>улица Кравченко, д. 11</v>
+        <v>г. Зеленоград, улица Болдов Ручей, д. 1</v>
       </c>
       <c r="J36" t="str">
         <v/>
@@ -1633,189 +1741,171 @@
     </row>
     <row r="37">
       <c r="A37" t="str">
-        <v>МАУ</v>
+        <v>Проект А</v>
       </c>
       <c r="B37" t="str">
-        <v>Сломинский Дмитрий</v>
+        <v>Алымкулов Акылбек</v>
       </c>
       <c r="C37" t="str">
-        <v>В272СУ177</v>
+        <v>М769АМ62</v>
       </c>
       <c r="D37">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E37" t="str">
-        <v>Волгоградский проспект, д. 177</v>
+        <v>г. Долгопрудный, Лихачёвское шоссе, д. 6</v>
       </c>
       <c r="F37" t="str">
         <v/>
       </c>
       <c r="G37" t="str">
-        <v>Снайперская улица, д. 9А</v>
+        <v>г. Долгопрудный, проспект Пацаева, д. 12</v>
       </c>
       <c r="H37" t="str">
         <v/>
       </c>
       <c r="I37" t="str">
-        <v>Рязанский проспект, д. 30, к. 2</v>
+        <v>г. Долгопрудный, Набережная улица, д. 31</v>
       </c>
       <c r="J37" t="str">
-        <v/>
-      </c>
-      <c r="K37" t="str">
-        <v>Сормовская улица, д. 6</v>
-      </c>
-      <c r="L37" t="str">
-        <v/>
-      </c>
-      <c r="M37" t="str">
-        <v>Лермонтовский проспект, д. 19, к. 1</v>
-      </c>
-      <c r="N37" t="str">
         <v/>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="str">
-        <v>МАУ</v>
+        <v>Проект А</v>
       </c>
       <c r="B38" t="str">
-        <v>Трушкин Максим</v>
+        <v>Артыков Мухамед</v>
       </c>
       <c r="C38" t="str">
-        <v>Р103КЕ790</v>
+        <v>У659КР136</v>
       </c>
       <c r="D38">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E38" t="str">
-        <v>Кастанаевская улица, д. 45, к. 2</v>
+        <v>г. Красногорск, бульвар Космонавтов, д. 17</v>
       </c>
       <c r="F38" t="str">
         <v/>
       </c>
       <c r="G38" t="str">
-        <v>площадь Джавахарлала Неру, д. 1</v>
+        <v>г. Красногорск, Светлая улица, д. 3А, стр. 4</v>
       </c>
       <c r="H38" t="str">
-        <v/>
-      </c>
-      <c r="I38" t="str">
-        <v>улица Вавилова, д. 66</v>
-      </c>
-      <c r="J38" t="str">
         <v/>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="str">
-        <v>МАУ</v>
+        <v>Проект А</v>
       </c>
       <c r="B39" t="str">
-        <v>Хлуденцов Иван</v>
+        <v>Аскарбеков Омурбек</v>
       </c>
       <c r="C39" t="str">
-        <v>О178РН68</v>
+        <v>А796ВО750</v>
       </c>
       <c r="D39">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E39" t="str">
-        <v>г. Дзержинский, Лесная улица, д. 11</v>
+        <v>г. Сергиев Посад, Кооперативная улица, д. 20</v>
       </c>
       <c r="F39" t="str">
         <v/>
       </c>
       <c r="G39" t="str">
-        <v>Новороссийская улица, д. 24, к. 1</v>
+        <v>г. Сергиев Посад, улица Дружбы, д. 14, к. А</v>
       </c>
       <c r="H39" t="str">
         <v/>
       </c>
       <c r="I39" t="str">
-        <v>улица Перерва, д. 45</v>
+        <v>г. Сергиев Посад, улица Матросова, д. 2/1, стр. 1</v>
       </c>
       <c r="J39" t="str">
-        <v/>
-      </c>
-      <c r="K39" t="str">
-        <v>Братиславская улица, д. 16, к. 1</v>
-      </c>
-      <c r="L39" t="str">
-        <v/>
-      </c>
-      <c r="M39" t="str">
-        <v>Братиславская улица, д. 33</v>
-      </c>
-      <c r="N39" t="str">
         <v/>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="str">
-        <v>МАУ</v>
+        <v>Проект А</v>
       </c>
       <c r="B40" t="str">
-        <v>Эркинбек Уулу Эмилбек</v>
+        <v>Атамкулов Айбек</v>
       </c>
       <c r="C40" t="str">
-        <v>С174СА777</v>
+        <v>Е818СВ197</v>
       </c>
       <c r="D40">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E40" t="str">
-        <v>г. Подольск, Февральская улица, д. 54/150</v>
+        <v>Измайловский проезд, д. 13</v>
       </c>
       <c r="F40" t="str">
         <v/>
       </c>
       <c r="G40" t="str">
-        <v>г. Подольск, улица Генерала Варенникова, д. 4</v>
+        <v>Измайловский проезд, д. 10, к. 3</v>
       </c>
       <c r="H40" t="str">
         <v/>
       </c>
       <c r="I40" t="str">
-        <v>г. Подольск, улица 50 лет ВЛКСМ, д. 18, к. А, кв. 13</v>
+        <v>Заводской проезд, д. 10</v>
       </c>
       <c r="J40" t="str">
+        <v/>
+      </c>
+      <c r="K40" t="str">
+        <v>Верхняя Первомайская улица, д. 59/35, к. 3</v>
+      </c>
+      <c r="L40" t="str">
+        <v/>
+      </c>
+      <c r="M40" t="str">
+        <v>9-я Парковая улица, д. 6, к. 1</v>
+      </c>
+      <c r="N40" t="str">
         <v/>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="str">
-        <v>МАУ</v>
+        <v>Проект А</v>
       </c>
       <c r="B41" t="str">
-        <v>Ядренников Андрей</v>
+        <v>Ашурбеков Магомед</v>
       </c>
       <c r="C41" t="str">
-        <v>Н351ХР197</v>
+        <v>Т500ВК05</v>
       </c>
       <c r="D41">
         <v>4</v>
       </c>
       <c r="E41" t="str">
-        <v>Большая Спасская улица, д. 8, стр. 1А</v>
+        <v>улица Шолохова, д. 5, к. 2</v>
       </c>
       <c r="F41" t="str">
         <v/>
       </c>
       <c r="G41" t="str">
-        <v>Плетешковский переулок, д. 17, стр. 1</v>
+        <v>Новопеределкинская улица, д. 13</v>
       </c>
       <c r="H41" t="str">
         <v/>
       </c>
       <c r="I41" t="str">
-        <v>Большая Почтовая улица, д. 43-45, стр. 2</v>
+        <v>улица Авиаторов, д. 5, к. 6</v>
       </c>
       <c r="J41" t="str">
         <v/>
       </c>
       <c r="K41" t="str">
-        <v>Сокольническая площадь, д. 9А, стр. А</v>
+        <v>Солнцевский проспект, д. 15</v>
       </c>
       <c r="L41" t="str">
         <v/>
@@ -1823,39 +1913,21 @@
     </row>
     <row r="42">
       <c r="A42" t="str">
-        <v>МАУ</v>
+        <v>Проект А</v>
       </c>
       <c r="B42" t="str">
-        <v>Ярковский Алексей</v>
+        <v>Бордашевский Сергей</v>
       </c>
       <c r="C42" t="str">
-        <v>Т973АН790</v>
+        <v>У624ЕХ777</v>
       </c>
       <c r="D42">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E42" t="str">
-        <v>Суворовская улица, д. 24</v>
+        <v>г. Звенигород, Почтовая улица, д. 41, к. 1</v>
       </c>
       <c r="F42" t="str">
-        <v/>
-      </c>
-      <c r="G42" t="str">
-        <v>улица Космонавтов, д. 22</v>
-      </c>
-      <c r="H42" t="str">
-        <v/>
-      </c>
-      <c r="I42" t="str">
-        <v>2-я Прогонная, д. 10</v>
-      </c>
-      <c r="J42" t="str">
-        <v/>
-      </c>
-      <c r="K42" t="str">
-        <v>Краснобогатырская улица, д. 90, стр. 2</v>
-      </c>
-      <c r="L42" t="str">
         <v/>
       </c>
     </row>
@@ -1864,24 +1936,36 @@
         <v>Проект А</v>
       </c>
       <c r="B43" t="str">
-        <v>Абдырахман Зайирбек</v>
+        <v>Дубанакулов Адылбек</v>
       </c>
       <c r="C43" t="str">
-        <v>Н600РХ777</v>
+        <v>С746НА790</v>
       </c>
       <c r="D43">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E43" t="str">
-        <v>улица Генерала Белобородова, д. 37</v>
+        <v>г. Мытищи, улица Семашко, д. 25</v>
       </c>
       <c r="F43" t="str">
         <v/>
       </c>
       <c r="G43" t="str">
-        <v>г. Красногорск, Заводская улица, д. 18, к. 2</v>
+        <v>г. Мытищи, Борисовка, д. 20А</v>
       </c>
       <c r="H43" t="str">
+        <v/>
+      </c>
+      <c r="I43" t="str">
+        <v>г. Мытищи, Лётная улица, д. 27А</v>
+      </c>
+      <c r="J43" t="str">
+        <v/>
+      </c>
+      <c r="K43" t="str">
+        <v>г. Мытищи, Новомытищинский проспект, д. 17</v>
+      </c>
+      <c r="L43" t="str">
         <v/>
       </c>
     </row>
@@ -1890,34 +1974,34 @@
         <v>Проект А</v>
       </c>
       <c r="B44" t="str">
-        <v>Алымкулов Акылбек</v>
+        <v>Дубанакулов Бактилек</v>
       </c>
       <c r="C44" t="str">
-        <v>М769АМ62</v>
+        <v>Х938КМ37</v>
       </c>
       <c r="D44">
         <v>4</v>
       </c>
       <c r="E44" t="str">
-        <v>г. Балашиха, улица Свердлова, д. 1А, кв. 151</v>
+        <v>улица Академика Миллионщикова, д. 19</v>
       </c>
       <c r="F44" t="str">
         <v/>
       </c>
       <c r="G44" t="str">
-        <v>г. Балашиха, Балашихинское шоссе, д. 10</v>
+        <v>Нагатинская улица, д. 16</v>
       </c>
       <c r="H44" t="str">
         <v/>
       </c>
       <c r="I44" t="str">
-        <v>г. Балашиха, улица Лукино, д. 55А</v>
+        <v>проспект Андропова, д. 22</v>
       </c>
       <c r="J44" t="str">
         <v/>
       </c>
       <c r="K44" t="str">
-        <v>г. Балашиха, Кольцевая улица, д. 3К2, к. 2</v>
+        <v>улица Речников, д. 14, к. 1</v>
       </c>
       <c r="L44" t="str">
         <v/>
@@ -1928,36 +2012,30 @@
         <v>Проект А</v>
       </c>
       <c r="B45" t="str">
-        <v>Артыков Мухамед</v>
+        <v>Исаков Гулмырза</v>
       </c>
       <c r="C45" t="str">
-        <v>У659КР136</v>
+        <v>Т754ММ142</v>
       </c>
       <c r="D45">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E45" t="str">
-        <v>улица Красного Маяка, д. 15А, стр. 1</v>
+        <v>улица Генерала Белобородова, д. 37</v>
       </c>
       <c r="F45" t="str">
         <v/>
       </c>
       <c r="G45" t="str">
-        <v>Чертановская улица, д. 32, к. 1</v>
+        <v>г. Красногорск, Красногорский бульвар, д. 14</v>
       </c>
       <c r="H45" t="str">
         <v/>
       </c>
       <c r="I45" t="str">
-        <v>Варшавское шоссе, д. вл132/2</v>
+        <v>г. Красногорск, Спасская улица, д. 12</v>
       </c>
       <c r="J45" t="str">
-        <v/>
-      </c>
-      <c r="K45" t="str">
-        <v>Кировоградская, д. 30</v>
-      </c>
-      <c r="L45" t="str">
         <v/>
       </c>
     </row>
@@ -1966,30 +2044,36 @@
         <v>Проект А</v>
       </c>
       <c r="B46" t="str">
-        <v>Аскарбеков Омурбек</v>
+        <v>Кандаров Азиз</v>
       </c>
       <c r="C46" t="str">
-        <v>А796ВО750</v>
+        <v>К331ТХ750</v>
       </c>
       <c r="D46">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E46" t="str">
-        <v>г. поселение Десеновское, 1-я Нововатутинская улица, д. 5</v>
+        <v>Алтуфьевское шоссе, д. 27</v>
       </c>
       <c r="F46" t="str">
         <v/>
       </c>
       <c r="G46" t="str">
-        <v>г. Московский, улица Хабарова, д. 2</v>
+        <v>3-й Нижнелихоборский проезд, д. 3, кв. 1</v>
       </c>
       <c r="H46" t="str">
         <v/>
       </c>
       <c r="I46" t="str">
-        <v>г. посёлок Коммунарка, улица Александры Монаховой, д. 96, к. 2</v>
+        <v>Большая Академическая улица, д. 75, к. 2</v>
       </c>
       <c r="J46" t="str">
+        <v/>
+      </c>
+      <c r="K46" t="str">
+        <v>Локомотивный проезд, д. 4</v>
+      </c>
+      <c r="L46" t="str">
         <v/>
       </c>
     </row>
@@ -1998,24 +2082,36 @@
         <v>Проект А</v>
       </c>
       <c r="B47" t="str">
-        <v>Атамкулов Айбек</v>
+        <v>Касымов Аскар</v>
       </c>
       <c r="C47" t="str">
-        <v>Е818СВ197</v>
+        <v>н703ху777</v>
       </c>
       <c r="D47">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E47" t="str">
-        <v>г. Апрелевка, Сентябрьская улица, д. 5, стр. 2</v>
+        <v>г. поселение Внуковское, улица Корнея Чуковского, д. 3</v>
       </c>
       <c r="F47" t="str">
         <v/>
       </c>
       <c r="G47" t="str">
-        <v>г. Селятино, Клубная, д. 55</v>
+        <v>улица Лётчика Грицевца, д. 12</v>
       </c>
       <c r="H47" t="str">
+        <v/>
+      </c>
+      <c r="I47" t="str">
+        <v>г. поселение Внуковское, Омская улица, д. 7А</v>
+      </c>
+      <c r="J47" t="str">
+        <v/>
+      </c>
+      <c r="K47" t="str">
+        <v>г. Внуково, Центральная улица, д. 8Б, кв. 212</v>
+      </c>
+      <c r="L47" t="str">
         <v/>
       </c>
     </row>
@@ -2024,36 +2120,30 @@
         <v>Проект А</v>
       </c>
       <c r="B48" t="str">
-        <v>Ашурбеков Магомед</v>
+        <v>Конев Алексей</v>
       </c>
       <c r="C48" t="str">
-        <v>Т500ВК05</v>
+        <v>Р682АХ68</v>
       </c>
       <c r="D48">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E48" t="str">
-        <v>Новотушинский проезд, д. 6, к. 1</v>
+        <v>г. Щёлково, микрорайон Финский, д. 11, к. 1</v>
       </c>
       <c r="F48" t="str">
         <v/>
       </c>
       <c r="G48" t="str">
-        <v>Митинская улица, д. 27</v>
+        <v>г. Щелково, 1-й Советский переулок, д. 5</v>
       </c>
       <c r="H48" t="str">
         <v/>
       </c>
       <c r="I48" t="str">
-        <v>Митинская улица, д. 55</v>
+        <v>г. Щелково, Пушкина, д. 3</v>
       </c>
       <c r="J48" t="str">
-        <v/>
-      </c>
-      <c r="K48" t="str">
-        <v>Пятницкое шоссе, д. 15, к. 1</v>
-      </c>
-      <c r="L48" t="str">
         <v/>
       </c>
     </row>
@@ -2062,34 +2152,34 @@
         <v>Проект А</v>
       </c>
       <c r="B49" t="str">
-        <v>Ашуров Рахмуддин</v>
+        <v>Магамедов Мурад Р</v>
       </c>
       <c r="C49" t="str">
-        <v>в135ук33</v>
+        <v>К056НЕ799</v>
       </c>
       <c r="D49">
         <v>4</v>
       </c>
       <c r="E49" t="str">
-        <v>Снежная улица, д. 27, к. 1</v>
+        <v>Большая Марфинская улица, д. 4, к. 1</v>
       </c>
       <c r="F49" t="str">
         <v/>
       </c>
       <c r="G49" t="str">
-        <v>проезд Дежнёва, д. 29, к. 1</v>
+        <v>Огородный проезд, д. 10</v>
       </c>
       <c r="H49" t="str">
         <v/>
       </c>
       <c r="I49" t="str">
-        <v>Ясный пр, д. 16</v>
+        <v>Шереметьевская улица, д. 20</v>
       </c>
       <c r="J49" t="str">
         <v/>
       </c>
       <c r="K49" t="str">
-        <v>Радужная улица, д. 4, к. 1</v>
+        <v>улица Академика Королёва, д. 13, стр. 1</v>
       </c>
       <c r="L49" t="str">
         <v/>
@@ -2100,28 +2190,28 @@
         <v>Проект А</v>
       </c>
       <c r="B50" t="str">
-        <v>Бабкин Александр</v>
+        <v>Мадалиев Максат</v>
       </c>
       <c r="C50" t="str">
-        <v>Р406АЕ790</v>
+        <v>е315ку19</v>
       </c>
       <c r="D50">
         <v>3</v>
       </c>
       <c r="E50" t="str">
-        <v>г. Химки, улица Чкалова, д. 10/6</v>
+        <v>Планерная улица, д. 7</v>
       </c>
       <c r="F50" t="str">
         <v/>
       </c>
       <c r="G50" t="str">
-        <v>г. Химки, улица Кирова, д. 10, к. 2</v>
+        <v>улица Героев Панфиловцев, д. 1А, кв. 211</v>
       </c>
       <c r="H50" t="str">
         <v/>
       </c>
       <c r="I50" t="str">
-        <v>г. Химки, улица Горшина, д. 5</v>
+        <v>бульвар Яна Райниса, д. 31</v>
       </c>
       <c r="J50" t="str">
         <v/>
@@ -2132,42 +2222,30 @@
         <v>Проект А</v>
       </c>
       <c r="B51" t="str">
-        <v>Бородин Александр</v>
+        <v>Максат Азамат</v>
       </c>
       <c r="C51" t="str">
-        <v>О519КО</v>
+        <v>К220ко77</v>
       </c>
       <c r="D51">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E51" t="str">
-        <v>г. Видное, Олимпийская улица, д. 1, к. 2</v>
+        <v>бульвар Академика Ландау, д. 3</v>
       </c>
       <c r="F51" t="str">
         <v/>
       </c>
       <c r="G51" t="str">
-        <v>г. Видное, Советская улица, д. вл10/1</v>
+        <v>г. Долгопрудный, Московское шоссе, д. 37, к. А</v>
       </c>
       <c r="H51" t="str">
         <v/>
       </c>
       <c r="I51" t="str">
-        <v>г. Видное, Берёзовая улица, д. 11</v>
+        <v>г. Долгопрудный, Московское шоссе, д. 27, к. Б</v>
       </c>
       <c r="J51" t="str">
-        <v/>
-      </c>
-      <c r="K51" t="str">
-        <v>г. Видное, Ольховая улица, д. 9</v>
-      </c>
-      <c r="L51" t="str">
-        <v/>
-      </c>
-      <c r="M51" t="str">
-        <v>г. Видное, проспект Ленинского Комсомола, д. 9, к. 3</v>
-      </c>
-      <c r="N51" t="str">
         <v/>
       </c>
     </row>
@@ -2176,34 +2254,34 @@
         <v>Проект А</v>
       </c>
       <c r="B52" t="str">
-        <v>Дубанакулов Адылбек</v>
+        <v>Максат Бакытбек</v>
       </c>
       <c r="C52" t="str">
-        <v>С746НА790</v>
+        <v>А060УА69</v>
       </c>
       <c r="D52">
         <v>4</v>
       </c>
       <c r="E52" t="str">
-        <v>Семеновский пер., д. 18</v>
+        <v>Нижегородская улица, д. 71</v>
       </c>
       <c r="F52" t="str">
         <v/>
       </c>
       <c r="G52" t="str">
-        <v>Щербаковская улица, д. 20</v>
+        <v>шоссе Энтузиастов, д. 10/2</v>
       </c>
       <c r="H52" t="str">
         <v/>
       </c>
       <c r="I52" t="str">
-        <v>Открытое шоссе, д. 24, к. 11</v>
+        <v>Перовское шоссе, д. 16/2</v>
       </c>
       <c r="J52" t="str">
         <v/>
       </c>
       <c r="K52" t="str">
-        <v>Амурская улица, д. 19</v>
+        <v>Красноказарменная улица, д. 14А, к. 2</v>
       </c>
       <c r="L52" t="str">
         <v/>
@@ -2214,28 +2292,28 @@
         <v>Проект А</v>
       </c>
       <c r="B53" t="str">
-        <v>Дубанакулов Бактилек</v>
+        <v>Мамытов Усон</v>
       </c>
       <c r="C53" t="str">
-        <v>Х938КМ37</v>
+        <v>в402но790</v>
       </c>
       <c r="D53">
         <v>3</v>
       </c>
       <c r="E53" t="str">
-        <v>г. Химки, улица имени К.И. Вороницына, д. 1, к. 1</v>
+        <v>г. деревня Путилково, Новотушинская улица, д. 2</v>
       </c>
       <c r="F53" t="str">
         <v/>
       </c>
       <c r="G53" t="str">
-        <v>г. Химки, Транспортный проезд, д. 3</v>
+        <v>Митинская улица, д. 55</v>
       </c>
       <c r="H53" t="str">
         <v/>
       </c>
       <c r="I53" t="str">
-        <v>г. Химки, Пролетарская, д. 15, к. 18</v>
+        <v>Митинская улица, д. 27</v>
       </c>
       <c r="J53" t="str">
         <v/>
@@ -2246,24 +2324,30 @@
         <v>Проект А</v>
       </c>
       <c r="B54" t="str">
-        <v>Исаков Гулмырза</v>
+        <v>Мирзакулов Талантбек</v>
       </c>
       <c r="C54" t="str">
-        <v>Т754ММ142</v>
+        <v>В549ТР62</v>
       </c>
       <c r="D54">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E54" t="str">
-        <v>г. Щёлково, улица Радиоцентра № 5, д. 16</v>
+        <v>г. Одинцово, Кутузовская улица, д. 72Б</v>
       </c>
       <c r="F54" t="str">
         <v/>
       </c>
       <c r="G54" t="str">
-        <v>г. Лосино-Петровский, улица Гоголя, д. 21</v>
+        <v>г. Одинцово, улица Чистяковой, д. 67</v>
       </c>
       <c r="H54" t="str">
+        <v/>
+      </c>
+      <c r="I54" t="str">
+        <v>г. Одинцово, улица Чикина, д. 8А, к. А</v>
+      </c>
+      <c r="J54" t="str">
         <v/>
       </c>
     </row>
@@ -2272,24 +2356,18 @@
         <v>Проект А</v>
       </c>
       <c r="B55" t="str">
-        <v>Кандаров Азиз</v>
+        <v>Набиев Далер</v>
       </c>
       <c r="C55" t="str">
-        <v>К331ТХ750</v>
+        <v>О295хм77</v>
       </c>
       <c r="D55">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E55" t="str">
-        <v>улица Габричевского, д. 10, к. 1</v>
+        <v>г. Дедовск, 1-ая Главная, д. 1</v>
       </c>
       <c r="F55" t="str">
-        <v/>
-      </c>
-      <c r="G55" t="str">
-        <v>улица Маршала Катукова, д. 3, к. 1</v>
-      </c>
-      <c r="H55" t="str">
         <v/>
       </c>
     </row>
@@ -2298,36 +2376,42 @@
         <v>Проект А</v>
       </c>
       <c r="B56" t="str">
-        <v>Магамедов Мурад Р</v>
+        <v>Нарынбеков Дастан</v>
       </c>
       <c r="C56" t="str">
-        <v>К056НЕ799</v>
+        <v>у820вх797</v>
       </c>
       <c r="D56">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E56" t="str">
-        <v>Большая Тульская улица, д. 13</v>
+        <v>г. Люберцы, 1-й Панковский проезд, д. 27</v>
       </c>
       <c r="F56" t="str">
         <v/>
       </c>
       <c r="G56" t="str">
-        <v>2-й Донской проезд, д. 10, стр. 2</v>
+        <v>г. Люберцы, Проспек Победы, д. 6, кв. 019</v>
       </c>
       <c r="H56" t="str">
         <v/>
       </c>
       <c r="I56" t="str">
-        <v>улица Серпуховский Вал, д. 17, к. 1</v>
+        <v>г. Люберцы, проспект Гагарина, д. 28/1</v>
       </c>
       <c r="J56" t="str">
         <v/>
       </c>
       <c r="K56" t="str">
-        <v>Севастопольский проспект, д. 11Е</v>
+        <v>г. Люберцы, Комсомольский проспект, д. 7/1</v>
       </c>
       <c r="L56" t="str">
+        <v/>
+      </c>
+      <c r="M56" t="str">
+        <v>г. Люберцы, Смирновская улица, д. 21, к. 2</v>
+      </c>
+      <c r="N56" t="str">
         <v/>
       </c>
     </row>
@@ -2336,24 +2420,30 @@
         <v>Проект А</v>
       </c>
       <c r="B57" t="str">
-        <v>Мадалиев Максат</v>
+        <v>Нематжанов Миразиз</v>
       </c>
       <c r="C57" t="str">
-        <v>е315ку19</v>
+        <v>а314тм62</v>
       </c>
       <c r="D57">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E57" t="str">
-        <v>г. Одинцово, Белорусская улица, д. 5</v>
+        <v>Дорогобужская улица, д. 3</v>
       </c>
       <c r="F57" t="str">
         <v/>
       </c>
       <c r="G57" t="str">
-        <v>г. Лесной Городок, Фасадная, д. 2, к. 1</v>
+        <v>Ярцевская улица, д. 19</v>
       </c>
       <c r="H57" t="str">
+        <v/>
+      </c>
+      <c r="I57" t="str">
+        <v>улица Толбухина, д. 13, к. 1</v>
+      </c>
+      <c r="J57" t="str">
         <v/>
       </c>
     </row>
@@ -2362,36 +2452,30 @@
         <v>Проект А</v>
       </c>
       <c r="B58" t="str">
-        <v>Максат Азамат</v>
+        <v>Омошев Бекмырза</v>
       </c>
       <c r="C58" t="str">
-        <v>К220ко77</v>
+        <v>Х011ЕС37</v>
       </c>
       <c r="D58">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E58" t="str">
-        <v>г. Мытищи, улица Колпакова, д. 10</v>
+        <v>улица Полины Осипенко, д. 8</v>
       </c>
       <c r="F58" t="str">
         <v/>
       </c>
       <c r="G58" t="str">
-        <v>г. Мытищи, Борисовка, д. 20А</v>
+        <v>Звенигородское шоссе, д. 4</v>
       </c>
       <c r="H58" t="str">
         <v/>
       </c>
       <c r="I58" t="str">
-        <v>г. Мытищи, Лётная улица, д. 27А</v>
+        <v>Ленинградский проспект, д. 5, стр. 7</v>
       </c>
       <c r="J58" t="str">
-        <v/>
-      </c>
-      <c r="K58" t="str">
-        <v>г. Мытищи, Новомытищинский проспект, д. 17</v>
-      </c>
-      <c r="L58" t="str">
         <v/>
       </c>
     </row>
@@ -2400,34 +2484,34 @@
         <v>Проект А</v>
       </c>
       <c r="B59" t="str">
-        <v>Максат Бакытбек</v>
+        <v>Омошев Замир</v>
       </c>
       <c r="C59" t="str">
-        <v>А060УА69</v>
+        <v>о122нт790</v>
       </c>
       <c r="D59">
         <v>4</v>
       </c>
       <c r="E59" t="str">
-        <v>Новокузнецкая улица, д. 13, стр. 1</v>
+        <v>г. Королёв, Пионерская улица, д. 30, к. 9</v>
       </c>
       <c r="F59" t="str">
         <v/>
       </c>
       <c r="G59" t="str">
-        <v>2-й Грайвороновский проезд, д. 44, к. 1</v>
+        <v>г. Королёв, проезд Макаренко, д. 1</v>
       </c>
       <c r="H59" t="str">
         <v/>
       </c>
       <c r="I59" t="str">
-        <v>Зарайская улица, д. 26</v>
+        <v>г. Королёв, проспект Космонавтов, д. 34Б, к. Б</v>
       </c>
       <c r="J59" t="str">
         <v/>
       </c>
       <c r="K59" t="str">
-        <v>улица Михайлова, д. 31А</v>
+        <v>г. Королёв, улица 50-летия ВЛКСМ, д. 6, к. Е</v>
       </c>
       <c r="L59" t="str">
         <v/>
@@ -2438,24 +2522,30 @@
         <v>Проект А</v>
       </c>
       <c r="B60" t="str">
-        <v>Мамытов Усон</v>
+        <v>Райев Жаныбек</v>
       </c>
       <c r="C60" t="str">
-        <v>в402но790</v>
+        <v>Р394ММ40</v>
       </c>
       <c r="D60">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E60" t="str">
-        <v>г. Солнечногорск, Обуховская улица, д. 50Б</v>
+        <v>Соболевский проезд, д. 22, стр. 1</v>
       </c>
       <c r="F60" t="str">
         <v/>
       </c>
       <c r="G60" t="str">
-        <v>г. деревня Голубое, Тверецкий проезд, д. 16, к. 3</v>
+        <v>Старопетровский проезд, д. 1, стр. 2</v>
       </c>
       <c r="H60" t="str">
+        <v/>
+      </c>
+      <c r="I60" t="str">
+        <v>Ленинградское шоссе, д. 13, к. 1</v>
+      </c>
+      <c r="J60" t="str">
         <v/>
       </c>
     </row>
@@ -2464,24 +2554,42 @@
         <v>Проект А</v>
       </c>
       <c r="B61" t="str">
-        <v>Мирзакулов Талантбек</v>
+        <v xml:space="preserve">Рамазанов Ибрагим </v>
       </c>
       <c r="C61" t="str">
-        <v>В549ТР62</v>
+        <v>р034кт05</v>
       </c>
       <c r="D61">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E61" t="str">
-        <v>Таллинская улица, д. 16, к. 1</v>
+        <v>Братеевская улица, д. 16, к. 6</v>
       </c>
       <c r="F61" t="str">
         <v/>
       </c>
       <c r="G61" t="str">
-        <v>Маршала Катукова, д. 24, к. 4</v>
+        <v>Паромная улица, д. 9, к. 1</v>
       </c>
       <c r="H61" t="str">
+        <v/>
+      </c>
+      <c r="I61" t="str">
+        <v>улица Борисовские Пруды, д. 5, к. 1</v>
+      </c>
+      <c r="J61" t="str">
+        <v/>
+      </c>
+      <c r="K61" t="str">
+        <v>улица Борисовские Пруды, д. 8А</v>
+      </c>
+      <c r="L61" t="str">
+        <v/>
+      </c>
+      <c r="M61" t="str">
+        <v>улица Борисовские Пруды, д. 14, к. 3</v>
+      </c>
+      <c r="N61" t="str">
         <v/>
       </c>
     </row>
@@ -2490,36 +2598,30 @@
         <v>Проект А</v>
       </c>
       <c r="B62" t="str">
-        <v>Нарынбеков Дастан</v>
+        <v>Сагындыков Бекназар</v>
       </c>
       <c r="C62" t="str">
-        <v>у820вх797</v>
+        <v>К417НК790</v>
       </c>
       <c r="D62">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E62" t="str">
-        <v>Звенигородское шоссе, д. 4</v>
+        <v>улица Маршала Тухачевского, д. 50, к. 2</v>
       </c>
       <c r="F62" t="str">
         <v/>
       </c>
       <c r="G62" t="str">
-        <v>улица Маршала Тухачевского, д. 50, к. 2</v>
+        <v>проспект Маршала Жукова, д. 49</v>
       </c>
       <c r="H62" t="str">
         <v/>
       </c>
       <c r="I62" t="str">
-        <v>проспект Маршала Жукова, д. 49</v>
+        <v>улица Мнёвники, д. 23</v>
       </c>
       <c r="J62" t="str">
-        <v/>
-      </c>
-      <c r="K62" t="str">
-        <v>улица Мнёвники, д. 23</v>
-      </c>
-      <c r="L62" t="str">
         <v/>
       </c>
     </row>
@@ -2528,30 +2630,24 @@
         <v>Проект А</v>
       </c>
       <c r="B63" t="str">
-        <v>Омошев Бекмырза</v>
+        <v>Солтанов  Эмиль</v>
       </c>
       <c r="C63" t="str">
-        <v>Х011ЕС37</v>
+        <v>А602КМ797</v>
       </c>
       <c r="D63">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E63" t="str">
-        <v>Дорогобужская улица, д. 3</v>
+        <v>г. Зеленоград, Центральный проспект, д. -, к. 438</v>
       </c>
       <c r="F63" t="str">
         <v/>
       </c>
       <c r="G63" t="str">
-        <v>Ярцевская улица, д. 19</v>
+        <v>г. Зеленоград, улица Панфилова, д. 28Б</v>
       </c>
       <c r="H63" t="str">
-        <v/>
-      </c>
-      <c r="I63" t="str">
-        <v>улица Толбухина, д. 13, к. 1</v>
-      </c>
-      <c r="J63" t="str">
         <v/>
       </c>
     </row>
@@ -2560,40 +2656,40 @@
         <v>Проект А</v>
       </c>
       <c r="B64" t="str">
-        <v>Омошев Замир</v>
+        <v>Сулейманов Ибаят</v>
       </c>
       <c r="C64" t="str">
-        <v>о122нт790</v>
+        <v>А320ТР62</v>
       </c>
       <c r="D64">
         <v>5</v>
       </c>
       <c r="E64" t="str">
-        <v>Каширское шоссе, д. 65, к. 3</v>
+        <v>г. Балашиха, шоссе Энтузиастов, д. вл1Алит6В</v>
       </c>
       <c r="F64" t="str">
         <v/>
       </c>
       <c r="G64" t="str">
-        <v>Каширское шоссе (дублёр), д. 61, к. 3А</v>
+        <v>шоссе Энтузиастов, д. 55</v>
       </c>
       <c r="H64" t="str">
         <v/>
       </c>
       <c r="I64" t="str">
-        <v>улица Генерала Белова, д. 43, к. 2</v>
+        <v>Хабаровская улица, д. 4, к. 1</v>
       </c>
       <c r="J64" t="str">
         <v/>
       </c>
       <c r="K64" t="str">
-        <v>Гурьевский проезд, д. 17, к. 1</v>
+        <v>Байкальская улица, д. 37</v>
       </c>
       <c r="L64" t="str">
         <v/>
       </c>
       <c r="M64" t="str">
-        <v>Ясеневая улица, д. 29</v>
+        <v>Щёлковское шоссе, д. 79, к. 1</v>
       </c>
       <c r="N64" t="str">
         <v/>
@@ -2604,42 +2700,36 @@
         <v>Проект А</v>
       </c>
       <c r="B65" t="str">
-        <v>Райев Жаныбек</v>
+        <v>Токтогулов Асан</v>
       </c>
       <c r="C65" t="str">
-        <v>Р394ММ40</v>
+        <v>а638тр62</v>
       </c>
       <c r="D65">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E65" t="str">
-        <v>г. Люберцы, Московская улица, д. 11</v>
+        <v>г. Лыткарино, Советская, д. 8, к. 2</v>
       </c>
       <c r="F65" t="str">
         <v/>
       </c>
       <c r="G65" t="str">
-        <v>г. Люберцы, Новорязанское шоссе, д. 1А</v>
+        <v>г. рабочий посёлок Октябрьский, улица Ленина, д. 25</v>
       </c>
       <c r="H65" t="str">
         <v/>
       </c>
       <c r="I65" t="str">
-        <v>Жулебинский бульвар, д. 30, к. 1</v>
+        <v>г. Жуковский, Молодёжная улица, д. 21, к. А</v>
       </c>
       <c r="J65" t="str">
         <v/>
       </c>
       <c r="K65" t="str">
-        <v>г. Люберцы, улица Кирова, д. 9, к. 5</v>
+        <v>г. рабочий посёлок Октябрьский, микрорайон Восточный, д. 1</v>
       </c>
       <c r="L65" t="str">
-        <v/>
-      </c>
-      <c r="M65" t="str">
-        <v>г. Люберцы, Комсомольский проспект, д. 7/1</v>
-      </c>
-      <c r="N65" t="str">
         <v/>
       </c>
     </row>
@@ -2648,42 +2738,30 @@
         <v>Проект А</v>
       </c>
       <c r="B66" t="str">
-        <v xml:space="preserve">Рамазанов Ибрагим </v>
+        <v>Турсуналиев Женишбек</v>
       </c>
       <c r="C66" t="str">
-        <v>р034кт05</v>
+        <v>Т440ЕК138</v>
       </c>
       <c r="D66">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E66" t="str">
-        <v>Донецкая улица, д. 34, к. 1</v>
+        <v>4-й Вятский переулок, д. 18, к. 2</v>
       </c>
       <c r="F66" t="str">
         <v/>
       </c>
       <c r="G66" t="str">
-        <v>улица Перерва, д. 32</v>
+        <v>улица Дубки, д. 4А</v>
       </c>
       <c r="H66" t="str">
         <v/>
       </c>
       <c r="I66" t="str">
-        <v>Люблинская улица, д. 102А</v>
+        <v>улица 8 Марта, д. 6</v>
       </c>
       <c r="J66" t="str">
-        <v/>
-      </c>
-      <c r="K66" t="str">
-        <v>Братеевская улица, д. 16, к. 6</v>
-      </c>
-      <c r="L66" t="str">
-        <v/>
-      </c>
-      <c r="M66" t="str">
-        <v>Паромная улица, д. 9, к. 1</v>
-      </c>
-      <c r="N66" t="str">
         <v/>
       </c>
     </row>
@@ -2692,36 +2770,24 @@
         <v>Проект А</v>
       </c>
       <c r="B67" t="str">
-        <v>Сагындыков Бекназар</v>
+        <v xml:space="preserve">Умаралиев  Мухамед </v>
       </c>
       <c r="C67" t="str">
-        <v>К417НК790</v>
+        <v>с851ак777</v>
       </c>
       <c r="D67">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E67" t="str">
-        <v>бульвар Яна Райниса, д. 31</v>
+        <v>г. Дмитров, Советская улица, д. 5</v>
       </c>
       <c r="F67" t="str">
         <v/>
       </c>
       <c r="G67" t="str">
-        <v>улица Героев Панфиловцев, д. 1А, кв. 211</v>
+        <v>г. Дмитров, Профессиональная улица, д. 22, к. 1</v>
       </c>
       <c r="H67" t="str">
-        <v/>
-      </c>
-      <c r="I67" t="str">
-        <v>Планерная улица, д. 7</v>
-      </c>
-      <c r="J67" t="str">
-        <v/>
-      </c>
-      <c r="K67" t="str">
-        <v>г. деревня Путилково, Новотушинская улица, д. 2</v>
-      </c>
-      <c r="L67" t="str">
         <v/>
       </c>
     </row>
@@ -2730,34 +2796,34 @@
         <v>Проект А</v>
       </c>
       <c r="B68" t="str">
-        <v>Солтанов  Эмиль</v>
+        <v>Хапизов Алтынбек</v>
       </c>
       <c r="C68" t="str">
-        <v>А602КМ797</v>
+        <v>У362УТ71</v>
       </c>
       <c r="D68">
         <v>4</v>
       </c>
       <c r="E68" t="str">
-        <v>улица Маршала Савицкого, д. 18, к. 2</v>
+        <v>г. Люберцы, улица Камова, д. 11/5</v>
       </c>
       <c r="F68" t="str">
         <v/>
       </c>
       <c r="G68" t="str">
-        <v>г. Подольск, Ленина, д. 14</v>
+        <v>г. Балашиха, улица Ленина, д. 1/5, к. 5</v>
       </c>
       <c r="H68" t="str">
         <v/>
       </c>
       <c r="I68" t="str">
-        <v>г. Подольск, Подольская улица, д. 10А</v>
+        <v>г. микрорайон Железнодорожный, Балашиха, Андрея Белого, д. 1</v>
       </c>
       <c r="J68" t="str">
         <v/>
       </c>
       <c r="K68" t="str">
-        <v>г. Подольск, Быковская улица, д. 10</v>
+        <v>г. Балашиха, Речная, д. 5</v>
       </c>
       <c r="L68" t="str">
         <v/>
@@ -2768,30 +2834,42 @@
         <v>Проект А</v>
       </c>
       <c r="B69" t="str">
-        <v>Сулейманов Ибаят</v>
+        <v>Чолпонбек Асан</v>
       </c>
       <c r="C69" t="str">
-        <v>А320ТР62</v>
+        <v>в877ме77</v>
       </c>
       <c r="D69">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E69" t="str">
-        <v>улица 8 Марта, д. 6</v>
+        <v>Суздальская улица, д. 12А</v>
       </c>
       <c r="F69" t="str">
         <v/>
       </c>
       <c r="G69" t="str">
-        <v>4-й Вятский переулок, д. 18, к. 2</v>
+        <v>г. Реутов, улица имени Академика В.Н. Челомея, д. 12</v>
       </c>
       <c r="H69" t="str">
         <v/>
       </c>
       <c r="I69" t="str">
-        <v>Тихвинская улица, д. 20</v>
+        <v>г. Реутов, Юбилейный проспект, д. 72</v>
       </c>
       <c r="J69" t="str">
+        <v/>
+      </c>
+      <c r="K69" t="str">
+        <v>г. Реутов, улица Октября, д. вл10</v>
+      </c>
+      <c r="L69" t="str">
+        <v/>
+      </c>
+      <c r="M69" t="str">
+        <v>г. Реутов, Комсомольская улица, д. 21, к. 1</v>
+      </c>
+      <c r="N69" t="str">
         <v/>
       </c>
     </row>
@@ -2800,30 +2878,42 @@
         <v>Проект А</v>
       </c>
       <c r="B70" t="str">
-        <v>Токтогулов Асан</v>
+        <v>Чыйбылов Сталбек</v>
       </c>
       <c r="C70" t="str">
-        <v>а638тр62</v>
+        <v>с495оа89</v>
       </c>
       <c r="D70">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E70" t="str">
-        <v>1-й Очаковский переулок, д. 1</v>
+        <v>улица Мусы Джалиля, д. 27, стр. 2, к. 2</v>
       </c>
       <c r="F70" t="str">
         <v/>
       </c>
       <c r="G70" t="str">
-        <v>улица Наташи Ковшовой, д. 8А, стр. А</v>
+        <v>Гурьевский проезд, д. 17, к. 1</v>
       </c>
       <c r="H70" t="str">
         <v/>
       </c>
       <c r="I70" t="str">
-        <v>Озёрная улица, д. 42</v>
+        <v>улица Генерала Белова, д. 43, к. 2</v>
       </c>
       <c r="J70" t="str">
+        <v/>
+      </c>
+      <c r="K70" t="str">
+        <v>Каширское шоссе (дублёр), д. 61, к. 3А</v>
+      </c>
+      <c r="L70" t="str">
+        <v/>
+      </c>
+      <c r="M70" t="str">
+        <v>Каширское шоссе, д. 80</v>
+      </c>
+      <c r="N70" t="str">
         <v/>
       </c>
     </row>
@@ -2832,92 +2922,110 @@
         <v>Проект А</v>
       </c>
       <c r="B71" t="str">
-        <v xml:space="preserve">Умаралиев  Мухамед </v>
+        <v>Юсупов Файзулло</v>
       </c>
       <c r="C71" t="str">
-        <v>с851ак777</v>
+        <v>О401УЕ40</v>
       </c>
       <c r="D71">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E71" t="str">
-        <v>г. Балашиха, улица Ленина, д. 1/5, к. 5</v>
+        <v>г. Мытищи, Коммунистическая улица, д. 1</v>
       </c>
       <c r="F71" t="str">
         <v/>
       </c>
       <c r="G71" t="str">
-        <v>г. микрорайон Железнодорожный, Балашиха, Андрея Белого, д. 1</v>
+        <v>г. Мытищи, Олимпийский проспект, д. 36, к. 3</v>
       </c>
       <c r="H71" t="str">
         <v/>
       </c>
       <c r="I71" t="str">
-        <v>г. Балашиха, Речная, д. 5</v>
+        <v>г. Мытищи, Олимпийский проспект, д. вл13с1, стр. 1, к. Б</v>
       </c>
       <c r="J71" t="str">
+        <v/>
+      </c>
+      <c r="K71" t="str">
+        <v>г. Мытищи, Вокзальная площадь, д. 2</v>
+      </c>
+      <c r="L71" t="str">
         <v/>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="str">
-        <v>Проект А</v>
+        <v>СТРИТ ЛОГИСТИК</v>
       </c>
       <c r="B72" t="str">
-        <v>Хапизов Алтынбек</v>
+        <v>Бакланов Сергей</v>
       </c>
       <c r="C72" t="str">
-        <v>У362УТ71</v>
+        <v>В979ЕХ979</v>
       </c>
       <c r="D72">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E72" t="str">
-        <v>бульвар Академика Ландау, д. 3</v>
+        <v>г. Видное, Олимпийская улица, д. 1, к. 2</v>
       </c>
       <c r="F72" t="str">
         <v/>
       </c>
       <c r="G72" t="str">
-        <v>улица Конёнкова, д. 23</v>
+        <v>г. Видное, Советская улица, д. вл10/1</v>
       </c>
       <c r="H72" t="str">
         <v/>
       </c>
       <c r="I72" t="str">
-        <v>Широкая улица, д. 7, к. 2</v>
+        <v>г. Видное, Берёзовая улица, д. 11</v>
       </c>
       <c r="J72" t="str">
+        <v/>
+      </c>
+      <c r="K72" t="str">
+        <v>г. Видное, Ольховая улица, д. 9</v>
+      </c>
+      <c r="L72" t="str">
+        <v/>
+      </c>
+      <c r="M72" t="str">
+        <v>г. Видное, проспект Ленинского Комсомола, д. 9, к. 3</v>
+      </c>
+      <c r="N72" t="str">
         <v/>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="str">
-        <v>Проект А</v>
+        <v>СТРИТ ЛОГИСТИК</v>
       </c>
       <c r="B73" t="str">
-        <v>Чолпонбек Асан</v>
+        <v>Билялов Ринат</v>
       </c>
       <c r="C73" t="str">
-        <v>в877ме77</v>
+        <v>Х475уу152</v>
       </c>
       <c r="D73">
         <v>3</v>
       </c>
       <c r="E73" t="str">
-        <v>3-й Сетуньский проезд, д. 16</v>
+        <v>г. Химки, Молодёжная улица, д. 15Б, к. Б</v>
       </c>
       <c r="F73" t="str">
         <v/>
       </c>
       <c r="G73" t="str">
-        <v>Мосфильмовская улица, д. 27</v>
+        <v>г. Химки, Молодёжная улица, д. 52</v>
       </c>
       <c r="H73" t="str">
         <v/>
       </c>
       <c r="I73" t="str">
-        <v>Ленинский проспект, д. 44</v>
+        <v>Соколово-Мещерская улица, д. 25</v>
       </c>
       <c r="J73" t="str">
         <v/>
@@ -2925,39 +3033,21 @@
     </row>
     <row r="74">
       <c r="A74" t="str">
-        <v>Проект А</v>
+        <v>СТРИТ ЛОГИСТИК</v>
       </c>
       <c r="B74" t="str">
-        <v>Чыйбылов Сталбек</v>
+        <v>Богачев Виталий</v>
       </c>
       <c r="C74" t="str">
-        <v>с495оа89</v>
+        <v>М046ЕТ790</v>
       </c>
       <c r="D74">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E74" t="str">
-        <v>г. Реутов, Комсомольская улица, д. 21, к. 1</v>
+        <v>г. Солнечногорск, Обуховская улица, д. 50Б</v>
       </c>
       <c r="F74" t="str">
-        <v/>
-      </c>
-      <c r="G74" t="str">
-        <v>г. Балашиха, улица Некрасова, д. 13А</v>
-      </c>
-      <c r="H74" t="str">
-        <v/>
-      </c>
-      <c r="I74" t="str">
-        <v>г. Старая Купавна, Октябрьская улица, д. 19</v>
-      </c>
-      <c r="J74" t="str">
-        <v/>
-      </c>
-      <c r="K74" t="str">
-        <v>г. Балашиха, шоссе Энтузиастов, д. вл1Алит6В</v>
-      </c>
-      <c r="L74" t="str">
         <v/>
       </c>
     </row>
@@ -2966,36 +3056,42 @@
         <v>СТРИТ ЛОГИСТИК</v>
       </c>
       <c r="B75" t="str">
-        <v>Бакланов Сергей</v>
+        <v>Галимов Динар</v>
       </c>
       <c r="C75" t="str">
-        <v>В979ЕХ979</v>
+        <v>Е099КН702</v>
       </c>
       <c r="D75">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E75" t="str">
-        <v>Волгоградский проспект, д. 32, к. 2</v>
+        <v>Братиславская улица, д. 16, к. 1</v>
       </c>
       <c r="F75" t="str">
         <v/>
       </c>
       <c r="G75" t="str">
-        <v>улица Мастеркова, д. 6</v>
+        <v>Донецкая улица, д. 34, к. 1</v>
       </c>
       <c r="H75" t="str">
         <v/>
       </c>
       <c r="I75" t="str">
-        <v>5-я Кожуховская улица, д. 9</v>
+        <v>Люблинская улица, д. 102А</v>
       </c>
       <c r="J75" t="str">
         <v/>
       </c>
       <c r="K75" t="str">
-        <v>улица Гурьянова, д. 30</v>
+        <v>улица Перерва, д. 32</v>
       </c>
       <c r="L75" t="str">
+        <v/>
+      </c>
+      <c r="M75" t="str">
+        <v>улица Перерва, д. 45</v>
+      </c>
+      <c r="N75" t="str">
         <v/>
       </c>
     </row>
@@ -3004,34 +3100,34 @@
         <v>СТРИТ ЛОГИСТИК</v>
       </c>
       <c r="B76" t="str">
-        <v>Баткаев Равиль</v>
+        <v>Егоров Илья</v>
       </c>
       <c r="C76" t="str">
-        <v>Р415ВУ190</v>
+        <v>Р399АВ99</v>
       </c>
       <c r="D76">
         <v>4</v>
       </c>
       <c r="E76" t="str">
-        <v>Ярославское шоссе, д. 124</v>
+        <v>улица Кравченко, д. 11</v>
       </c>
       <c r="F76" t="str">
         <v/>
       </c>
       <c r="G76" t="str">
-        <v>г. Мытищи, улица Семашко, д. 25</v>
+        <v>улица Марии Ульяновой, д. 9, к. 3</v>
       </c>
       <c r="H76" t="str">
         <v/>
       </c>
       <c r="I76" t="str">
-        <v>г. Мытищи, Олимпийский проспект, д. вл13с1, стр. 1, к. Б</v>
+        <v>площадь Джавахарлала Неру, д. 1</v>
       </c>
       <c r="J76" t="str">
         <v/>
       </c>
       <c r="K76" t="str">
-        <v>г. Мытищи, Вокзальная площадь, д. 2</v>
+        <v>улица Вавилова, д. 66</v>
       </c>
       <c r="L76" t="str">
         <v/>
@@ -3042,30 +3138,36 @@
         <v>СТРИТ ЛОГИСТИК</v>
       </c>
       <c r="B77" t="str">
-        <v>Билялов Ринат</v>
+        <v>Заднев Евгений</v>
       </c>
       <c r="C77" t="str">
-        <v>Х475уу152</v>
+        <v>к803ее163</v>
       </c>
       <c r="D77">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E77" t="str">
-        <v>Правобережная улица, д. 1Б</v>
+        <v>Профсоюзная улица, д. 103А</v>
       </c>
       <c r="F77" t="str">
         <v/>
       </c>
       <c r="G77" t="str">
-        <v>г. Долгопрудный, Лихачёвское шоссе, д. 6</v>
+        <v>Профсоюзная улица, д. 102А</v>
       </c>
       <c r="H77" t="str">
         <v/>
       </c>
       <c r="I77" t="str">
-        <v>г. Химки, Совхозная улица, д. 13</v>
+        <v>Профсоюзная улица, д. 61А</v>
       </c>
       <c r="J77" t="str">
+        <v/>
+      </c>
+      <c r="K77" t="str">
+        <v>Перекопская улица, д. 34, к. 3</v>
+      </c>
+      <c r="L77" t="str">
         <v/>
       </c>
     </row>
@@ -3074,36 +3176,30 @@
         <v>СТРИТ ЛОГИСТИК</v>
       </c>
       <c r="B78" t="str">
-        <v>Богачев Виталий</v>
+        <v>Зверев Андрей</v>
       </c>
       <c r="C78" t="str">
-        <v>М046ЕТ790</v>
+        <v>С722ВН797</v>
       </c>
       <c r="D78">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E78" t="str">
-        <v>Чонгарский бульвар, д. 26А, к. 3</v>
+        <v>Волоколамское шоссе, д. 1, стр. 1</v>
       </c>
       <c r="F78" t="str">
         <v/>
       </c>
       <c r="G78" t="str">
-        <v>Варшавское шоссе, д. 86А</v>
+        <v>Волоколамское шоссе, д. 15/22, кв. 1</v>
       </c>
       <c r="H78" t="str">
         <v/>
       </c>
       <c r="I78" t="str">
-        <v>Сумской проезд, д. 8, к. 1</v>
+        <v>Самеда Вургуна, д. 11</v>
       </c>
       <c r="J78" t="str">
-        <v/>
-      </c>
-      <c r="K78" t="str">
-        <v>Варшавское шоссе, д. 97</v>
-      </c>
-      <c r="L78" t="str">
         <v/>
       </c>
     </row>
@@ -3112,30 +3208,36 @@
         <v>СТРИТ ЛОГИСТИК</v>
       </c>
       <c r="B79" t="str">
-        <v>Галимов Динар</v>
+        <v>Ивочкин Сергей</v>
       </c>
       <c r="C79" t="str">
-        <v>Е099КН702</v>
+        <v>A811AE790</v>
       </c>
       <c r="D79">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E79" t="str">
-        <v>Новопеределкинская улица, д. 13</v>
+        <v>1-й Очаковский переулок, д. 1</v>
       </c>
       <c r="F79" t="str">
         <v/>
       </c>
       <c r="G79" t="str">
-        <v>г. поселение Внуковское, улица Корнея Чуковского, д. 3</v>
+        <v>улица Наташи Ковшовой, д. 8А, стр. А</v>
       </c>
       <c r="H79" t="str">
         <v/>
       </c>
       <c r="I79" t="str">
-        <v>улица Шолохова, д. 5, к. 2</v>
+        <v>Озёрная улица, д. 42</v>
       </c>
       <c r="J79" t="str">
+        <v/>
+      </c>
+      <c r="K79" t="str">
+        <v>Боровское шоссе, д. 2А, к. 1</v>
+      </c>
+      <c r="L79" t="str">
         <v/>
       </c>
     </row>
@@ -3144,42 +3246,36 @@
         <v>СТРИТ ЛОГИСТИК</v>
       </c>
       <c r="B80" t="str">
-        <v>Евтюшкин Иван</v>
+        <v>Котляров Алексей</v>
       </c>
       <c r="C80" t="str">
-        <v>е135ус799</v>
+        <v>Р 043 КО 750</v>
       </c>
       <c r="D80">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E80" t="str">
-        <v>Измайловский проезд, д. 13</v>
+        <v>Новокузнецкая улица, д. 13, стр. 1</v>
       </c>
       <c r="F80" t="str">
         <v/>
       </c>
       <c r="G80" t="str">
-        <v>Верхняя Первомайская улица, д. 59/35, к. 3</v>
+        <v>Большая Тульская улица, д. 13</v>
       </c>
       <c r="H80" t="str">
         <v/>
       </c>
       <c r="I80" t="str">
-        <v>Щёлковское шоссе, д. 79, к. 1</v>
+        <v>2-й Донской проезд, д. 10, стр. 2</v>
       </c>
       <c r="J80" t="str">
         <v/>
       </c>
       <c r="K80" t="str">
-        <v>Байкальская улица, д. 37</v>
+        <v>улица Серпуховский Вал, д. 17, к. 1</v>
       </c>
       <c r="L80" t="str">
-        <v/>
-      </c>
-      <c r="M80" t="str">
-        <v>Хабаровская улица, д. 4, к. 1</v>
-      </c>
-      <c r="N80" t="str">
         <v/>
       </c>
     </row>
@@ -3188,42 +3284,36 @@
         <v>СТРИТ ЛОГИСТИК</v>
       </c>
       <c r="B81" t="str">
-        <v>Егоров Илья</v>
+        <v>Кузнецов Александр Васильевич</v>
       </c>
       <c r="C81" t="str">
-        <v>Р399АВ99</v>
+        <v>у823ех790</v>
       </c>
       <c r="D81">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E81" t="str">
-        <v>Краснодарская улица, д. 16</v>
+        <v>г. Домодедово, улица Корнеева, д. 1</v>
       </c>
       <c r="F81" t="str">
         <v/>
       </c>
       <c r="G81" t="str">
-        <v>улица Артюхиной, д. 24, к. 1</v>
+        <v>г. Домодедово, Южнодомодедовская улица, д. 16</v>
       </c>
       <c r="H81" t="str">
         <v/>
       </c>
       <c r="I81" t="str">
-        <v>Волжский бульвар, д. 38</v>
+        <v>г. Домодедово, Курыжова, д. 30, к. 1</v>
       </c>
       <c r="J81" t="str">
         <v/>
       </c>
       <c r="K81" t="str">
-        <v>улица Васильцовский Стан, д. 9</v>
+        <v>г. Домодедово, улица Гагарина, д. 37</v>
       </c>
       <c r="L81" t="str">
-        <v/>
-      </c>
-      <c r="M81" t="str">
-        <v>улица Юных Ленинцев, д. 52</v>
-      </c>
-      <c r="N81" t="str">
         <v/>
       </c>
     </row>
@@ -3232,34 +3322,34 @@
         <v>СТРИТ ЛОГИСТИК</v>
       </c>
       <c r="B82" t="str">
-        <v>Заднев Евгений</v>
+        <v>Кузнецов Алексей Др</v>
       </c>
       <c r="C82" t="str">
-        <v>к803ее163</v>
+        <v>Н081НМ777</v>
       </c>
       <c r="D82">
         <v>4</v>
       </c>
       <c r="E82" t="str">
-        <v>улица Академика Миллионщикова, д. 19</v>
+        <v>Большая Спасская улица, д. 8, стр. 1А</v>
       </c>
       <c r="F82" t="str">
         <v/>
       </c>
       <c r="G82" t="str">
-        <v>Нагатинская улица, д. 16</v>
+        <v>Плетешковский переулок, д. 17, стр. 1</v>
       </c>
       <c r="H82" t="str">
         <v/>
       </c>
       <c r="I82" t="str">
-        <v>проспект Андропова, д. 22</v>
+        <v>Большая Почтовая улица, д. 43-45, стр. 2</v>
       </c>
       <c r="J82" t="str">
         <v/>
       </c>
       <c r="K82" t="str">
-        <v>улица Речников, д. 14, к. 1</v>
+        <v>Сокольническая площадь, д. 9А, стр. А</v>
       </c>
       <c r="L82" t="str">
         <v/>
@@ -3270,36 +3360,30 @@
         <v>СТРИТ ЛОГИСТИК</v>
       </c>
       <c r="B83" t="str">
-        <v>Зверев Андрей</v>
+        <v>Лось Владимир</v>
       </c>
       <c r="C83" t="str">
-        <v>С722ВН797</v>
+        <v>М316НС193</v>
       </c>
       <c r="D83">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E83" t="str">
-        <v>Дмитровское шоссе, д. 165Д, к. 6</v>
+        <v>г. Раменское, Крымская улица, д. 12, стр. офис 17</v>
       </c>
       <c r="F83" t="str">
         <v/>
       </c>
       <c r="G83" t="str">
-        <v>г. Долгопрудный, Московское шоссе, д. 27, к. Б</v>
+        <v>г. Раменское, улица Михалевича, д. 5</v>
       </c>
       <c r="H83" t="str">
         <v/>
       </c>
       <c r="I83" t="str">
-        <v>г. Долгопрудный, Московское шоссе, д. 37, к. А</v>
+        <v>г. Раменское, улица Чугунова, д. 32А</v>
       </c>
       <c r="J83" t="str">
-        <v/>
-      </c>
-      <c r="K83" t="str">
-        <v>г. Долгопрудный, проспект Пацаева, д. 12</v>
-      </c>
-      <c r="L83" t="str">
         <v/>
       </c>
     </row>
@@ -3308,36 +3392,30 @@
         <v>СТРИТ ЛОГИСТИК</v>
       </c>
       <c r="B84" t="str">
-        <v>Ивочкин Сергей</v>
+        <v>Максимов Алексей</v>
       </c>
       <c r="C84" t="str">
-        <v>A811AE790</v>
+        <v>Е759вк797</v>
       </c>
       <c r="D84">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E84" t="str">
-        <v>Дубнинская, д. 3</v>
+        <v>г. Химки, Совхозная улица, д. 13</v>
       </c>
       <c r="F84" t="str">
         <v/>
       </c>
       <c r="G84" t="str">
-        <v>Селигерская, д. 18, к. 3</v>
+        <v>улица Дыбенко, д. 36, к. 4</v>
       </c>
       <c r="H84" t="str">
         <v/>
       </c>
       <c r="I84" t="str">
-        <v>Дубнинская улица, д. 53, к. 3</v>
+        <v>Правобережная улица, д. 1Б</v>
       </c>
       <c r="J84" t="str">
-        <v/>
-      </c>
-      <c r="K84" t="str">
-        <v>Дубнинская улица, д. 12Б, стр. 12</v>
-      </c>
-      <c r="L84" t="str">
         <v/>
       </c>
     </row>
@@ -3346,34 +3424,34 @@
         <v>СТРИТ ЛОГИСТИК</v>
       </c>
       <c r="B85" t="str">
-        <v>Котляров Алексей</v>
+        <v>Макухин Антон</v>
       </c>
       <c r="C85" t="str">
-        <v>Р 043 КО 750</v>
+        <v>Х871УС197</v>
       </c>
       <c r="D85">
         <v>4</v>
       </c>
       <c r="E85" t="str">
-        <v>улица Лётчика Бабушкина, д. 39</v>
+        <v>Селигерская, д. 18, к. 3</v>
       </c>
       <c r="F85" t="str">
         <v/>
       </c>
       <c r="G85" t="str">
-        <v>Минусинская улица, д. 9</v>
+        <v>Дубнинская улица, д. 53, к. 3</v>
       </c>
       <c r="H85" t="str">
         <v/>
       </c>
       <c r="I85" t="str">
-        <v>улица Коминтерна, д. 33, к. 2</v>
+        <v>Дубнинская улица, д. 12Б, стр. 12</v>
       </c>
       <c r="J85" t="str">
         <v/>
       </c>
       <c r="K85" t="str">
-        <v>Тайнинская улица, д. 9</v>
+        <v>Дубнинская, д. 3</v>
       </c>
       <c r="L85" t="str">
         <v/>
@@ -3384,36 +3462,30 @@
         <v>СТРИТ ЛОГИСТИК</v>
       </c>
       <c r="B86" t="str">
-        <v>Кузнецов Александр Васильевич</v>
+        <v>Малянов Евгений</v>
       </c>
       <c r="C86" t="str">
-        <v>у823ех790</v>
+        <v>Р583КУ177</v>
       </c>
       <c r="D86">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E86" t="str">
-        <v>г. Лыткарино, Советская, д. 8, к. 2</v>
+        <v>г. Одинцово, Союзная улица, д. 1, к. В</v>
       </c>
       <c r="F86" t="str">
         <v/>
       </c>
       <c r="G86" t="str">
-        <v>г. Жуковский, Молодёжная улица, д. 21, к. А</v>
+        <v>г. Одинцово, Белорусская улица, д. 5</v>
       </c>
       <c r="H86" t="str">
         <v/>
       </c>
       <c r="I86" t="str">
-        <v>г. Жуковский, улица Гагарина, д. 24</v>
+        <v>г. Лесной Городок, Фасадная, д. 2, к. 1</v>
       </c>
       <c r="J86" t="str">
-        <v/>
-      </c>
-      <c r="K86" t="str">
-        <v>г. Жуковский, улица Баженова, д. 4/1</v>
-      </c>
-      <c r="L86" t="str">
         <v/>
       </c>
     </row>
@@ -3422,42 +3494,36 @@
         <v>СТРИТ ЛОГИСТИК</v>
       </c>
       <c r="B87" t="str">
-        <v>Кузнецов Алексей Др</v>
+        <v>Мацюк Валентин</v>
       </c>
       <c r="C87" t="str">
-        <v>Н081НМ777</v>
+        <v>Т302вн05</v>
       </c>
       <c r="D87">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E87" t="str">
-        <v>Покровская улица, д. 17, к. 3</v>
+        <v>улица Космонавтов, д. 22</v>
       </c>
       <c r="F87" t="str">
         <v/>
       </c>
       <c r="G87" t="str">
-        <v>Рождественская улица, д. 4</v>
+        <v>проспект Мира, д. 124, к. 2</v>
       </c>
       <c r="H87" t="str">
         <v/>
       </c>
       <c r="I87" t="str">
-        <v>г. Люберцы, улица Попова, д. 34/1</v>
+        <v>Долгоруковская улица, д. 40, кв. 10</v>
       </c>
       <c r="J87" t="str">
         <v/>
       </c>
       <c r="K87" t="str">
-        <v>г. Люберцы, улица Шевлякова, д. 2/24</v>
+        <v>Тихвинская улица, д. 20</v>
       </c>
       <c r="L87" t="str">
-        <v/>
-      </c>
-      <c r="M87" t="str">
-        <v>Святоозёрская улица, д. 14</v>
-      </c>
-      <c r="N87" t="str">
         <v/>
       </c>
     </row>
@@ -3466,28 +3532,28 @@
         <v>СТРИТ ЛОГИСТИК</v>
       </c>
       <c r="B88" t="str">
-        <v>Лапшинов Павел</v>
+        <v>Метлихин Игорь</v>
       </c>
       <c r="C88" t="str">
-        <v>С364ак177</v>
+        <v>М609КТ790</v>
       </c>
       <c r="D88">
         <v>3</v>
       </c>
       <c r="E88" t="str">
-        <v>Ленинградский проспект, д. 5, стр. 7</v>
+        <v>Таллинская улица, д. 16, к. 1</v>
       </c>
       <c r="F88" t="str">
         <v/>
       </c>
       <c r="G88" t="str">
-        <v>улица Полины Осипенко, д. 8</v>
+        <v>улица Маршала Катукова, д. 3, к. 1</v>
       </c>
       <c r="H88" t="str">
         <v/>
       </c>
       <c r="I88" t="str">
-        <v>Долгоруковская улица, д. 40, кв. 10</v>
+        <v>Маршала Катукова, д. 24, к. 4</v>
       </c>
       <c r="J88" t="str">
         <v/>
@@ -3498,24 +3564,36 @@
         <v>СТРИТ ЛОГИСТИК</v>
       </c>
       <c r="B89" t="str">
-        <v>Лось Владимир</v>
+        <v>Мифтахутдинов Айрат</v>
       </c>
       <c r="C89" t="str">
-        <v>М316НС193</v>
+        <v>р987ав777</v>
       </c>
       <c r="D89">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E89" t="str">
-        <v>Волоколамское шоссе, д. 15/22, кв. 1</v>
+        <v>г. Пушкино, Московский проспект, д. 59</v>
       </c>
       <c r="F89" t="str">
         <v/>
       </c>
       <c r="G89" t="str">
-        <v>улица Маршала Бирюзова, д. 4, к. 1</v>
+        <v>г. Пушкино, Набережная улица, д. 35, к. 6</v>
       </c>
       <c r="H89" t="str">
+        <v/>
+      </c>
+      <c r="I89" t="str">
+        <v>г. Пушкино, микрорайон Серебрянка, д. 48, к. 2</v>
+      </c>
+      <c r="J89" t="str">
+        <v/>
+      </c>
+      <c r="K89" t="str">
+        <v>г. Мытищи, 2-я Институтская улица, д. 26</v>
+      </c>
+      <c r="L89" t="str">
         <v/>
       </c>
     </row>
@@ -3524,42 +3602,30 @@
         <v>СТРИТ ЛОГИСТИК</v>
       </c>
       <c r="B90" t="str">
-        <v>Макухин Антон</v>
+        <v>Мовила Александр</v>
       </c>
       <c r="C90" t="str">
-        <v>Х871УС197</v>
+        <v>р124ма40</v>
       </c>
       <c r="D90">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E90" t="str">
-        <v>г. Люберцы, 1-й Панковский проезд, д. 27</v>
+        <v>г. Апрелевка, Сентябрьская улица, д. 5, стр. 2</v>
       </c>
       <c r="F90" t="str">
         <v/>
       </c>
       <c r="G90" t="str">
-        <v>г. Люберцы, улица Камова, д. 11/5</v>
+        <v>г. Селятино, Клубная, д. 55</v>
       </c>
       <c r="H90" t="str">
         <v/>
       </c>
       <c r="I90" t="str">
-        <v>г. Люберцы, проспект Гагарина, д. 28/1</v>
+        <v>г. Московский, улица Хабарова, д. 2</v>
       </c>
       <c r="J90" t="str">
-        <v/>
-      </c>
-      <c r="K90" t="str">
-        <v>г. Люберцы, Проспек Победы, д. 6, кв. 019</v>
-      </c>
-      <c r="L90" t="str">
-        <v/>
-      </c>
-      <c r="M90" t="str">
-        <v>г. Люберцы, Смирновская улица, д. 21, к. 2</v>
-      </c>
-      <c r="N90" t="str">
         <v/>
       </c>
     </row>
@@ -3568,28 +3634,28 @@
         <v>СТРИТ ЛОГИСТИК</v>
       </c>
       <c r="B91" t="str">
-        <v>Малянов Евгений</v>
+        <v>Мусаев Бахлул</v>
       </c>
       <c r="C91" t="str">
-        <v>Р583КУ177</v>
+        <v>В207Во797</v>
       </c>
       <c r="D91">
         <v>3</v>
       </c>
       <c r="E91" t="str">
-        <v>улица Лавочкина, д. 34</v>
+        <v>Большая Академическая улица, д. 24, к. 2</v>
       </c>
       <c r="F91" t="str">
         <v/>
       </c>
       <c r="G91" t="str">
-        <v>Авангардная улица, д. 3</v>
+        <v>улица Расплетина, д. 13</v>
       </c>
       <c r="H91" t="str">
         <v/>
       </c>
       <c r="I91" t="str">
-        <v>Самеда Вургуна, д. 11</v>
+        <v>улица Маршала Бирюзова, д. 4, к. 1</v>
       </c>
       <c r="J91" t="str">
         <v/>
@@ -3600,34 +3666,34 @@
         <v>СТРИТ ЛОГИСТИК</v>
       </c>
       <c r="B92" t="str">
-        <v>Метлихин Игорь</v>
+        <v>Нариманов Тамирлан</v>
       </c>
       <c r="C92" t="str">
-        <v>М609КТ790</v>
+        <v>с469ок777</v>
       </c>
       <c r="D92">
         <v>4</v>
       </c>
       <c r="E92" t="str">
-        <v>проспект Мира, д. 124, к. 2</v>
+        <v>г. Жуковский, улица Баженова, д. 4/1</v>
       </c>
       <c r="F92" t="str">
         <v/>
       </c>
       <c r="G92" t="str">
-        <v>улица Академика Королёва, д. 13, стр. 1</v>
+        <v>г. Жуковский, улица Горького, д. 4</v>
       </c>
       <c r="H92" t="str">
         <v/>
       </c>
       <c r="I92" t="str">
-        <v>Огородный проезд, д. 10</v>
+        <v>г. Жуковский, улица Чкалова, д. 2А, стр. 1</v>
       </c>
       <c r="J92" t="str">
         <v/>
       </c>
       <c r="K92" t="str">
-        <v>Шереметьевская улица, д. 20</v>
+        <v>г. Жуковский, улица Гагарина, д. 24</v>
       </c>
       <c r="L92" t="str">
         <v/>
@@ -3638,34 +3704,34 @@
         <v>СТРИТ ЛОГИСТИК</v>
       </c>
       <c r="B93" t="str">
-        <v>Мифтахутдинов Айрат</v>
+        <v>Неменущий Илья</v>
       </c>
       <c r="C93" t="str">
-        <v>р987ав777</v>
+        <v>м631ео82</v>
       </c>
       <c r="D93">
         <v>4</v>
       </c>
       <c r="E93" t="str">
-        <v>улица Тёплый Стан, д. 10</v>
+        <v>г. Подольск, Мраморная улица, д. 4</v>
       </c>
       <c r="F93" t="str">
         <v/>
       </c>
       <c r="G93" t="str">
-        <v>улица Тёплый Стан, д. 1А</v>
+        <v>г. Подольск, Февральская улица, д. 54/150</v>
       </c>
       <c r="H93" t="str">
         <v/>
       </c>
       <c r="I93" t="str">
-        <v>Профсоюзная улица, д. 103А</v>
+        <v>г. Подольск, Быковская улица, д. 10</v>
       </c>
       <c r="J93" t="str">
         <v/>
       </c>
       <c r="K93" t="str">
-        <v>Ясногорская улица, д. 7А</v>
+        <v>г. Подольск, Ленина, д. 14</v>
       </c>
       <c r="L93" t="str">
         <v/>
@@ -3676,30 +3742,42 @@
         <v>СТРИТ ЛОГИСТИК</v>
       </c>
       <c r="B94" t="str">
-        <v>Мусаев Бахлул</v>
+        <v>Овсепян Хачатур</v>
       </c>
       <c r="C94" t="str">
-        <v>В207Во797</v>
+        <v>Е564ка164</v>
       </c>
       <c r="D94">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E94" t="str">
-        <v>г. Раменское, Крымская улица, д. 12, стр. офис 17</v>
+        <v>Каширское шоссе, д. 65, к. 3</v>
       </c>
       <c r="F94" t="str">
         <v/>
       </c>
       <c r="G94" t="str">
-        <v>г. Раменское, улица Михалевича, д. 5</v>
+        <v>Ясеневая улица, д. 29</v>
       </c>
       <c r="H94" t="str">
         <v/>
       </c>
       <c r="I94" t="str">
-        <v>г. Раменское, улица Чугунова, д. 32А</v>
+        <v>Булатниковская улица, д. 2А</v>
       </c>
       <c r="J94" t="str">
+        <v/>
+      </c>
+      <c r="K94" t="str">
+        <v>Бирюлёвская улица, д. 43</v>
+      </c>
+      <c r="L94" t="str">
+        <v/>
+      </c>
+      <c r="M94" t="str">
+        <v>Михневская улица, д. 4</v>
+      </c>
+      <c r="N94" t="str">
         <v/>
       </c>
     </row>
@@ -3708,34 +3786,34 @@
         <v>СТРИТ ЛОГИСТИК</v>
       </c>
       <c r="B95" t="str">
-        <v>Нариманов Тамирлан</v>
+        <v>Основин Артём</v>
       </c>
       <c r="C95" t="str">
-        <v>с469ок777</v>
+        <v xml:space="preserve">т453кв190 </v>
       </c>
       <c r="D95">
         <v>4</v>
       </c>
       <c r="E95" t="str">
-        <v>г. Пушкино, Московский проспект, д. 59</v>
+        <v>г. поселение Десеновское, 1-я Нововатутинская улица, д. 5</v>
       </c>
       <c r="F95" t="str">
         <v/>
       </c>
       <c r="G95" t="str">
-        <v>г. Пушкино, микрорайон Серебрянка, д. 48, к. 2</v>
+        <v>г. Троицк, микрорайон В, д. 50</v>
       </c>
       <c r="H95" t="str">
         <v/>
       </c>
       <c r="I95" t="str">
-        <v>г. Пушкино, Набережная улица, д. 35, к. 6</v>
+        <v>г. Троицк, Академическая площадь, д. 3, кв. 2А</v>
       </c>
       <c r="J95" t="str">
         <v/>
       </c>
       <c r="K95" t="str">
-        <v>г. Мытищи, 2-я Институтская улица, д. 26</v>
+        <v>г. Троицк, Городская улица, д. вл6</v>
       </c>
       <c r="L95" t="str">
         <v/>
@@ -3746,34 +3824,34 @@
         <v>СТРИТ ЛОГИСТИК</v>
       </c>
       <c r="B96" t="str">
-        <v>Неменущий Илья</v>
+        <v>Попов Андрей</v>
       </c>
       <c r="C96" t="str">
-        <v>м631ео82</v>
+        <v xml:space="preserve">Е544АК190 </v>
       </c>
       <c r="D96">
         <v>4</v>
       </c>
       <c r="E96" t="str">
-        <v>Большая Марфинская улица, д. 4, к. 1</v>
+        <v>г. Подольск, Подольская улица, д. 10А</v>
       </c>
       <c r="F96" t="str">
         <v/>
       </c>
       <c r="G96" t="str">
-        <v>Алтуфьевское шоссе, д. 40Г</v>
+        <v>г. Щербинка, Индустриальная, д. 9</v>
       </c>
       <c r="H96" t="str">
         <v/>
       </c>
       <c r="I96" t="str">
-        <v>Алтуфьевское шоссе, д. 48, к. 2</v>
+        <v>г. поселение Воскресенское, Чечёрский проезд, д. 122, к. 1</v>
       </c>
       <c r="J96" t="str">
         <v/>
       </c>
       <c r="K96" t="str">
-        <v>Плещеева, д. 8</v>
+        <v>Южнобутовская улица, д. 117</v>
       </c>
       <c r="L96" t="str">
         <v/>
@@ -3784,36 +3862,30 @@
         <v>СТРИТ ЛОГИСТИК</v>
       </c>
       <c r="B97" t="str">
-        <v>Овсепян Хачатур</v>
+        <v>Рыбин Алексей</v>
       </c>
       <c r="C97" t="str">
-        <v>Е564ка164</v>
+        <v>к973ом777</v>
       </c>
       <c r="D97">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E97" t="str">
-        <v>г. Бутово, жилой комплекс Бутово Парк, д. 28</v>
+        <v>г. Химки, Транспортный проезд, д. 3</v>
       </c>
       <c r="F97" t="str">
         <v/>
       </c>
       <c r="G97" t="str">
-        <v>г. Щербинка, Индустриальная, д. 9</v>
+        <v>г. Химки, улица имени К.И. Вороницына, д. 1, к. 1</v>
       </c>
       <c r="H97" t="str">
         <v/>
       </c>
       <c r="I97" t="str">
-        <v>улица Брусилова, д. 13</v>
+        <v>г. Химки, улица Чкалова, д. 10/6</v>
       </c>
       <c r="J97" t="str">
-        <v/>
-      </c>
-      <c r="K97" t="str">
-        <v>г. рабочий посёлок Дрожжино, Новое шоссе, д. 11</v>
-      </c>
-      <c r="L97" t="str">
         <v/>
       </c>
     </row>
@@ -3822,34 +3894,34 @@
         <v>СТРИТ ЛОГИСТИК</v>
       </c>
       <c r="B98" t="str">
-        <v>Основин Артём</v>
+        <v>Стукалин Дмитрий</v>
       </c>
       <c r="C98" t="str">
-        <v xml:space="preserve">т453кв190 </v>
+        <v>у155не790</v>
       </c>
       <c r="D98">
         <v>4</v>
       </c>
       <c r="E98" t="str">
-        <v>Лобненская улица, д. 4А</v>
+        <v>Варшавское шоссе, д. 26, стр. 7</v>
       </c>
       <c r="F98" t="str">
         <v/>
       </c>
       <c r="G98" t="str">
-        <v>Ангарская улица, д. 57, к. 1</v>
+        <v>Электролитный проезд, д. 16, к. 1</v>
       </c>
       <c r="H98" t="str">
         <v/>
       </c>
       <c r="I98" t="str">
-        <v>Коровинское шоссе, д. 19, к. 1</v>
+        <v>Варшавское шоссе, д. 86А</v>
       </c>
       <c r="J98" t="str">
         <v/>
       </c>
       <c r="K98" t="str">
-        <v>Дегунинская улица, д. 10, стр. 2</v>
+        <v>Чонгарский бульвар, д. 26А, к. 3</v>
       </c>
       <c r="L98" t="str">
         <v/>
@@ -3860,28 +3932,28 @@
         <v>СТРИТ ЛОГИСТИК</v>
       </c>
       <c r="B99" t="str">
-        <v>Попов Андрей</v>
+        <v>Сулайманов Кубат</v>
       </c>
       <c r="C99" t="str">
-        <v xml:space="preserve">Е544АК190 </v>
+        <v>Е641ХМ199</v>
       </c>
       <c r="D99">
         <v>3</v>
       </c>
       <c r="E99" t="str">
-        <v>Алтуфьевское шоссе, д. 27</v>
+        <v>г. Химки, улица Кирова, д. 10, к. 2</v>
       </c>
       <c r="F99" t="str">
         <v/>
       </c>
       <c r="G99" t="str">
-        <v>Олонецкая улица, д. 4</v>
+        <v>г. Химки, Пролетарская, д. 15, к. 18</v>
       </c>
       <c r="H99" t="str">
         <v/>
       </c>
       <c r="I99" t="str">
-        <v>Лазоревый проезд, д. 1А, к. 1</v>
+        <v>г. Химки, улица Горшина, д. 5</v>
       </c>
       <c r="J99" t="str">
         <v/>
@@ -3892,42 +3964,30 @@
         <v>СТРИТ ЛОГИСТИК</v>
       </c>
       <c r="B100" t="str">
-        <v>Рыбин Алексей</v>
+        <v>Третьяков Сергей</v>
       </c>
       <c r="C100" t="str">
-        <v>к973ом777</v>
+        <v>Н915АЕ790</v>
       </c>
       <c r="D100">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E100" t="str">
-        <v>г. Зеленоград, улица Болдов Ручей, д. 1</v>
+        <v>г. Красногорск, улица Жуковского, д. 17</v>
       </c>
       <c r="F100" t="str">
         <v/>
       </c>
       <c r="G100" t="str">
-        <v>г. Зеленоград, -, д. 403А, стр. 9</v>
+        <v>г. Красногорск, Заводская улица, д. 18, к. 2</v>
       </c>
       <c r="H100" t="str">
         <v/>
       </c>
       <c r="I100" t="str">
-        <v>г. Зеленоград, Центральный проспект, д. -, к. 438</v>
+        <v>г. Красногорск, улица Ленина, д. 26А</v>
       </c>
       <c r="J100" t="str">
-        <v/>
-      </c>
-      <c r="K100" t="str">
-        <v>г. Химки, Тепличный проезд, д. 8</v>
-      </c>
-      <c r="L100" t="str">
-        <v/>
-      </c>
-      <c r="M100" t="str">
-        <v>г. Химки, Октябрьская улица, д. 1А</v>
-      </c>
-      <c r="N100" t="str">
         <v/>
       </c>
     </row>
@@ -3936,42 +3996,24 @@
         <v>СТРИТ ЛОГИСТИК</v>
       </c>
       <c r="B101" t="str">
-        <v>Стукалин Дмитрий</v>
+        <v>Федарков Сергей</v>
       </c>
       <c r="C101" t="str">
-        <v>у155не790</v>
+        <v>х460тх197</v>
       </c>
       <c r="D101">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E101" t="str">
-        <v>Булатниковская улица, д. 2А</v>
+        <v>г. Химки, улица Лётчика Ивана Фёдорова, д. 8, к. 1</v>
       </c>
       <c r="F101" t="str">
         <v/>
       </c>
       <c r="G101" t="str">
-        <v>Булатниковский проезд, д. 2В, к. 4</v>
+        <v>г. Лобня, улица Ленина, д. 18</v>
       </c>
       <c r="H101" t="str">
-        <v/>
-      </c>
-      <c r="I101" t="str">
-        <v>Россошанский проезд, д. 3</v>
-      </c>
-      <c r="J101" t="str">
-        <v/>
-      </c>
-      <c r="K101" t="str">
-        <v>Бирюлёвская улица, д. 43</v>
-      </c>
-      <c r="L101" t="str">
-        <v/>
-      </c>
-      <c r="M101" t="str">
-        <v>Михневская улица, д. 4</v>
-      </c>
-      <c r="N101" t="str">
         <v/>
       </c>
     </row>
@@ -3980,24 +4022,42 @@
         <v>СТРИТ ЛОГИСТИК</v>
       </c>
       <c r="B102" t="str">
-        <v>Сулайманов Кубат</v>
+        <v>Федорин Евгений</v>
       </c>
       <c r="C102" t="str">
-        <v>Е641ХМ199</v>
+        <v>У093оу77</v>
       </c>
       <c r="D102">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E102" t="str">
-        <v>г. Одинцово, Союзная улица, д. 1, к. В</v>
+        <v>г. Люберцы, Московская улица, д. 11</v>
       </c>
       <c r="F102" t="str">
         <v/>
       </c>
       <c r="G102" t="str">
-        <v>г. Одинцово, улица Чикина, д. 8А, к. А</v>
+        <v>г. Люберцы, Новорязанское шоссе, д. 1А</v>
       </c>
       <c r="H102" t="str">
+        <v/>
+      </c>
+      <c r="I102" t="str">
+        <v>г. Люберцы, улица Кирова, д. 9, к. 5</v>
+      </c>
+      <c r="J102" t="str">
+        <v/>
+      </c>
+      <c r="K102" t="str">
+        <v>Жулебинский бульвар, д. 30, к. 1</v>
+      </c>
+      <c r="L102" t="str">
+        <v/>
+      </c>
+      <c r="M102" t="str">
+        <v>Лермонтовский проспект, д. 19, к. 1</v>
+      </c>
+      <c r="N102" t="str">
         <v/>
       </c>
     </row>
@@ -4006,34 +4066,34 @@
         <v>СТРИТ ЛОГИСТИК</v>
       </c>
       <c r="B103" t="str">
-        <v>Третьяков Сергей</v>
+        <v>Фейзула Владимир</v>
       </c>
       <c r="C103" t="str">
-        <v>Н915АЕ790</v>
+        <v>н268вт797</v>
       </c>
       <c r="D103">
         <v>4</v>
       </c>
       <c r="E103" t="str">
-        <v>г. Мытищи, Коммунистическая улица, д. 1</v>
+        <v>Вольная улица, д. 28/4, к. 1</v>
       </c>
       <c r="F103" t="str">
         <v/>
       </c>
       <c r="G103" t="str">
-        <v>г. Королёв, Пионерская улица, д. 12</v>
+        <v>Щербаковская улица, д. 20</v>
       </c>
       <c r="H103" t="str">
         <v/>
       </c>
       <c r="I103" t="str">
-        <v>г. Королёв, улица Карла Маркса, д. 1А</v>
+        <v>Открытое шоссе, д. 24, к. 11</v>
       </c>
       <c r="J103" t="str">
         <v/>
       </c>
       <c r="K103" t="str">
-        <v>г. Королёв, Пионерская улица, д. 15, к. 2</v>
+        <v>Амурская улица, д. 19</v>
       </c>
       <c r="L103" t="str">
         <v/>
@@ -4044,34 +4104,34 @@
         <v>СТРИТ ЛОГИСТИК</v>
       </c>
       <c r="B104" t="str">
-        <v>Федарков Сергей</v>
+        <v>Хлебников Олег</v>
       </c>
       <c r="C104" t="str">
-        <v>х460тх197</v>
+        <v>н210нс68</v>
       </c>
       <c r="D104">
         <v>4</v>
       </c>
       <c r="E104" t="str">
-        <v>г. Балашиха, улица Евстафьева, д. 1/9</v>
+        <v>Лазоревый проезд, д. 1А, к. 1</v>
       </c>
       <c r="F104" t="str">
         <v/>
       </c>
       <c r="G104" t="str">
-        <v>г. Балашиха, проспект Ленина, д. 74</v>
+        <v>Снежная улица, д. 27, к. 1</v>
       </c>
       <c r="H104" t="str">
         <v/>
       </c>
       <c r="I104" t="str">
-        <v>г. Балашиха, улица Твардовского, д. 44</v>
+        <v>Радужная улица, д. 4, к. 1</v>
       </c>
       <c r="J104" t="str">
         <v/>
       </c>
       <c r="K104" t="str">
-        <v>г. Балашиха, Живописная улица, д. 1</v>
+        <v>Ярославское шоссе, д. 124</v>
       </c>
       <c r="L104" t="str">
         <v/>
@@ -4082,24 +4142,36 @@
         <v>СТРИТ ЛОГИСТИК</v>
       </c>
       <c r="B105" t="str">
-        <v>Федорин Евгений</v>
+        <v>Хохряев Сергей</v>
       </c>
       <c r="C105" t="str">
-        <v>У093оу77</v>
+        <v>р220оа77</v>
       </c>
       <c r="D105">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E105" t="str">
-        <v>г. Одинцово, Кутузовская улица, д. 72Б</v>
+        <v>улица Гурьянова, д. 30</v>
       </c>
       <c r="F105" t="str">
         <v/>
       </c>
       <c r="G105" t="str">
-        <v>г. Одинцово, улица Чистяковой, д. 67</v>
+        <v>5-я Кожуховская улица, д. 9</v>
       </c>
       <c r="H105" t="str">
+        <v/>
+      </c>
+      <c r="I105" t="str">
+        <v>улица Мастеркова, д. 6</v>
+      </c>
+      <c r="J105" t="str">
+        <v/>
+      </c>
+      <c r="K105" t="str">
+        <v>Волгоградский проспект, д. 32, к. 2</v>
+      </c>
+      <c r="L105" t="str">
         <v/>
       </c>
     </row>
@@ -4108,176 +4180,42 @@
         <v>СТРИТ ЛОГИСТИК</v>
       </c>
       <c r="B106" t="str">
-        <v>Фейзула Владимир</v>
+        <v>Шорохов Василий</v>
       </c>
       <c r="C106" t="str">
-        <v>н268вт797</v>
+        <v xml:space="preserve"> Н118ХР123</v>
       </c>
       <c r="D106">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E106" t="str">
-        <v>г. Красногорск, улица Ленина, д. 26А</v>
+        <v>г. Балашиха, улица Евстафьева, д. 1/9</v>
       </c>
       <c r="F106" t="str">
         <v/>
       </c>
       <c r="G106" t="str">
-        <v>г. Красногорск, бульвар Космонавтов, д. 17</v>
+        <v>г. Балашиха, улица Лукино, д. 55А</v>
       </c>
       <c r="H106" t="str">
         <v/>
       </c>
       <c r="I106" t="str">
-        <v>г. Красногорск, Светлая улица, д. 3А, стр. 4</v>
+        <v>г. Балашиха, Балашихинское шоссе, д. 10</v>
       </c>
       <c r="J106" t="str">
         <v/>
       </c>
-    </row>
-    <row r="107">
-      <c r="A107" t="str">
-        <v>СТРИТ ЛОГИСТИК</v>
-      </c>
-      <c r="B107" t="str">
-        <v>Хасянов Рафик</v>
-      </c>
-      <c r="C107" t="str">
-        <v>В862ХР197</v>
-      </c>
-      <c r="D107">
-        <v>3</v>
-      </c>
-      <c r="E107" t="str">
-        <v>улица Лётчика Грицевца, д. 12</v>
-      </c>
-      <c r="F107" t="str">
-        <v/>
-      </c>
-      <c r="G107" t="str">
-        <v>г. поселение Внуковское, Омская улица, д. 7А</v>
-      </c>
-      <c r="H107" t="str">
-        <v/>
-      </c>
-      <c r="I107" t="str">
-        <v>г. Внуково, Центральная улица, д. 8Б, кв. 212</v>
-      </c>
-      <c r="J107" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="108">
-      <c r="A108" t="str">
-        <v>СТРИТ ЛОГИСТИК</v>
-      </c>
-      <c r="B108" t="str">
-        <v>Хохряев Сергей</v>
-      </c>
-      <c r="C108" t="str">
-        <v>р220оа77</v>
-      </c>
-      <c r="D108">
-        <v>4</v>
-      </c>
-      <c r="E108" t="str">
-        <v>Варшавское шоссе, д. 141А, к. 2, кв. пом. 5</v>
-      </c>
-      <c r="F108" t="str">
-        <v/>
-      </c>
-      <c r="G108" t="str">
-        <v>улица Поляны, д. 5</v>
-      </c>
-      <c r="H108" t="str">
-        <v/>
-      </c>
-      <c r="I108" t="str">
-        <v>улица Знаменские Садки, д. 1, к. 1</v>
-      </c>
-      <c r="J108" t="str">
-        <v/>
-      </c>
-      <c r="K108" t="str">
-        <v>Старокачаловская, д. 1, к. 2</v>
-      </c>
-      <c r="L108" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="109">
-      <c r="A109" t="str">
-        <v>СТРИТ ЛОГИСТИК</v>
-      </c>
-      <c r="B109" t="str">
-        <v>Чёрный Алексей</v>
-      </c>
-      <c r="C109" t="str">
-        <v>А780КС797</v>
-      </c>
-      <c r="D109">
-        <v>4</v>
-      </c>
-      <c r="E109" t="str">
-        <v>г. Мытищи, улица Комарова, д. 2, к. 2</v>
-      </c>
-      <c r="F109" t="str">
-        <v/>
-      </c>
-      <c r="G109" t="str">
-        <v>г. Мытищи, Олимпийский проспект, д. 36, к. 3</v>
-      </c>
-      <c r="H109" t="str">
-        <v/>
-      </c>
-      <c r="I109" t="str">
-        <v>г. Мытищи, проспект Астрахова, д. 6</v>
-      </c>
-      <c r="J109" t="str">
-        <v/>
-      </c>
-      <c r="K109" t="str">
-        <v>г. Мытищи, 1-й Щёлковский проезд, д. 7</v>
-      </c>
-      <c r="L109" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="110">
-      <c r="A110" t="str">
-        <v>СТРИТ ЛОГИСТИК</v>
-      </c>
-      <c r="B110" t="str">
-        <v>Шорохов Василий</v>
-      </c>
-      <c r="C110" t="str">
-        <v xml:space="preserve"> Н118ХР123</v>
-      </c>
-      <c r="D110">
-        <v>3</v>
-      </c>
-      <c r="E110" t="str">
-        <v>г. рабочий посёлок Октябрьский, улица Ленина, д. 25</v>
-      </c>
-      <c r="F110" t="str">
-        <v/>
-      </c>
-      <c r="G110" t="str">
-        <v>г. Бронницы, Советская улица, д. 73</v>
-      </c>
-      <c r="H110" t="str">
-        <v/>
-      </c>
-      <c r="I110" t="str">
-        <v>г. рабочий посёлок Октябрьский, микрорайон Восточный, д. 1</v>
-      </c>
-      <c r="J110" t="str">
+      <c r="K106" t="str">
+        <v>г. Балашиха, Кольцевая улица, д. 3К2, к. 2</v>
+      </c>
+      <c r="L106" t="str">
         <v/>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:U110"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:U106"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>